<commit_message>
Update unique borrower spreadsheet
</commit_message>
<xml_diff>
--- a/statistics_files/2022/2022.d.monthly_circ_by_borrower.unique_borrowers.xlsx
+++ b/statistics_files/2022/2022.d.monthly_circ_by_borrower.unique_borrowers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5CB4AC2-BC8B-4BB2-AF82-12226CEC33D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A66554F-3B36-486B-B546-3874B61C89EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="894" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="894" activeTab="1" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="69">
   <si>
     <t>branchname</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>Winchester Public Library</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>2022-02-01 - 2022-02-28</t>
   </si>
 </sst>
 </file>
@@ -609,11 +615,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A36" sqref="A36"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5212,9 +5218,9 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3351FCFD-2A2A-4342-87F8-3564DBC5D720}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="B2:AF2"/>
+  <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -5227,38 +5233,4136 @@
     <col min="2" max="33" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44593</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44594</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44595</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44596</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44597</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44598</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44599</v>
+      </c>
+      <c r="I2" s="1">
+        <v>44600</v>
+      </c>
+      <c r="J2" s="1">
+        <v>44601</v>
+      </c>
+      <c r="K2" s="1">
+        <v>44602</v>
+      </c>
+      <c r="L2" s="1">
+        <v>44603</v>
+      </c>
+      <c r="M2" s="1">
+        <v>44604</v>
+      </c>
+      <c r="N2" s="1">
+        <v>44605</v>
+      </c>
+      <c r="O2" s="1">
+        <v>44606</v>
+      </c>
+      <c r="P2" s="1">
+        <v>44607</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>44608</v>
+      </c>
+      <c r="R2" s="1">
+        <v>44609</v>
+      </c>
+      <c r="S2" s="1">
+        <v>44610</v>
+      </c>
+      <c r="T2" s="1">
+        <v>44611</v>
+      </c>
+      <c r="U2" s="1">
+        <v>44612</v>
+      </c>
+      <c r="V2" s="1">
+        <v>44613</v>
+      </c>
+      <c r="W2" s="1">
+        <v>44614</v>
+      </c>
+      <c r="X2" s="1">
+        <v>44615</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>44616</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>44617</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>44618</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>44619</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>44620</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>70</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>42</v>
+      </c>
+      <c r="E4">
+        <v>44</v>
+      </c>
+      <c r="F4">
+        <v>34</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>67</v>
+      </c>
+      <c r="I4">
+        <v>63</v>
+      </c>
+      <c r="J4">
+        <v>57</v>
+      </c>
+      <c r="K4">
+        <v>73</v>
+      </c>
+      <c r="L4">
+        <v>60</v>
+      </c>
+      <c r="M4">
+        <v>34</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>69</v>
+      </c>
+      <c r="P4">
+        <v>62</v>
+      </c>
+      <c r="Q4">
+        <v>82</v>
+      </c>
+      <c r="R4">
+        <v>37</v>
+      </c>
+      <c r="S4">
+        <v>44</v>
+      </c>
+      <c r="T4">
+        <v>30</v>
+      </c>
+      <c r="U4">
+        <v>4</v>
+      </c>
+      <c r="V4">
+        <v>6</v>
+      </c>
+      <c r="W4">
+        <v>77</v>
+      </c>
+      <c r="X4">
+        <v>57</v>
+      </c>
+      <c r="Y4">
+        <v>39</v>
+      </c>
+      <c r="Z4">
+        <v>65</v>
+      </c>
+      <c r="AA4">
+        <v>46</v>
+      </c>
+      <c r="AB4">
+        <v>3</v>
+      </c>
+      <c r="AC4">
+        <v>62</v>
+      </c>
+      <c r="AG4">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>18</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>37</v>
+      </c>
+      <c r="I5">
+        <v>43</v>
+      </c>
+      <c r="J5">
+        <v>38</v>
+      </c>
+      <c r="K5">
+        <v>38</v>
+      </c>
+      <c r="L5">
+        <v>30</v>
+      </c>
+      <c r="M5">
+        <v>12</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>34</v>
+      </c>
+      <c r="P5">
+        <v>44</v>
+      </c>
+      <c r="Q5">
+        <v>44</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>29</v>
+      </c>
+      <c r="T5">
+        <v>15</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>35</v>
+      </c>
+      <c r="W5">
+        <v>34</v>
+      </c>
+      <c r="X5">
+        <v>40</v>
+      </c>
+      <c r="Y5">
+        <v>19</v>
+      </c>
+      <c r="Z5">
+        <v>29</v>
+      </c>
+      <c r="AA5">
+        <v>20</v>
+      </c>
+      <c r="AB5">
+        <v>3</v>
+      </c>
+      <c r="AC5">
+        <v>26</v>
+      </c>
+      <c r="AG5">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>87</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>47</v>
+      </c>
+      <c r="E6">
+        <v>61</v>
+      </c>
+      <c r="F6">
+        <v>58</v>
+      </c>
+      <c r="G6">
+        <v>42</v>
+      </c>
+      <c r="H6">
+        <v>78</v>
+      </c>
+      <c r="I6">
+        <v>80</v>
+      </c>
+      <c r="J6">
+        <v>93</v>
+      </c>
+      <c r="K6">
+        <v>72</v>
+      </c>
+      <c r="L6">
+        <v>71</v>
+      </c>
+      <c r="M6">
+        <v>53</v>
+      </c>
+      <c r="N6">
+        <v>46</v>
+      </c>
+      <c r="O6">
+        <v>79</v>
+      </c>
+      <c r="P6">
+        <v>94</v>
+      </c>
+      <c r="Q6">
+        <v>106</v>
+      </c>
+      <c r="R6">
+        <v>10</v>
+      </c>
+      <c r="S6">
+        <v>33</v>
+      </c>
+      <c r="T6">
+        <v>41</v>
+      </c>
+      <c r="U6">
+        <v>46</v>
+      </c>
+      <c r="V6">
+        <v>11</v>
+      </c>
+      <c r="W6">
+        <v>81</v>
+      </c>
+      <c r="X6">
+        <v>112</v>
+      </c>
+      <c r="Y6">
+        <v>63</v>
+      </c>
+      <c r="Z6">
+        <v>76</v>
+      </c>
+      <c r="AA6">
+        <v>69</v>
+      </c>
+      <c r="AB6">
+        <v>35</v>
+      </c>
+      <c r="AC6">
+        <v>85</v>
+      </c>
+      <c r="AG6">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>2</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>5</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>72</v>
+      </c>
+      <c r="C8">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>38</v>
+      </c>
+      <c r="F8">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>26</v>
+      </c>
+      <c r="H8">
+        <v>59</v>
+      </c>
+      <c r="I8">
+        <v>54</v>
+      </c>
+      <c r="J8">
+        <v>62</v>
+      </c>
+      <c r="K8">
+        <v>54</v>
+      </c>
+      <c r="L8">
+        <v>45</v>
+      </c>
+      <c r="M8">
+        <v>37</v>
+      </c>
+      <c r="N8">
+        <v>20</v>
+      </c>
+      <c r="O8">
+        <v>62</v>
+      </c>
+      <c r="P8">
+        <v>65</v>
+      </c>
+      <c r="Q8">
+        <v>65</v>
+      </c>
+      <c r="R8">
+        <v>4</v>
+      </c>
+      <c r="S8">
+        <v>28</v>
+      </c>
+      <c r="T8">
+        <v>48</v>
+      </c>
+      <c r="U8">
+        <v>21</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>65</v>
+      </c>
+      <c r="X8">
+        <v>56</v>
+      </c>
+      <c r="Y8">
+        <v>44</v>
+      </c>
+      <c r="Z8">
+        <v>57</v>
+      </c>
+      <c r="AA8">
+        <v>53</v>
+      </c>
+      <c r="AB8">
+        <v>26</v>
+      </c>
+      <c r="AC8">
+        <v>74</v>
+      </c>
+      <c r="AG8">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>14</v>
+      </c>
+      <c r="I9">
+        <v>12</v>
+      </c>
+      <c r="J9">
+        <v>12</v>
+      </c>
+      <c r="K9">
+        <v>11</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>8</v>
+      </c>
+      <c r="O9">
+        <v>7</v>
+      </c>
+      <c r="P9">
+        <v>9</v>
+      </c>
+      <c r="Q9">
+        <v>6</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>5</v>
+      </c>
+      <c r="T9">
+        <v>5</v>
+      </c>
+      <c r="V9">
+        <v>6</v>
+      </c>
+      <c r="W9">
+        <v>8</v>
+      </c>
+      <c r="X9">
+        <v>5</v>
+      </c>
+      <c r="Y9">
+        <v>4</v>
+      </c>
+      <c r="Z9">
+        <v>16</v>
+      </c>
+      <c r="AA9">
+        <v>6</v>
+      </c>
+      <c r="AB9">
+        <v>1</v>
+      </c>
+      <c r="AC9">
+        <v>9</v>
+      </c>
+      <c r="AG9">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>15</v>
+      </c>
+      <c r="K10">
+        <v>13</v>
+      </c>
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <v>4</v>
+      </c>
+      <c r="O10">
+        <v>7</v>
+      </c>
+      <c r="P10">
+        <v>6</v>
+      </c>
+      <c r="Q10">
+        <v>19</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
+      </c>
+      <c r="T10">
+        <v>7</v>
+      </c>
+      <c r="W10">
+        <v>13</v>
+      </c>
+      <c r="X10">
+        <v>16</v>
+      </c>
+      <c r="Y10">
+        <v>5</v>
+      </c>
+      <c r="Z10">
+        <v>11</v>
+      </c>
+      <c r="AA10">
+        <v>7</v>
+      </c>
+      <c r="AC10">
+        <v>10</v>
+      </c>
+      <c r="AG10">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
+      <c r="O11">
+        <v>6</v>
+      </c>
+      <c r="Q11">
+        <v>5</v>
+      </c>
+      <c r="R11">
+        <v>3</v>
+      </c>
+      <c r="S11">
+        <v>7</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>6</v>
+      </c>
+      <c r="X11">
+        <v>6</v>
+      </c>
+      <c r="Y11">
+        <v>2</v>
+      </c>
+      <c r="Z11">
+        <v>6</v>
+      </c>
+      <c r="AC11">
+        <v>8</v>
+      </c>
+      <c r="AG11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="AG12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>4</v>
+      </c>
+      <c r="R14">
+        <v>4</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>3</v>
+      </c>
+      <c r="X14">
+        <v>2</v>
+      </c>
+      <c r="Y14">
+        <v>4</v>
+      </c>
+      <c r="Z14">
+        <v>2</v>
+      </c>
+      <c r="AC14">
+        <v>1</v>
+      </c>
+      <c r="AG14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15">
+        <v>7</v>
+      </c>
+      <c r="J15">
+        <v>8</v>
+      </c>
+      <c r="K15">
+        <v>7</v>
+      </c>
+      <c r="L15">
+        <v>5</v>
+      </c>
+      <c r="O15">
+        <v>8</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="Q15">
+        <v>11</v>
+      </c>
+      <c r="R15">
+        <v>13</v>
+      </c>
+      <c r="S15">
+        <v>5</v>
+      </c>
+      <c r="W15">
+        <v>9</v>
+      </c>
+      <c r="X15">
+        <v>5</v>
+      </c>
+      <c r="Y15">
+        <v>3</v>
+      </c>
+      <c r="Z15">
+        <v>7</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>5</v>
+      </c>
+      <c r="AG15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <v>9</v>
+      </c>
+      <c r="J16">
+        <v>12</v>
+      </c>
+      <c r="K16">
+        <v>20</v>
+      </c>
+      <c r="L16">
+        <v>7</v>
+      </c>
+      <c r="M16">
+        <v>6</v>
+      </c>
+      <c r="O16">
+        <v>12</v>
+      </c>
+      <c r="P16">
+        <v>7</v>
+      </c>
+      <c r="Q16">
+        <v>12</v>
+      </c>
+      <c r="R16">
+        <v>7</v>
+      </c>
+      <c r="S16">
+        <v>10</v>
+      </c>
+      <c r="T16">
+        <v>4</v>
+      </c>
+      <c r="W16">
+        <v>10</v>
+      </c>
+      <c r="X16">
+        <v>17</v>
+      </c>
+      <c r="Y16">
+        <v>7</v>
+      </c>
+      <c r="Z16">
+        <v>12</v>
+      </c>
+      <c r="AA16">
+        <v>4</v>
+      </c>
+      <c r="AC16">
+        <v>15</v>
+      </c>
+      <c r="AG16">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>8</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>21</v>
+      </c>
+      <c r="L17">
+        <v>3</v>
+      </c>
+      <c r="M17">
+        <v>3</v>
+      </c>
+      <c r="O17">
+        <v>9</v>
+      </c>
+      <c r="P17">
+        <v>5</v>
+      </c>
+      <c r="Q17">
+        <v>4</v>
+      </c>
+      <c r="R17">
+        <v>6</v>
+      </c>
+      <c r="S17">
+        <v>6</v>
+      </c>
+      <c r="T17">
+        <v>2</v>
+      </c>
+      <c r="W17">
+        <v>4</v>
+      </c>
+      <c r="X17">
+        <v>3</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>3</v>
+      </c>
+      <c r="AA17">
+        <v>2</v>
+      </c>
+      <c r="AC17">
+        <v>8</v>
+      </c>
+      <c r="AG17">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>4</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>2</v>
+      </c>
+      <c r="X18">
+        <v>4</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>4</v>
+      </c>
+      <c r="AA18">
+        <v>2</v>
+      </c>
+      <c r="AC18">
+        <v>3</v>
+      </c>
+      <c r="AG18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>23</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>41</v>
+      </c>
+      <c r="I19">
+        <v>21</v>
+      </c>
+      <c r="J19">
+        <v>27</v>
+      </c>
+      <c r="K19">
+        <v>26</v>
+      </c>
+      <c r="L19">
+        <v>27</v>
+      </c>
+      <c r="M19">
+        <v>23</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+      <c r="O19">
+        <v>31</v>
+      </c>
+      <c r="P19">
+        <v>16</v>
+      </c>
+      <c r="Q19">
+        <v>30</v>
+      </c>
+      <c r="R19">
+        <v>2</v>
+      </c>
+      <c r="S19">
+        <v>2</v>
+      </c>
+      <c r="T19">
+        <v>12</v>
+      </c>
+      <c r="U19">
+        <v>2</v>
+      </c>
+      <c r="V19">
+        <v>4</v>
+      </c>
+      <c r="W19">
+        <v>38</v>
+      </c>
+      <c r="X19">
+        <v>24</v>
+      </c>
+      <c r="Y19">
+        <v>12</v>
+      </c>
+      <c r="Z19">
+        <v>26</v>
+      </c>
+      <c r="AA19">
+        <v>25</v>
+      </c>
+      <c r="AB19">
+        <v>2</v>
+      </c>
+      <c r="AC19">
+        <v>21</v>
+      </c>
+      <c r="AG19">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+      <c r="K20">
+        <v>6</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+      <c r="O20">
+        <v>3</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>3</v>
+      </c>
+      <c r="R20">
+        <v>2</v>
+      </c>
+      <c r="S20">
+        <v>4</v>
+      </c>
+      <c r="X20">
+        <v>4</v>
+      </c>
+      <c r="Y20">
+        <v>3</v>
+      </c>
+      <c r="Z20">
+        <v>4</v>
+      </c>
+      <c r="AC20">
+        <v>3</v>
+      </c>
+      <c r="AG20">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>39</v>
+      </c>
+      <c r="C21">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>27</v>
+      </c>
+      <c r="E21">
+        <v>32</v>
+      </c>
+      <c r="F21">
+        <v>16</v>
+      </c>
+      <c r="G21">
+        <v>16</v>
+      </c>
+      <c r="H21">
+        <v>32</v>
+      </c>
+      <c r="I21">
+        <v>33</v>
+      </c>
+      <c r="J21">
+        <v>21</v>
+      </c>
+      <c r="K21">
+        <v>37</v>
+      </c>
+      <c r="L21">
+        <v>29</v>
+      </c>
+      <c r="M21">
+        <v>13</v>
+      </c>
+      <c r="N21">
+        <v>7</v>
+      </c>
+      <c r="O21">
+        <v>33</v>
+      </c>
+      <c r="P21">
+        <v>43</v>
+      </c>
+      <c r="Q21">
+        <v>22</v>
+      </c>
+      <c r="R21">
+        <v>25</v>
+      </c>
+      <c r="S21">
+        <v>24</v>
+      </c>
+      <c r="T21">
+        <v>12</v>
+      </c>
+      <c r="U21">
+        <v>8</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>34</v>
+      </c>
+      <c r="X21">
+        <v>30</v>
+      </c>
+      <c r="Y21">
+        <v>26</v>
+      </c>
+      <c r="Z21">
+        <v>30</v>
+      </c>
+      <c r="AA21">
+        <v>21</v>
+      </c>
+      <c r="AB21">
+        <v>9</v>
+      </c>
+      <c r="AC21">
+        <v>23</v>
+      </c>
+      <c r="AG21">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>2</v>
+      </c>
+      <c r="Q22">
+        <v>2</v>
+      </c>
+      <c r="R22">
+        <v>2</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>2</v>
+      </c>
+      <c r="X22">
+        <v>1</v>
+      </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
+      <c r="Z22">
+        <v>3</v>
+      </c>
+      <c r="AC22">
+        <v>2</v>
+      </c>
+      <c r="AG22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>50</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>38</v>
+      </c>
+      <c r="F23">
+        <v>13</v>
+      </c>
+      <c r="H23">
+        <v>31</v>
+      </c>
+      <c r="I23">
+        <v>29</v>
+      </c>
+      <c r="J23">
+        <v>42</v>
+      </c>
+      <c r="K23">
+        <v>55</v>
+      </c>
+      <c r="L23">
+        <v>34</v>
+      </c>
+      <c r="M23">
+        <v>16</v>
+      </c>
+      <c r="O23">
+        <v>43</v>
+      </c>
+      <c r="P23">
+        <v>33</v>
+      </c>
+      <c r="Q23">
+        <v>55</v>
+      </c>
+      <c r="R23">
+        <v>25</v>
+      </c>
+      <c r="S23">
+        <v>28</v>
+      </c>
+      <c r="T23">
+        <v>16</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23">
+        <v>3</v>
+      </c>
+      <c r="W23">
+        <v>38</v>
+      </c>
+      <c r="X23">
+        <v>42</v>
+      </c>
+      <c r="Y23">
+        <v>26</v>
+      </c>
+      <c r="Z23">
+        <v>42</v>
+      </c>
+      <c r="AA23">
+        <v>18</v>
+      </c>
+      <c r="AB23">
+        <v>5</v>
+      </c>
+      <c r="AC23">
+        <v>47</v>
+      </c>
+      <c r="AG23">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <v>3</v>
+      </c>
+      <c r="L24">
+        <v>5</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>7</v>
+      </c>
+      <c r="Q24">
+        <v>4</v>
+      </c>
+      <c r="S24">
+        <v>2</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="V24">
+        <v>4</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24">
+        <v>2</v>
+      </c>
+      <c r="Y24">
+        <v>2</v>
+      </c>
+      <c r="Z24">
+        <v>2</v>
+      </c>
+      <c r="AA24">
+        <v>2</v>
+      </c>
+      <c r="AC24">
+        <v>3</v>
+      </c>
+      <c r="AG24">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <v>42</v>
+      </c>
+      <c r="F25">
+        <v>22</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>28</v>
+      </c>
+      <c r="I25">
+        <v>46</v>
+      </c>
+      <c r="J25">
+        <v>28</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>2</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="V25">
+        <v>2</v>
+      </c>
+      <c r="W25">
+        <v>2</v>
+      </c>
+      <c r="X25">
+        <v>16</v>
+      </c>
+      <c r="Y25">
+        <v>15</v>
+      </c>
+      <c r="Z25">
+        <v>30</v>
+      </c>
+      <c r="AA25">
+        <v>19</v>
+      </c>
+      <c r="AC25">
+        <v>39</v>
+      </c>
+      <c r="AG25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>147</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>65</v>
+      </c>
+      <c r="E26">
+        <v>59</v>
+      </c>
+      <c r="F26">
+        <v>66</v>
+      </c>
+      <c r="G26">
+        <v>39</v>
+      </c>
+      <c r="H26">
+        <v>82</v>
+      </c>
+      <c r="I26">
+        <v>105</v>
+      </c>
+      <c r="J26">
+        <v>104</v>
+      </c>
+      <c r="K26">
+        <v>123</v>
+      </c>
+      <c r="L26">
+        <v>116</v>
+      </c>
+      <c r="M26">
+        <v>74</v>
+      </c>
+      <c r="N26">
+        <v>43</v>
+      </c>
+      <c r="O26">
+        <v>80</v>
+      </c>
+      <c r="P26">
+        <v>84</v>
+      </c>
+      <c r="Q26">
+        <v>104</v>
+      </c>
+      <c r="R26">
+        <v>14</v>
+      </c>
+      <c r="S26">
+        <v>62</v>
+      </c>
+      <c r="T26">
+        <v>79</v>
+      </c>
+      <c r="U26">
+        <v>46</v>
+      </c>
+      <c r="V26">
+        <v>16</v>
+      </c>
+      <c r="W26">
+        <v>118</v>
+      </c>
+      <c r="X26">
+        <v>99</v>
+      </c>
+      <c r="Y26">
+        <v>84</v>
+      </c>
+      <c r="Z26">
+        <v>75</v>
+      </c>
+      <c r="AA26">
+        <v>80</v>
+      </c>
+      <c r="AB26">
+        <v>56</v>
+      </c>
+      <c r="AC26">
+        <v>98</v>
+      </c>
+      <c r="AG26">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <v>14</v>
+      </c>
+      <c r="I27">
+        <v>8</v>
+      </c>
+      <c r="J27">
+        <v>6</v>
+      </c>
+      <c r="K27">
+        <v>11</v>
+      </c>
+      <c r="L27">
+        <v>11</v>
+      </c>
+      <c r="M27">
+        <v>2</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>7</v>
+      </c>
+      <c r="P27">
+        <v>6</v>
+      </c>
+      <c r="Q27">
+        <v>9</v>
+      </c>
+      <c r="R27">
+        <v>2</v>
+      </c>
+      <c r="S27">
+        <v>2</v>
+      </c>
+      <c r="T27">
+        <v>2</v>
+      </c>
+      <c r="W27">
+        <v>13</v>
+      </c>
+      <c r="X27">
+        <v>6</v>
+      </c>
+      <c r="Y27">
+        <v>14</v>
+      </c>
+      <c r="Z27">
+        <v>8</v>
+      </c>
+      <c r="AA27">
+        <v>4</v>
+      </c>
+      <c r="AC27">
+        <v>9</v>
+      </c>
+      <c r="AG27">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>11</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>16</v>
+      </c>
+      <c r="I29">
+        <v>12</v>
+      </c>
+      <c r="J29">
+        <v>12</v>
+      </c>
+      <c r="K29">
+        <v>11</v>
+      </c>
+      <c r="M29">
+        <v>6</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>11</v>
+      </c>
+      <c r="P29">
+        <v>13</v>
+      </c>
+      <c r="Q29">
+        <v>11</v>
+      </c>
+      <c r="R29">
+        <v>2</v>
+      </c>
+      <c r="T29">
+        <v>7</v>
+      </c>
+      <c r="U29">
+        <v>2</v>
+      </c>
+      <c r="W29">
+        <v>13</v>
+      </c>
+      <c r="X29">
+        <v>12</v>
+      </c>
+      <c r="Y29">
+        <v>4</v>
+      </c>
+      <c r="AA29">
+        <v>9</v>
+      </c>
+      <c r="AC29">
+        <v>13</v>
+      </c>
+      <c r="AG29">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>9</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="J30">
+        <v>8</v>
+      </c>
+      <c r="K30">
+        <v>6</v>
+      </c>
+      <c r="M30">
+        <v>5</v>
+      </c>
+      <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <v>3</v>
+      </c>
+      <c r="Q30">
+        <v>5</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="T30">
+        <v>1</v>
+      </c>
+      <c r="V30">
+        <v>5</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <v>3</v>
+      </c>
+      <c r="Y30">
+        <v>1</v>
+      </c>
+      <c r="Z30">
+        <v>5</v>
+      </c>
+      <c r="AA30">
+        <v>1</v>
+      </c>
+      <c r="AC30">
+        <v>1</v>
+      </c>
+      <c r="AG30">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>35</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>18</v>
+      </c>
+      <c r="F31">
+        <v>10</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>15</v>
+      </c>
+      <c r="I31">
+        <v>29</v>
+      </c>
+      <c r="J31">
+        <v>18</v>
+      </c>
+      <c r="K31">
+        <v>18</v>
+      </c>
+      <c r="L31">
+        <v>26</v>
+      </c>
+      <c r="M31">
+        <v>14</v>
+      </c>
+      <c r="O31">
+        <v>13</v>
+      </c>
+      <c r="P31">
+        <v>22</v>
+      </c>
+      <c r="Q31">
+        <v>27</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>20</v>
+      </c>
+      <c r="T31">
+        <v>6</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31">
+        <v>20</v>
+      </c>
+      <c r="W31">
+        <v>16</v>
+      </c>
+      <c r="X31">
+        <v>18</v>
+      </c>
+      <c r="Y31">
+        <v>16</v>
+      </c>
+      <c r="Z31">
+        <v>12</v>
+      </c>
+      <c r="AA31">
+        <v>8</v>
+      </c>
+      <c r="AC31">
+        <v>22</v>
+      </c>
+      <c r="AG31">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <v>6</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+      <c r="O32">
+        <v>3</v>
+      </c>
+      <c r="Q32">
+        <v>2</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+      <c r="V32">
+        <v>3</v>
+      </c>
+      <c r="W32">
+        <v>2</v>
+      </c>
+      <c r="X32">
+        <v>5</v>
+      </c>
+      <c r="Z32">
+        <v>4</v>
+      </c>
+      <c r="AC32">
+        <v>3</v>
+      </c>
+      <c r="AG32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>9</v>
+      </c>
+      <c r="J33">
+        <v>5</v>
+      </c>
+      <c r="K33">
+        <v>4</v>
+      </c>
+      <c r="L33">
+        <v>4</v>
+      </c>
+      <c r="M33">
+        <v>2</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <v>7</v>
+      </c>
+      <c r="Q33">
+        <v>7</v>
+      </c>
+      <c r="R33">
+        <v>2</v>
+      </c>
+      <c r="S33">
+        <v>6</v>
+      </c>
+      <c r="T33">
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <v>6</v>
+      </c>
+      <c r="X33">
+        <v>2</v>
+      </c>
+      <c r="Y33">
+        <v>4</v>
+      </c>
+      <c r="Z33">
+        <v>3</v>
+      </c>
+      <c r="AA33">
+        <v>6</v>
+      </c>
+      <c r="AG33">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34">
+        <v>43</v>
+      </c>
+      <c r="D34">
+        <v>18</v>
+      </c>
+      <c r="E34">
+        <v>30</v>
+      </c>
+      <c r="F34">
+        <v>21</v>
+      </c>
+      <c r="H34">
+        <v>37</v>
+      </c>
+      <c r="I34">
+        <v>36</v>
+      </c>
+      <c r="J34">
+        <v>37</v>
+      </c>
+      <c r="K34">
+        <v>31</v>
+      </c>
+      <c r="L34">
+        <v>24</v>
+      </c>
+      <c r="M34">
+        <v>16</v>
+      </c>
+      <c r="O34">
+        <v>39</v>
+      </c>
+      <c r="P34">
+        <v>29</v>
+      </c>
+      <c r="Q34">
+        <v>40</v>
+      </c>
+      <c r="R34">
+        <v>2</v>
+      </c>
+      <c r="S34">
+        <v>21</v>
+      </c>
+      <c r="T34">
+        <v>16</v>
+      </c>
+      <c r="U34">
+        <v>1</v>
+      </c>
+      <c r="W34">
+        <v>48</v>
+      </c>
+      <c r="X34">
+        <v>32</v>
+      </c>
+      <c r="Y34">
+        <v>22</v>
+      </c>
+      <c r="Z34">
+        <v>25</v>
+      </c>
+      <c r="AA34">
+        <v>16</v>
+      </c>
+      <c r="AC34">
+        <v>40</v>
+      </c>
+      <c r="AG34">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>19</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>7</v>
+      </c>
+      <c r="E35">
+        <v>25</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>38</v>
+      </c>
+      <c r="I35">
+        <v>32</v>
+      </c>
+      <c r="J35">
+        <v>32</v>
+      </c>
+      <c r="K35">
+        <v>10</v>
+      </c>
+      <c r="L35">
+        <v>33</v>
+      </c>
+      <c r="M35">
+        <v>4</v>
+      </c>
+      <c r="N35">
+        <v>3</v>
+      </c>
+      <c r="O35">
+        <v>29</v>
+      </c>
+      <c r="P35">
+        <v>24</v>
+      </c>
+      <c r="Q35">
+        <v>18</v>
+      </c>
+      <c r="R35">
+        <v>4</v>
+      </c>
+      <c r="S35">
+        <v>2</v>
+      </c>
+      <c r="T35">
+        <v>9</v>
+      </c>
+      <c r="U35">
+        <v>3</v>
+      </c>
+      <c r="V35">
+        <v>1</v>
+      </c>
+      <c r="W35">
+        <v>47</v>
+      </c>
+      <c r="X35">
+        <v>42</v>
+      </c>
+      <c r="Y35">
+        <v>37</v>
+      </c>
+      <c r="Z35">
+        <v>28</v>
+      </c>
+      <c r="AA35">
+        <v>14</v>
+      </c>
+      <c r="AC35">
+        <v>41</v>
+      </c>
+      <c r="AG35">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36">
+        <v>28</v>
+      </c>
+      <c r="D36">
+        <v>17</v>
+      </c>
+      <c r="E36">
+        <v>16</v>
+      </c>
+      <c r="F36">
+        <v>7</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>15</v>
+      </c>
+      <c r="I36">
+        <v>18</v>
+      </c>
+      <c r="J36">
+        <v>13</v>
+      </c>
+      <c r="K36">
+        <v>19</v>
+      </c>
+      <c r="L36">
+        <v>17</v>
+      </c>
+      <c r="M36">
+        <v>8</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>21</v>
+      </c>
+      <c r="P36">
+        <v>14</v>
+      </c>
+      <c r="Q36">
+        <v>22</v>
+      </c>
+      <c r="S36">
+        <v>11</v>
+      </c>
+      <c r="T36">
+        <v>10</v>
+      </c>
+      <c r="U36">
+        <v>1</v>
+      </c>
+      <c r="V36">
+        <v>13</v>
+      </c>
+      <c r="W36">
+        <v>19</v>
+      </c>
+      <c r="X36">
+        <v>7</v>
+      </c>
+      <c r="Y36">
+        <v>17</v>
+      </c>
+      <c r="Z36">
+        <v>16</v>
+      </c>
+      <c r="AA36">
+        <v>11</v>
+      </c>
+      <c r="AC36">
+        <v>19</v>
+      </c>
+      <c r="AG36">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <v>76</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>47</v>
+      </c>
+      <c r="E37">
+        <v>56</v>
+      </c>
+      <c r="F37">
+        <v>30</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>57</v>
+      </c>
+      <c r="I37">
+        <v>67</v>
+      </c>
+      <c r="J37">
+        <v>71</v>
+      </c>
+      <c r="K37">
+        <v>66</v>
+      </c>
+      <c r="L37">
+        <v>72</v>
+      </c>
+      <c r="M37">
+        <v>40</v>
+      </c>
+      <c r="N37">
+        <v>6</v>
+      </c>
+      <c r="O37">
+        <v>76</v>
+      </c>
+      <c r="P37">
+        <v>60</v>
+      </c>
+      <c r="Q37">
+        <v>64</v>
+      </c>
+      <c r="R37">
+        <v>5</v>
+      </c>
+      <c r="S37">
+        <v>43</v>
+      </c>
+      <c r="T37">
+        <v>49</v>
+      </c>
+      <c r="U37">
+        <v>7</v>
+      </c>
+      <c r="V37">
+        <v>64</v>
+      </c>
+      <c r="W37">
+        <v>82</v>
+      </c>
+      <c r="X37">
+        <v>70</v>
+      </c>
+      <c r="Y37">
+        <v>51</v>
+      </c>
+      <c r="Z37">
+        <v>61</v>
+      </c>
+      <c r="AA37">
+        <v>31</v>
+      </c>
+      <c r="AB37">
+        <v>3</v>
+      </c>
+      <c r="AC37">
+        <v>65</v>
+      </c>
+      <c r="AG37">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38">
+        <v>19</v>
+      </c>
+      <c r="D38">
+        <v>9</v>
+      </c>
+      <c r="E38">
+        <v>19</v>
+      </c>
+      <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>10</v>
+      </c>
+      <c r="I38">
+        <v>16</v>
+      </c>
+      <c r="J38">
+        <v>15</v>
+      </c>
+      <c r="K38">
+        <v>16</v>
+      </c>
+      <c r="L38">
+        <v>7</v>
+      </c>
+      <c r="M38">
+        <v>13</v>
+      </c>
+      <c r="O38">
+        <v>25</v>
+      </c>
+      <c r="P38">
+        <v>12</v>
+      </c>
+      <c r="Q38">
+        <v>17</v>
+      </c>
+      <c r="S38">
+        <v>15</v>
+      </c>
+      <c r="T38">
+        <v>8</v>
+      </c>
+      <c r="V38">
+        <v>17</v>
+      </c>
+      <c r="W38">
+        <v>14</v>
+      </c>
+      <c r="X38">
+        <v>14</v>
+      </c>
+      <c r="Y38">
+        <v>8</v>
+      </c>
+      <c r="Z38">
+        <v>12</v>
+      </c>
+      <c r="AA38">
+        <v>6</v>
+      </c>
+      <c r="AC38">
+        <v>22</v>
+      </c>
+      <c r="AG38">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>64</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>36</v>
+      </c>
+      <c r="F39">
+        <v>24</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>37</v>
+      </c>
+      <c r="I39">
+        <v>40</v>
+      </c>
+      <c r="J39">
+        <v>39</v>
+      </c>
+      <c r="K39">
+        <v>40</v>
+      </c>
+      <c r="L39">
+        <v>38</v>
+      </c>
+      <c r="M39">
+        <v>28</v>
+      </c>
+      <c r="N39">
+        <v>4</v>
+      </c>
+      <c r="O39">
+        <v>36</v>
+      </c>
+      <c r="P39">
+        <v>34</v>
+      </c>
+      <c r="Q39">
+        <v>45</v>
+      </c>
+      <c r="S39">
+        <v>2</v>
+      </c>
+      <c r="T39">
+        <v>29</v>
+      </c>
+      <c r="V39">
+        <v>5</v>
+      </c>
+      <c r="W39">
+        <v>58</v>
+      </c>
+      <c r="X39">
+        <v>48</v>
+      </c>
+      <c r="Y39">
+        <v>28</v>
+      </c>
+      <c r="Z39">
+        <v>53</v>
+      </c>
+      <c r="AA39">
+        <v>23</v>
+      </c>
+      <c r="AB39">
+        <v>2</v>
+      </c>
+      <c r="AC39">
+        <v>29</v>
+      </c>
+      <c r="AG39">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
+      <c r="K40">
+        <v>5</v>
+      </c>
+      <c r="P40">
+        <v>5</v>
+      </c>
+      <c r="T40">
+        <v>2</v>
+      </c>
+      <c r="W40">
+        <v>9</v>
+      </c>
+      <c r="Y40">
+        <v>2</v>
+      </c>
+      <c r="Z40">
+        <v>1</v>
+      </c>
+      <c r="AA40">
+        <v>2</v>
+      </c>
+      <c r="AG40">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41">
+        <v>6</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>4</v>
+      </c>
+      <c r="J41">
+        <v>4</v>
+      </c>
+      <c r="K41">
+        <v>2</v>
+      </c>
+      <c r="L41">
+        <v>5</v>
+      </c>
+      <c r="M41">
+        <v>2</v>
+      </c>
+      <c r="P41">
+        <v>2</v>
+      </c>
+      <c r="Q41">
+        <v>4</v>
+      </c>
+      <c r="R41">
+        <v>2</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="W41">
+        <v>2</v>
+      </c>
+      <c r="X41">
+        <v>3</v>
+      </c>
+      <c r="Y41">
+        <v>1</v>
+      </c>
+      <c r="Z41">
+        <v>5</v>
+      </c>
+      <c r="AA41">
+        <v>1</v>
+      </c>
+      <c r="AG41">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <v>12</v>
+      </c>
+      <c r="E42">
+        <v>11</v>
+      </c>
+      <c r="H42">
+        <v>10</v>
+      </c>
+      <c r="I42">
+        <v>5</v>
+      </c>
+      <c r="J42">
+        <v>3</v>
+      </c>
+      <c r="K42">
+        <v>22</v>
+      </c>
+      <c r="L42">
+        <v>15</v>
+      </c>
+      <c r="O42">
+        <v>15</v>
+      </c>
+      <c r="R42">
+        <v>12</v>
+      </c>
+      <c r="S42">
+        <v>15</v>
+      </c>
+      <c r="W42">
+        <v>12</v>
+      </c>
+      <c r="X42">
+        <v>10</v>
+      </c>
+      <c r="Y42">
+        <v>16</v>
+      </c>
+      <c r="Z42">
+        <v>8</v>
+      </c>
+      <c r="AA42">
+        <v>1</v>
+      </c>
+      <c r="AC42">
+        <v>12</v>
+      </c>
+      <c r="AG42">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43">
+        <v>63</v>
+      </c>
+      <c r="D43">
+        <v>86</v>
+      </c>
+      <c r="E43">
+        <v>53</v>
+      </c>
+      <c r="H43">
+        <v>50</v>
+      </c>
+      <c r="I43">
+        <v>63</v>
+      </c>
+      <c r="J43">
+        <v>41</v>
+      </c>
+      <c r="K43">
+        <v>63</v>
+      </c>
+      <c r="L43">
+        <v>62</v>
+      </c>
+      <c r="O43">
+        <v>76</v>
+      </c>
+      <c r="P43">
+        <v>61</v>
+      </c>
+      <c r="Q43">
+        <v>58</v>
+      </c>
+      <c r="R43">
+        <v>62</v>
+      </c>
+      <c r="S43">
+        <v>39</v>
+      </c>
+      <c r="W43">
+        <v>65</v>
+      </c>
+      <c r="X43">
+        <v>82</v>
+      </c>
+      <c r="Y43">
+        <v>97</v>
+      </c>
+      <c r="Z43">
+        <v>49</v>
+      </c>
+      <c r="AC43">
+        <v>71</v>
+      </c>
+      <c r="AG43">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>6</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>7</v>
+      </c>
+      <c r="I44">
+        <v>11</v>
+      </c>
+      <c r="K44">
+        <v>16</v>
+      </c>
+      <c r="L44">
+        <v>6</v>
+      </c>
+      <c r="O44">
+        <v>6</v>
+      </c>
+      <c r="P44">
+        <v>5</v>
+      </c>
+      <c r="Q44">
+        <v>3</v>
+      </c>
+      <c r="R44">
+        <v>3</v>
+      </c>
+      <c r="S44">
+        <v>3</v>
+      </c>
+      <c r="W44">
+        <v>4</v>
+      </c>
+      <c r="X44">
+        <v>4</v>
+      </c>
+      <c r="Y44">
+        <v>1</v>
+      </c>
+      <c r="Z44">
+        <v>1</v>
+      </c>
+      <c r="AG44">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45">
+        <v>14</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="H45">
+        <v>8</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>2</v>
+      </c>
+      <c r="L45">
+        <v>9</v>
+      </c>
+      <c r="O45">
+        <v>11</v>
+      </c>
+      <c r="P45">
+        <v>2</v>
+      </c>
+      <c r="R45">
+        <v>3</v>
+      </c>
+      <c r="S45">
+        <v>2</v>
+      </c>
+      <c r="W45">
+        <v>8</v>
+      </c>
+      <c r="X45">
+        <v>6</v>
+      </c>
+      <c r="Y45">
+        <v>7</v>
+      </c>
+      <c r="Z45">
+        <v>3</v>
+      </c>
+      <c r="AC45">
+        <v>10</v>
+      </c>
+      <c r="AG45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>41</v>
+      </c>
+      <c r="E46">
+        <v>9</v>
+      </c>
+      <c r="I46">
+        <v>10</v>
+      </c>
+      <c r="J46">
+        <v>16</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="Q46">
+        <v>55</v>
+      </c>
+      <c r="R46">
+        <v>16</v>
+      </c>
+      <c r="W46">
+        <v>7</v>
+      </c>
+      <c r="X46">
+        <v>17</v>
+      </c>
+      <c r="Y46">
+        <v>20</v>
+      </c>
+      <c r="Z46">
+        <v>8</v>
+      </c>
+      <c r="AC46">
+        <v>2</v>
+      </c>
+      <c r="AG46">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>8</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>5</v>
+      </c>
+      <c r="J47">
+        <v>14</v>
+      </c>
+      <c r="K47">
+        <v>6</v>
+      </c>
+      <c r="L47">
+        <v>8</v>
+      </c>
+      <c r="M47">
+        <v>3</v>
+      </c>
+      <c r="O47">
+        <v>10</v>
+      </c>
+      <c r="Q47">
+        <v>15</v>
+      </c>
+      <c r="R47">
+        <v>2</v>
+      </c>
+      <c r="S47">
+        <v>7</v>
+      </c>
+      <c r="V47">
+        <v>2</v>
+      </c>
+      <c r="X47">
+        <v>7</v>
+      </c>
+      <c r="Y47">
+        <v>7</v>
+      </c>
+      <c r="Z47">
+        <v>7</v>
+      </c>
+      <c r="AA47">
+        <v>3</v>
+      </c>
+      <c r="AB47">
+        <v>1</v>
+      </c>
+      <c r="AC47">
+        <v>7</v>
+      </c>
+      <c r="AG47">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48">
+        <v>26</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>19</v>
+      </c>
+      <c r="E48">
+        <v>18</v>
+      </c>
+      <c r="F48">
+        <v>8</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
+      </c>
+      <c r="H48">
+        <v>16</v>
+      </c>
+      <c r="I48">
+        <v>15</v>
+      </c>
+      <c r="J48">
+        <v>19</v>
+      </c>
+      <c r="K48">
+        <v>17</v>
+      </c>
+      <c r="L48">
+        <v>23</v>
+      </c>
+      <c r="M48">
+        <v>7</v>
+      </c>
+      <c r="O48">
+        <v>18</v>
+      </c>
+      <c r="P48">
+        <v>46</v>
+      </c>
+      <c r="Q48">
+        <v>17</v>
+      </c>
+      <c r="R48">
+        <v>7</v>
+      </c>
+      <c r="S48">
+        <v>35</v>
+      </c>
+      <c r="T48">
+        <v>7</v>
+      </c>
+      <c r="V48">
+        <v>1</v>
+      </c>
+      <c r="W48">
+        <v>30</v>
+      </c>
+      <c r="X48">
+        <v>16</v>
+      </c>
+      <c r="Y48">
+        <v>19</v>
+      </c>
+      <c r="Z48">
+        <v>17</v>
+      </c>
+      <c r="AA48">
+        <v>7</v>
+      </c>
+      <c r="AC48">
+        <v>20</v>
+      </c>
+      <c r="AG48">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49">
+        <v>47</v>
+      </c>
+      <c r="C49">
+        <v>19</v>
+      </c>
+      <c r="D49">
+        <v>22</v>
+      </c>
+      <c r="E49">
+        <v>37</v>
+      </c>
+      <c r="F49">
+        <v>18</v>
+      </c>
+      <c r="H49">
+        <v>32</v>
+      </c>
+      <c r="I49">
+        <v>35</v>
+      </c>
+      <c r="J49">
+        <v>47</v>
+      </c>
+      <c r="K49">
+        <v>23</v>
+      </c>
+      <c r="L49">
+        <v>25</v>
+      </c>
+      <c r="M49">
+        <v>20</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>27</v>
+      </c>
+      <c r="P49">
+        <v>30</v>
+      </c>
+      <c r="Q49">
+        <v>31</v>
+      </c>
+      <c r="R49">
+        <v>22</v>
+      </c>
+      <c r="S49">
+        <v>29</v>
+      </c>
+      <c r="T49">
+        <v>13</v>
+      </c>
+      <c r="V49">
+        <v>40</v>
+      </c>
+      <c r="W49">
+        <v>26</v>
+      </c>
+      <c r="X49">
+        <v>34</v>
+      </c>
+      <c r="Y49">
+        <v>25</v>
+      </c>
+      <c r="Z49">
+        <v>25</v>
+      </c>
+      <c r="AA49">
+        <v>16</v>
+      </c>
+      <c r="AB49">
+        <v>1</v>
+      </c>
+      <c r="AC49">
+        <v>37</v>
+      </c>
+      <c r="AG49">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50">
+        <v>23</v>
+      </c>
+      <c r="C50">
+        <v>11</v>
+      </c>
+      <c r="D50">
+        <v>16</v>
+      </c>
+      <c r="E50">
+        <v>27</v>
+      </c>
+      <c r="F50">
+        <v>13</v>
+      </c>
+      <c r="H50">
+        <v>37</v>
+      </c>
+      <c r="I50">
+        <v>28</v>
+      </c>
+      <c r="J50">
+        <v>21</v>
+      </c>
+      <c r="K50">
+        <v>24</v>
+      </c>
+      <c r="L50">
+        <v>21</v>
+      </c>
+      <c r="M50">
+        <v>10</v>
+      </c>
+      <c r="O50">
+        <v>33</v>
+      </c>
+      <c r="P50">
+        <v>29</v>
+      </c>
+      <c r="Q50">
+        <v>12</v>
+      </c>
+      <c r="R50">
+        <v>21</v>
+      </c>
+      <c r="S50">
+        <v>20</v>
+      </c>
+      <c r="T50">
+        <v>11</v>
+      </c>
+      <c r="V50">
+        <v>21</v>
+      </c>
+      <c r="W50">
+        <v>11</v>
+      </c>
+      <c r="X50">
+        <v>13</v>
+      </c>
+      <c r="Y50">
+        <v>14</v>
+      </c>
+      <c r="Z50">
+        <v>28</v>
+      </c>
+      <c r="AA50">
+        <v>12</v>
+      </c>
+      <c r="AB50">
+        <v>3</v>
+      </c>
+      <c r="AC50">
+        <v>28</v>
+      </c>
+      <c r="AG50">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51">
+        <v>31</v>
+      </c>
+      <c r="D51">
+        <v>5</v>
+      </c>
+      <c r="E51">
+        <v>17</v>
+      </c>
+      <c r="F51">
+        <v>4</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>22</v>
+      </c>
+      <c r="I51">
+        <v>33</v>
+      </c>
+      <c r="J51">
+        <v>37</v>
+      </c>
+      <c r="K51">
+        <v>15</v>
+      </c>
+      <c r="L51">
+        <v>18</v>
+      </c>
+      <c r="M51">
+        <v>5</v>
+      </c>
+      <c r="O51">
+        <v>18</v>
+      </c>
+      <c r="P51">
+        <v>40</v>
+      </c>
+      <c r="Q51">
+        <v>26</v>
+      </c>
+      <c r="R51">
+        <v>1</v>
+      </c>
+      <c r="S51">
+        <v>20</v>
+      </c>
+      <c r="T51">
+        <v>4</v>
+      </c>
+      <c r="V51">
+        <v>22</v>
+      </c>
+      <c r="W51">
+        <v>14</v>
+      </c>
+      <c r="X51">
+        <v>35</v>
+      </c>
+      <c r="Y51">
+        <v>12</v>
+      </c>
+      <c r="Z51">
+        <v>23</v>
+      </c>
+      <c r="AA51">
+        <v>5</v>
+      </c>
+      <c r="AB51">
+        <v>1</v>
+      </c>
+      <c r="AC51">
+        <v>22</v>
+      </c>
+      <c r="AG51">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52">
+        <v>49</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>30</v>
+      </c>
+      <c r="E52">
+        <v>46</v>
+      </c>
+      <c r="F52">
+        <v>15</v>
+      </c>
+      <c r="G52">
+        <v>12</v>
+      </c>
+      <c r="H52">
+        <v>39</v>
+      </c>
+      <c r="I52">
+        <v>28</v>
+      </c>
+      <c r="J52">
+        <v>49</v>
+      </c>
+      <c r="K52">
+        <v>33</v>
+      </c>
+      <c r="L52">
+        <v>50</v>
+      </c>
+      <c r="M52">
+        <v>19</v>
+      </c>
+      <c r="N52">
+        <v>18</v>
+      </c>
+      <c r="O52">
+        <v>38</v>
+      </c>
+      <c r="P52">
+        <v>39</v>
+      </c>
+      <c r="Q52">
+        <v>47</v>
+      </c>
+      <c r="R52">
+        <v>2</v>
+      </c>
+      <c r="S52">
+        <v>32</v>
+      </c>
+      <c r="T52">
+        <v>21</v>
+      </c>
+      <c r="U52">
+        <v>16</v>
+      </c>
+      <c r="V52">
+        <v>39</v>
+      </c>
+      <c r="W52">
+        <v>29</v>
+      </c>
+      <c r="X52">
+        <v>40</v>
+      </c>
+      <c r="Y52">
+        <v>35</v>
+      </c>
+      <c r="Z52">
+        <v>32</v>
+      </c>
+      <c r="AA52">
+        <v>30</v>
+      </c>
+      <c r="AB52">
+        <v>13</v>
+      </c>
+      <c r="AC52">
+        <v>36</v>
+      </c>
+      <c r="AG52">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="E53">
+        <v>7</v>
+      </c>
+      <c r="F53">
+        <v>6</v>
+      </c>
+      <c r="H53">
+        <v>5</v>
+      </c>
+      <c r="I53">
+        <v>3</v>
+      </c>
+      <c r="J53">
+        <v>9</v>
+      </c>
+      <c r="K53">
+        <v>4</v>
+      </c>
+      <c r="L53">
+        <v>3</v>
+      </c>
+      <c r="M53">
+        <v>7</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <v>7</v>
+      </c>
+      <c r="P53">
+        <v>8</v>
+      </c>
+      <c r="Q53">
+        <v>8</v>
+      </c>
+      <c r="R53">
+        <v>2</v>
+      </c>
+      <c r="S53">
+        <v>4</v>
+      </c>
+      <c r="T53">
+        <v>1</v>
+      </c>
+      <c r="V53">
+        <v>2</v>
+      </c>
+      <c r="W53">
+        <v>2</v>
+      </c>
+      <c r="X53">
+        <v>9</v>
+      </c>
+      <c r="Y53">
+        <v>3</v>
+      </c>
+      <c r="Z53">
+        <v>2</v>
+      </c>
+      <c r="AA53">
+        <v>3</v>
+      </c>
+      <c r="AC53">
+        <v>10</v>
+      </c>
+      <c r="AG53">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54">
+        <v>17</v>
+      </c>
+      <c r="C54">
+        <v>5</v>
+      </c>
+      <c r="D54">
+        <v>9</v>
+      </c>
+      <c r="E54">
+        <v>14</v>
+      </c>
+      <c r="F54">
+        <v>14</v>
+      </c>
+      <c r="H54">
+        <v>11</v>
+      </c>
+      <c r="I54">
+        <v>21</v>
+      </c>
+      <c r="J54">
+        <v>28</v>
+      </c>
+      <c r="K54">
+        <v>11</v>
+      </c>
+      <c r="L54">
+        <v>17</v>
+      </c>
+      <c r="M54">
+        <v>4</v>
+      </c>
+      <c r="N54">
+        <v>2</v>
+      </c>
+      <c r="O54">
+        <v>16</v>
+      </c>
+      <c r="P54">
+        <v>18</v>
+      </c>
+      <c r="Q54">
+        <v>25</v>
+      </c>
+      <c r="S54">
+        <v>15</v>
+      </c>
+      <c r="T54">
+        <v>15</v>
+      </c>
+      <c r="U54">
+        <v>1</v>
+      </c>
+      <c r="V54">
+        <v>8</v>
+      </c>
+      <c r="W54">
+        <v>32</v>
+      </c>
+      <c r="X54">
+        <v>15</v>
+      </c>
+      <c r="Y54">
+        <v>15</v>
+      </c>
+      <c r="Z54">
+        <v>17</v>
+      </c>
+      <c r="AA54">
+        <v>6</v>
+      </c>
+      <c r="AB54">
+        <v>3</v>
+      </c>
+      <c r="AC54">
+        <v>19</v>
+      </c>
+      <c r="AG54">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="H55">
+        <v>6</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+      <c r="J55">
+        <v>3</v>
+      </c>
+      <c r="K55">
+        <v>2</v>
+      </c>
+      <c r="L55">
+        <v>2</v>
+      </c>
+      <c r="M55">
+        <v>2</v>
+      </c>
+      <c r="O55">
+        <v>4</v>
+      </c>
+      <c r="P55">
+        <v>1</v>
+      </c>
+      <c r="Q55">
+        <v>5</v>
+      </c>
+      <c r="R55">
+        <v>1</v>
+      </c>
+      <c r="S55">
+        <v>3</v>
+      </c>
+      <c r="T55">
+        <v>3</v>
+      </c>
+      <c r="V55">
+        <v>2</v>
+      </c>
+      <c r="W55">
+        <v>1</v>
+      </c>
+      <c r="X55">
+        <v>2</v>
+      </c>
+      <c r="Y55">
+        <v>1</v>
+      </c>
+      <c r="Z55">
+        <v>6</v>
+      </c>
+      <c r="AA55">
+        <v>1</v>
+      </c>
+      <c r="AC55">
+        <v>3</v>
+      </c>
+      <c r="AG55">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>2</v>
+      </c>
+      <c r="I56">
+        <v>5</v>
+      </c>
+      <c r="J56">
+        <v>4</v>
+      </c>
+      <c r="K56">
+        <v>4</v>
+      </c>
+      <c r="M56">
+        <v>2</v>
+      </c>
+      <c r="O56">
+        <v>2</v>
+      </c>
+      <c r="P56">
+        <v>3</v>
+      </c>
+      <c r="Q56">
+        <v>7</v>
+      </c>
+      <c r="T56">
+        <v>2</v>
+      </c>
+      <c r="U56">
+        <v>1</v>
+      </c>
+      <c r="W56">
+        <v>3</v>
+      </c>
+      <c r="X56">
+        <v>1</v>
+      </c>
+      <c r="Y56">
+        <v>2</v>
+      </c>
+      <c r="AA56">
+        <v>3</v>
+      </c>
+      <c r="AC56">
+        <v>2</v>
+      </c>
+      <c r="AG56">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57">
+        <v>8</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>6</v>
+      </c>
+      <c r="E57">
+        <v>7</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="H57">
+        <v>10</v>
+      </c>
+      <c r="I57">
+        <v>8</v>
+      </c>
+      <c r="J57">
+        <v>3</v>
+      </c>
+      <c r="K57">
+        <v>12</v>
+      </c>
+      <c r="L57">
+        <v>7</v>
+      </c>
+      <c r="M57">
+        <v>2</v>
+      </c>
+      <c r="N57">
+        <v>2</v>
+      </c>
+      <c r="O57">
+        <v>8</v>
+      </c>
+      <c r="P57">
+        <v>7</v>
+      </c>
+      <c r="Q57">
+        <v>5</v>
+      </c>
+      <c r="S57">
+        <v>9</v>
+      </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
+      <c r="V57">
+        <v>11</v>
+      </c>
+      <c r="W57">
+        <v>6</v>
+      </c>
+      <c r="X57">
+        <v>7</v>
+      </c>
+      <c r="Y57">
+        <v>3</v>
+      </c>
+      <c r="Z57">
+        <v>9</v>
+      </c>
+      <c r="AA57">
+        <v>1</v>
+      </c>
+      <c r="AC57">
+        <v>6</v>
+      </c>
+      <c r="AG57">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update all files for April 5
</commit_message>
<xml_diff>
--- a/statistics_files/2022/2022.d.monthly_circ_by_borrower.unique_borrowers.xlsx
+++ b/statistics_files/2022/2022.d.monthly_circ_by_borrower.unique_borrowers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A66554F-3B36-486B-B546-3874B61C89EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B9A3B3-2BA5-4C8C-AED6-6E6B33046CFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="894" activeTab="1" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="894" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="2" r:id="rId1"/>
@@ -28,6 +28,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">January!$A$3:$AG$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">March!$A$3:$AG$57</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="70">
   <si>
     <t>branchname</t>
   </si>
@@ -246,6 +247,9 @@
   </si>
   <si>
     <t>2022-02-01 - 2022-02-28</t>
+  </si>
+  <si>
+    <t>2022-03-01 - 2022-03-30</t>
   </si>
 </sst>
 </file>
@@ -615,7 +619,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -5220,7 +5224,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -9372,7 +9376,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A65A5CD-B538-4B7C-B2A7-48592120D8ED}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="B2:AF2"/>
+  <dimension ref="A1:AG57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
@@ -9387,40 +9391,4556 @@
     <col min="2" max="33" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44621</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44622</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44623</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44624</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44625</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44626</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44627</v>
+      </c>
+      <c r="I2" s="1">
+        <v>44628</v>
+      </c>
+      <c r="J2" s="1">
+        <v>44629</v>
+      </c>
+      <c r="K2" s="1">
+        <v>44630</v>
+      </c>
+      <c r="L2" s="1">
+        <v>44631</v>
+      </c>
+      <c r="M2" s="1">
+        <v>44632</v>
+      </c>
+      <c r="N2" s="1">
+        <v>44633</v>
+      </c>
+      <c r="O2" s="1">
+        <v>44634</v>
+      </c>
+      <c r="P2" s="1">
+        <v>44635</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>44636</v>
+      </c>
+      <c r="R2" s="1">
+        <v>44637</v>
+      </c>
+      <c r="S2" s="1">
+        <v>44638</v>
+      </c>
+      <c r="T2" s="1">
+        <v>44639</v>
+      </c>
+      <c r="U2" s="1">
+        <v>44640</v>
+      </c>
+      <c r="V2" s="1">
+        <v>44641</v>
+      </c>
+      <c r="W2" s="1">
+        <v>44642</v>
+      </c>
+      <c r="X2" s="1">
+        <v>44643</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>44644</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>44645</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>44646</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>44647</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>44648</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>44649</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>44650</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>44651</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>72</v>
+      </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>66</v>
+      </c>
+      <c r="E4">
+        <v>65</v>
+      </c>
+      <c r="F4">
+        <v>49</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>38</v>
+      </c>
+      <c r="I4">
+        <v>60</v>
+      </c>
+      <c r="J4">
+        <v>78</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>42</v>
+      </c>
+      <c r="M4">
+        <v>29</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>59</v>
+      </c>
+      <c r="P4">
+        <v>59</v>
+      </c>
+      <c r="Q4">
+        <v>60</v>
+      </c>
+      <c r="R4">
+        <v>68</v>
+      </c>
+      <c r="S4">
+        <v>59</v>
+      </c>
+      <c r="T4">
+        <v>39</v>
+      </c>
+      <c r="U4">
+        <v>4</v>
+      </c>
+      <c r="V4">
+        <v>80</v>
+      </c>
+      <c r="W4">
+        <v>58</v>
+      </c>
+      <c r="X4">
+        <v>74</v>
+      </c>
+      <c r="Y4">
+        <v>81</v>
+      </c>
+      <c r="Z4">
+        <v>60</v>
+      </c>
+      <c r="AA4">
+        <v>30</v>
+      </c>
+      <c r="AB4">
+        <v>3</v>
+      </c>
+      <c r="AC4">
+        <v>82</v>
+      </c>
+      <c r="AD4">
+        <v>63</v>
+      </c>
+      <c r="AE4">
+        <v>57</v>
+      </c>
+      <c r="AF4">
+        <v>73</v>
+      </c>
+      <c r="AG4">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>34</v>
+      </c>
+      <c r="E5">
+        <v>31</v>
+      </c>
+      <c r="F5">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>34</v>
+      </c>
+      <c r="I5">
+        <v>30</v>
+      </c>
+      <c r="J5">
+        <v>45</v>
+      </c>
+      <c r="K5">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <v>35</v>
+      </c>
+      <c r="M5">
+        <v>22</v>
+      </c>
+      <c r="O5">
+        <v>34</v>
+      </c>
+      <c r="P5">
+        <v>37</v>
+      </c>
+      <c r="Q5">
+        <v>33</v>
+      </c>
+      <c r="R5">
+        <v>31</v>
+      </c>
+      <c r="S5">
+        <v>23</v>
+      </c>
+      <c r="T5">
+        <v>20</v>
+      </c>
+      <c r="U5">
+        <v>3</v>
+      </c>
+      <c r="V5">
+        <v>22</v>
+      </c>
+      <c r="W5">
+        <v>38</v>
+      </c>
+      <c r="X5">
+        <v>60</v>
+      </c>
+      <c r="Y5">
+        <v>38</v>
+      </c>
+      <c r="Z5">
+        <v>24</v>
+      </c>
+      <c r="AA5">
+        <v>12</v>
+      </c>
+      <c r="AB5">
+        <v>3</v>
+      </c>
+      <c r="AC5">
+        <v>33</v>
+      </c>
+      <c r="AD5">
+        <v>43</v>
+      </c>
+      <c r="AE5">
+        <v>41</v>
+      </c>
+      <c r="AF5">
+        <v>27</v>
+      </c>
+      <c r="AG5">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>80</v>
+      </c>
+      <c r="C6">
+        <v>83</v>
+      </c>
+      <c r="D6">
+        <v>86</v>
+      </c>
+      <c r="E6">
+        <v>56</v>
+      </c>
+      <c r="F6">
+        <v>68</v>
+      </c>
+      <c r="G6">
+        <v>35</v>
+      </c>
+      <c r="H6">
+        <v>57</v>
+      </c>
+      <c r="I6">
+        <v>84</v>
+      </c>
+      <c r="J6">
+        <v>98</v>
+      </c>
+      <c r="K6">
+        <v>31</v>
+      </c>
+      <c r="L6">
+        <v>52</v>
+      </c>
+      <c r="M6">
+        <v>59</v>
+      </c>
+      <c r="N6">
+        <v>37</v>
+      </c>
+      <c r="O6">
+        <v>72</v>
+      </c>
+      <c r="P6">
+        <v>86</v>
+      </c>
+      <c r="Q6">
+        <v>69</v>
+      </c>
+      <c r="R6">
+        <v>78</v>
+      </c>
+      <c r="S6">
+        <v>75</v>
+      </c>
+      <c r="T6">
+        <v>47</v>
+      </c>
+      <c r="U6">
+        <v>42</v>
+      </c>
+      <c r="V6">
+        <v>89</v>
+      </c>
+      <c r="W6">
+        <v>72</v>
+      </c>
+      <c r="X6">
+        <v>88</v>
+      </c>
+      <c r="Y6">
+        <v>73</v>
+      </c>
+      <c r="Z6">
+        <v>55</v>
+      </c>
+      <c r="AA6">
+        <v>53</v>
+      </c>
+      <c r="AB6">
+        <v>37</v>
+      </c>
+      <c r="AC6">
+        <v>90</v>
+      </c>
+      <c r="AD6">
+        <v>67</v>
+      </c>
+      <c r="AE6">
+        <v>99</v>
+      </c>
+      <c r="AF6">
+        <v>69</v>
+      </c>
+      <c r="AG6">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>4</v>
+      </c>
+      <c r="AC7">
+        <v>3</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <v>2</v>
+      </c>
+      <c r="AG7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>47</v>
+      </c>
+      <c r="C8">
+        <v>61</v>
+      </c>
+      <c r="D8">
+        <v>48</v>
+      </c>
+      <c r="E8">
+        <v>46</v>
+      </c>
+      <c r="F8">
+        <v>46</v>
+      </c>
+      <c r="G8">
+        <v>21</v>
+      </c>
+      <c r="H8">
+        <v>55</v>
+      </c>
+      <c r="I8">
+        <v>53</v>
+      </c>
+      <c r="J8">
+        <v>72</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>37</v>
+      </c>
+      <c r="M8">
+        <v>34</v>
+      </c>
+      <c r="N8">
+        <v>24</v>
+      </c>
+      <c r="O8">
+        <v>49</v>
+      </c>
+      <c r="P8">
+        <v>60</v>
+      </c>
+      <c r="Q8">
+        <v>53</v>
+      </c>
+      <c r="R8">
+        <v>44</v>
+      </c>
+      <c r="S8">
+        <v>34</v>
+      </c>
+      <c r="T8">
+        <v>42</v>
+      </c>
+      <c r="U8">
+        <v>17</v>
+      </c>
+      <c r="V8">
+        <v>60</v>
+      </c>
+      <c r="W8">
+        <v>46</v>
+      </c>
+      <c r="X8">
+        <v>59</v>
+      </c>
+      <c r="Y8">
+        <v>38</v>
+      </c>
+      <c r="Z8">
+        <v>40</v>
+      </c>
+      <c r="AA8">
+        <v>46</v>
+      </c>
+      <c r="AB8">
+        <v>23</v>
+      </c>
+      <c r="AC8">
+        <v>60</v>
+      </c>
+      <c r="AD8">
+        <v>56</v>
+      </c>
+      <c r="AE8">
+        <v>51</v>
+      </c>
+      <c r="AF8">
+        <v>37</v>
+      </c>
+      <c r="AG8">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <v>7</v>
+      </c>
+      <c r="P9">
+        <v>7</v>
+      </c>
+      <c r="Q9">
+        <v>12</v>
+      </c>
+      <c r="R9">
+        <v>10</v>
+      </c>
+      <c r="S9">
+        <v>8</v>
+      </c>
+      <c r="T9">
+        <v>5</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
+      <c r="W9">
+        <v>15</v>
+      </c>
+      <c r="X9">
+        <v>8</v>
+      </c>
+      <c r="Y9">
+        <v>7</v>
+      </c>
+      <c r="Z9">
+        <v>7</v>
+      </c>
+      <c r="AA9">
+        <v>5</v>
+      </c>
+      <c r="AC9">
+        <v>7</v>
+      </c>
+      <c r="AD9">
+        <v>6</v>
+      </c>
+      <c r="AE9">
+        <v>10</v>
+      </c>
+      <c r="AF9">
+        <v>13</v>
+      </c>
+      <c r="AG9">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>14</v>
+      </c>
+      <c r="F10">
+        <v>11</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <v>13</v>
+      </c>
+      <c r="L10">
+        <v>11</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="O10">
+        <v>17</v>
+      </c>
+      <c r="P10">
+        <v>11</v>
+      </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
+      <c r="R10">
+        <v>7</v>
+      </c>
+      <c r="S10">
+        <v>10</v>
+      </c>
+      <c r="T10">
+        <v>6</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>8</v>
+      </c>
+      <c r="W10">
+        <v>11</v>
+      </c>
+      <c r="X10">
+        <v>14</v>
+      </c>
+      <c r="Y10">
+        <v>12</v>
+      </c>
+      <c r="Z10">
+        <v>17</v>
+      </c>
+      <c r="AA10">
+        <v>8</v>
+      </c>
+      <c r="AC10">
+        <v>11</v>
+      </c>
+      <c r="AD10">
+        <v>4</v>
+      </c>
+      <c r="AE10">
+        <v>12</v>
+      </c>
+      <c r="AF10">
+        <v>7</v>
+      </c>
+      <c r="AG10">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
+      <c r="O11">
+        <v>7</v>
+      </c>
+      <c r="Q11">
+        <v>4</v>
+      </c>
+      <c r="R11">
+        <v>2</v>
+      </c>
+      <c r="S11">
+        <v>9</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>5</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>6</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>7</v>
+      </c>
+      <c r="AC11">
+        <v>4</v>
+      </c>
+      <c r="AE11">
+        <v>9</v>
+      </c>
+      <c r="AF11">
+        <v>3</v>
+      </c>
+      <c r="AG11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="AG12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>7</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="P14">
+        <v>3</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="S14">
+        <v>5</v>
+      </c>
+      <c r="W14">
+        <v>2</v>
+      </c>
+      <c r="X14">
+        <v>2</v>
+      </c>
+      <c r="Y14">
+        <v>4</v>
+      </c>
+      <c r="Z14">
+        <v>3</v>
+      </c>
+      <c r="AC14">
+        <v>1</v>
+      </c>
+      <c r="AD14">
+        <v>4</v>
+      </c>
+      <c r="AE14">
+        <v>1</v>
+      </c>
+      <c r="AF14">
+        <v>5</v>
+      </c>
+      <c r="AG14">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <v>11</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>7</v>
+      </c>
+      <c r="O15">
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <v>4</v>
+      </c>
+      <c r="Q15">
+        <v>8</v>
+      </c>
+      <c r="R15">
+        <v>10</v>
+      </c>
+      <c r="S15">
+        <v>7</v>
+      </c>
+      <c r="V15">
+        <v>5</v>
+      </c>
+      <c r="W15">
+        <v>3</v>
+      </c>
+      <c r="X15">
+        <v>9</v>
+      </c>
+      <c r="Y15">
+        <v>6</v>
+      </c>
+      <c r="Z15">
+        <v>7</v>
+      </c>
+      <c r="AC15">
+        <v>6</v>
+      </c>
+      <c r="AD15">
+        <v>4</v>
+      </c>
+      <c r="AE15">
+        <v>7</v>
+      </c>
+      <c r="AF15">
+        <v>6</v>
+      </c>
+      <c r="AG15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>13</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>6</v>
+      </c>
+      <c r="I16">
+        <v>9</v>
+      </c>
+      <c r="J16">
+        <v>14</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>7</v>
+      </c>
+      <c r="M16">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <v>16</v>
+      </c>
+      <c r="P16">
+        <v>12</v>
+      </c>
+      <c r="Q16">
+        <v>8</v>
+      </c>
+      <c r="R16">
+        <v>9</v>
+      </c>
+      <c r="S16">
+        <v>13</v>
+      </c>
+      <c r="T16">
+        <v>3</v>
+      </c>
+      <c r="V16">
+        <v>8</v>
+      </c>
+      <c r="W16">
+        <v>15</v>
+      </c>
+      <c r="X16">
+        <v>9</v>
+      </c>
+      <c r="Y16">
+        <v>15</v>
+      </c>
+      <c r="Z16">
+        <v>10</v>
+      </c>
+      <c r="AA16">
+        <v>11</v>
+      </c>
+      <c r="AC16">
+        <v>15</v>
+      </c>
+      <c r="AD16">
+        <v>14</v>
+      </c>
+      <c r="AE16">
+        <v>11</v>
+      </c>
+      <c r="AF16">
+        <v>11</v>
+      </c>
+      <c r="AG16">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <v>11</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>4</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="O17">
+        <v>8</v>
+      </c>
+      <c r="P17">
+        <v>3</v>
+      </c>
+      <c r="Q17">
+        <v>4</v>
+      </c>
+      <c r="R17">
+        <v>8</v>
+      </c>
+      <c r="S17">
+        <v>2</v>
+      </c>
+      <c r="T17">
+        <v>3</v>
+      </c>
+      <c r="V17">
+        <v>13</v>
+      </c>
+      <c r="W17">
+        <v>16</v>
+      </c>
+      <c r="X17">
+        <v>6</v>
+      </c>
+      <c r="Y17">
+        <v>6</v>
+      </c>
+      <c r="Z17">
+        <v>4</v>
+      </c>
+      <c r="AA17">
+        <v>2</v>
+      </c>
+      <c r="AC17">
+        <v>7</v>
+      </c>
+      <c r="AD17">
+        <v>5</v>
+      </c>
+      <c r="AE17">
+        <v>2</v>
+      </c>
+      <c r="AF17">
+        <v>5</v>
+      </c>
+      <c r="AG17">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>6</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>3</v>
+      </c>
+      <c r="R18">
+        <v>5</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>3</v>
+      </c>
+      <c r="V18">
+        <v>3</v>
+      </c>
+      <c r="W18">
+        <v>5</v>
+      </c>
+      <c r="X18">
+        <v>3</v>
+      </c>
+      <c r="Y18">
+        <v>3</v>
+      </c>
+      <c r="Z18">
+        <v>4</v>
+      </c>
+      <c r="AA18">
+        <v>4</v>
+      </c>
+      <c r="AC18">
+        <v>3</v>
+      </c>
+      <c r="AE18">
+        <v>4</v>
+      </c>
+      <c r="AF18">
+        <v>2</v>
+      </c>
+      <c r="AG18">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>27</v>
+      </c>
+      <c r="E19">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
+      <c r="H19">
+        <v>23</v>
+      </c>
+      <c r="I19">
+        <v>22</v>
+      </c>
+      <c r="J19">
+        <v>26</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>23</v>
+      </c>
+      <c r="M19">
+        <v>23</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+      <c r="O19">
+        <v>30</v>
+      </c>
+      <c r="P19">
+        <v>17</v>
+      </c>
+      <c r="Q19">
+        <v>20</v>
+      </c>
+      <c r="R19">
+        <v>15</v>
+      </c>
+      <c r="S19">
+        <v>11</v>
+      </c>
+      <c r="T19">
+        <v>19</v>
+      </c>
+      <c r="U19">
+        <v>2</v>
+      </c>
+      <c r="V19">
+        <v>40</v>
+      </c>
+      <c r="W19">
+        <v>23</v>
+      </c>
+      <c r="X19">
+        <v>19</v>
+      </c>
+      <c r="Y19">
+        <v>24</v>
+      </c>
+      <c r="Z19">
+        <v>13</v>
+      </c>
+      <c r="AA19">
+        <v>22</v>
+      </c>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
+        <v>16</v>
+      </c>
+      <c r="AD19">
+        <v>24</v>
+      </c>
+      <c r="AE19">
+        <v>29</v>
+      </c>
+      <c r="AF19">
+        <v>18</v>
+      </c>
+      <c r="AG19">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>3</v>
+      </c>
+      <c r="Q20">
+        <v>2</v>
+      </c>
+      <c r="R20">
+        <v>3</v>
+      </c>
+      <c r="S20">
+        <v>2</v>
+      </c>
+      <c r="T20">
+        <v>3</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>3</v>
+      </c>
+      <c r="X20">
+        <v>2</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>2</v>
+      </c>
+      <c r="AA20">
+        <v>1</v>
+      </c>
+      <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <v>3</v>
+      </c>
+      <c r="AD20">
+        <v>1</v>
+      </c>
+      <c r="AE20">
+        <v>4</v>
+      </c>
+      <c r="AF20">
+        <v>5</v>
+      </c>
+      <c r="AG20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>32</v>
+      </c>
+      <c r="D21">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>25</v>
+      </c>
+      <c r="F21">
+        <v>12</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>28</v>
+      </c>
+      <c r="I21">
+        <v>43</v>
+      </c>
+      <c r="J21">
+        <v>31</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>19</v>
+      </c>
+      <c r="M21">
+        <v>19</v>
+      </c>
+      <c r="N21">
+        <v>9</v>
+      </c>
+      <c r="O21">
+        <v>46</v>
+      </c>
+      <c r="P21">
+        <v>41</v>
+      </c>
+      <c r="Q21">
+        <v>5</v>
+      </c>
+      <c r="R21">
+        <v>39</v>
+      </c>
+      <c r="S21">
+        <v>23</v>
+      </c>
+      <c r="T21">
+        <v>15</v>
+      </c>
+      <c r="U21">
+        <v>9</v>
+      </c>
+      <c r="V21">
+        <v>36</v>
+      </c>
+      <c r="W21">
+        <v>46</v>
+      </c>
+      <c r="X21">
+        <v>32</v>
+      </c>
+      <c r="Y21">
+        <v>30</v>
+      </c>
+      <c r="Z21">
+        <v>30</v>
+      </c>
+      <c r="AA21">
+        <v>20</v>
+      </c>
+      <c r="AB21">
+        <v>5</v>
+      </c>
+      <c r="AC21">
+        <v>40</v>
+      </c>
+      <c r="AD21">
+        <v>43</v>
+      </c>
+      <c r="AE21">
+        <v>22</v>
+      </c>
+      <c r="AF21">
+        <v>31</v>
+      </c>
+      <c r="AG21">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>5</v>
+      </c>
+      <c r="W22">
+        <v>4</v>
+      </c>
+      <c r="X22">
+        <v>1</v>
+      </c>
+      <c r="Y22">
+        <v>2</v>
+      </c>
+      <c r="Z22">
+        <v>1</v>
+      </c>
+      <c r="AC22">
+        <v>1</v>
+      </c>
+      <c r="AD22">
+        <v>2</v>
+      </c>
+      <c r="AE22">
+        <v>2</v>
+      </c>
+      <c r="AF22">
+        <v>4</v>
+      </c>
+      <c r="AG22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>34</v>
+      </c>
+      <c r="C23">
+        <v>51</v>
+      </c>
+      <c r="D23">
+        <v>26</v>
+      </c>
+      <c r="E23">
+        <v>30</v>
+      </c>
+      <c r="F23">
+        <v>13</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>23</v>
+      </c>
+      <c r="I23">
+        <v>40</v>
+      </c>
+      <c r="J23">
+        <v>51</v>
+      </c>
+      <c r="L23">
+        <v>45</v>
+      </c>
+      <c r="M23">
+        <v>18</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>37</v>
+      </c>
+      <c r="P23">
+        <v>48</v>
+      </c>
+      <c r="Q23">
+        <v>33</v>
+      </c>
+      <c r="R23">
+        <v>52</v>
+      </c>
+      <c r="S23">
+        <v>7</v>
+      </c>
+      <c r="T23">
+        <v>23</v>
+      </c>
+      <c r="U23">
+        <v>2</v>
+      </c>
+      <c r="V23">
+        <v>45</v>
+      </c>
+      <c r="W23">
+        <v>39</v>
+      </c>
+      <c r="X23">
+        <v>28</v>
+      </c>
+      <c r="Y23">
+        <v>53</v>
+      </c>
+      <c r="Z23">
+        <v>29</v>
+      </c>
+      <c r="AA23">
+        <v>15</v>
+      </c>
+      <c r="AC23">
+        <v>32</v>
+      </c>
+      <c r="AD23">
+        <v>28</v>
+      </c>
+      <c r="AE23">
+        <v>27</v>
+      </c>
+      <c r="AF23">
+        <v>43</v>
+      </c>
+      <c r="AG23">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="O24">
+        <v>4</v>
+      </c>
+      <c r="P24">
+        <v>3</v>
+      </c>
+      <c r="Q24">
+        <v>3</v>
+      </c>
+      <c r="R24">
+        <v>3</v>
+      </c>
+      <c r="S24">
+        <v>3</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="V24">
+        <v>5</v>
+      </c>
+      <c r="W24">
+        <v>2</v>
+      </c>
+      <c r="X24">
+        <v>1</v>
+      </c>
+      <c r="Y24">
+        <v>1</v>
+      </c>
+      <c r="Z24">
+        <v>1</v>
+      </c>
+      <c r="AA24">
+        <v>1</v>
+      </c>
+      <c r="AB24">
+        <v>1</v>
+      </c>
+      <c r="AC24">
+        <v>3</v>
+      </c>
+      <c r="AD24">
+        <v>2</v>
+      </c>
+      <c r="AE24">
+        <v>1</v>
+      </c>
+      <c r="AF24">
+        <v>5</v>
+      </c>
+      <c r="AG24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>40</v>
+      </c>
+      <c r="D25">
+        <v>28</v>
+      </c>
+      <c r="E25">
+        <v>26</v>
+      </c>
+      <c r="F25">
+        <v>22</v>
+      </c>
+      <c r="H25">
+        <v>21</v>
+      </c>
+      <c r="I25">
+        <v>28</v>
+      </c>
+      <c r="J25">
+        <v>38</v>
+      </c>
+      <c r="K25">
+        <v>6</v>
+      </c>
+      <c r="L25">
+        <v>48</v>
+      </c>
+      <c r="M25">
+        <v>22</v>
+      </c>
+      <c r="O25">
+        <v>28</v>
+      </c>
+      <c r="P25">
+        <v>22</v>
+      </c>
+      <c r="Q25">
+        <v>34</v>
+      </c>
+      <c r="R25">
+        <v>13</v>
+      </c>
+      <c r="S25">
+        <v>29</v>
+      </c>
+      <c r="T25">
+        <v>19</v>
+      </c>
+      <c r="U25">
+        <v>6</v>
+      </c>
+      <c r="V25">
+        <v>35</v>
+      </c>
+      <c r="W25">
+        <v>29</v>
+      </c>
+      <c r="X25">
+        <v>32</v>
+      </c>
+      <c r="Y25">
+        <v>31</v>
+      </c>
+      <c r="Z25">
+        <v>28</v>
+      </c>
+      <c r="AA25">
+        <v>22</v>
+      </c>
+      <c r="AB25">
+        <v>1</v>
+      </c>
+      <c r="AC25">
+        <v>23</v>
+      </c>
+      <c r="AD25">
+        <v>29</v>
+      </c>
+      <c r="AE25">
+        <v>33</v>
+      </c>
+      <c r="AF25">
+        <v>29</v>
+      </c>
+      <c r="AG25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>106</v>
+      </c>
+      <c r="C26">
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>82</v>
+      </c>
+      <c r="E26">
+        <v>74</v>
+      </c>
+      <c r="F26">
+        <v>78</v>
+      </c>
+      <c r="G26">
+        <v>45</v>
+      </c>
+      <c r="H26">
+        <v>82</v>
+      </c>
+      <c r="I26">
+        <v>101</v>
+      </c>
+      <c r="J26">
+        <v>122</v>
+      </c>
+      <c r="K26">
+        <v>48</v>
+      </c>
+      <c r="L26">
+        <v>71</v>
+      </c>
+      <c r="M26">
+        <v>76</v>
+      </c>
+      <c r="N26">
+        <v>41</v>
+      </c>
+      <c r="O26">
+        <v>101</v>
+      </c>
+      <c r="P26">
+        <v>112</v>
+      </c>
+      <c r="Q26">
+        <v>95</v>
+      </c>
+      <c r="R26">
+        <v>64</v>
+      </c>
+      <c r="S26">
+        <v>89</v>
+      </c>
+      <c r="T26">
+        <v>58</v>
+      </c>
+      <c r="U26">
+        <v>23</v>
+      </c>
+      <c r="V26">
+        <v>116</v>
+      </c>
+      <c r="W26">
+        <v>93</v>
+      </c>
+      <c r="X26">
+        <v>108</v>
+      </c>
+      <c r="Y26">
+        <v>104</v>
+      </c>
+      <c r="Z26">
+        <v>77</v>
+      </c>
+      <c r="AA26">
+        <v>66</v>
+      </c>
+      <c r="AB26">
+        <v>34</v>
+      </c>
+      <c r="AC26">
+        <v>94</v>
+      </c>
+      <c r="AD26">
+        <v>95</v>
+      </c>
+      <c r="AE26">
+        <v>79</v>
+      </c>
+      <c r="AF26">
+        <v>88</v>
+      </c>
+      <c r="AG26">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>9</v>
+      </c>
+      <c r="E27">
+        <v>11</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="H27">
+        <v>13</v>
+      </c>
+      <c r="I27">
+        <v>11</v>
+      </c>
+      <c r="J27">
+        <v>8</v>
+      </c>
+      <c r="L27">
+        <v>11</v>
+      </c>
+      <c r="M27">
+        <v>4</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>8</v>
+      </c>
+      <c r="P27">
+        <v>5</v>
+      </c>
+      <c r="Q27">
+        <v>9</v>
+      </c>
+      <c r="R27">
+        <v>10</v>
+      </c>
+      <c r="S27">
+        <v>8</v>
+      </c>
+      <c r="T27">
+        <v>3</v>
+      </c>
+      <c r="V27">
+        <v>4</v>
+      </c>
+      <c r="W27">
+        <v>8</v>
+      </c>
+      <c r="X27">
+        <v>6</v>
+      </c>
+      <c r="Y27">
+        <v>9</v>
+      </c>
+      <c r="Z27">
+        <v>8</v>
+      </c>
+      <c r="AB27">
+        <v>2</v>
+      </c>
+      <c r="AC27">
+        <v>6</v>
+      </c>
+      <c r="AD27">
+        <v>7</v>
+      </c>
+      <c r="AE27">
+        <v>17</v>
+      </c>
+      <c r="AF27">
+        <v>11</v>
+      </c>
+      <c r="AG27">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>6</v>
+      </c>
+      <c r="H29">
+        <v>11</v>
+      </c>
+      <c r="I29">
+        <v>17</v>
+      </c>
+      <c r="J29">
+        <v>12</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>8</v>
+      </c>
+      <c r="O29">
+        <v>10</v>
+      </c>
+      <c r="P29">
+        <v>6</v>
+      </c>
+      <c r="Q29">
+        <v>7</v>
+      </c>
+      <c r="R29">
+        <v>7</v>
+      </c>
+      <c r="T29">
+        <v>7</v>
+      </c>
+      <c r="V29">
+        <v>10</v>
+      </c>
+      <c r="W29">
+        <v>11</v>
+      </c>
+      <c r="X29">
+        <v>16</v>
+      </c>
+      <c r="Y29">
+        <v>6</v>
+      </c>
+      <c r="AA29">
+        <v>10</v>
+      </c>
+      <c r="AB29">
+        <v>4</v>
+      </c>
+      <c r="AC29">
+        <v>14</v>
+      </c>
+      <c r="AD29">
+        <v>7</v>
+      </c>
+      <c r="AE29">
+        <v>10</v>
+      </c>
+      <c r="AF29">
+        <v>14</v>
+      </c>
+      <c r="AG29">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="J30">
+        <v>7</v>
+      </c>
+      <c r="L30">
+        <v>5</v>
+      </c>
+      <c r="M30">
+        <v>3</v>
+      </c>
+      <c r="O30">
+        <v>4</v>
+      </c>
+      <c r="P30">
+        <v>3</v>
+      </c>
+      <c r="Q30">
+        <v>5</v>
+      </c>
+      <c r="R30">
+        <v>5</v>
+      </c>
+      <c r="S30">
+        <v>3</v>
+      </c>
+      <c r="T30">
+        <v>2</v>
+      </c>
+      <c r="V30">
+        <v>6</v>
+      </c>
+      <c r="W30">
+        <v>4</v>
+      </c>
+      <c r="X30">
+        <v>6</v>
+      </c>
+      <c r="Y30">
+        <v>2</v>
+      </c>
+      <c r="Z30">
+        <v>6</v>
+      </c>
+      <c r="AC30">
+        <v>3</v>
+      </c>
+      <c r="AD30">
+        <v>3</v>
+      </c>
+      <c r="AE30">
+        <v>5</v>
+      </c>
+      <c r="AF30">
+        <v>5</v>
+      </c>
+      <c r="AG30">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>22</v>
+      </c>
+      <c r="D31">
+        <v>12</v>
+      </c>
+      <c r="E31">
+        <v>16</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="H31">
+        <v>20</v>
+      </c>
+      <c r="I31">
+        <v>25</v>
+      </c>
+      <c r="J31">
+        <v>46</v>
+      </c>
+      <c r="M31">
+        <v>9</v>
+      </c>
+      <c r="O31">
+        <v>16</v>
+      </c>
+      <c r="P31">
+        <v>6</v>
+      </c>
+      <c r="Q31">
+        <v>3</v>
+      </c>
+      <c r="R31">
+        <v>19</v>
+      </c>
+      <c r="S31">
+        <v>15</v>
+      </c>
+      <c r="T31">
+        <v>16</v>
+      </c>
+      <c r="V31">
+        <v>17</v>
+      </c>
+      <c r="W31">
+        <v>12</v>
+      </c>
+      <c r="X31">
+        <v>25</v>
+      </c>
+      <c r="Y31">
+        <v>21</v>
+      </c>
+      <c r="Z31">
+        <v>18</v>
+      </c>
+      <c r="AA31">
+        <v>9</v>
+      </c>
+      <c r="AB31">
+        <v>2</v>
+      </c>
+      <c r="AC31">
+        <v>16</v>
+      </c>
+      <c r="AD31">
+        <v>22</v>
+      </c>
+      <c r="AE31">
+        <v>21</v>
+      </c>
+      <c r="AF31">
+        <v>18</v>
+      </c>
+      <c r="AG31">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>5</v>
+      </c>
+      <c r="Q32">
+        <v>3</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>1</v>
+      </c>
+      <c r="X32">
+        <v>1</v>
+      </c>
+      <c r="Y32">
+        <v>2</v>
+      </c>
+      <c r="Z32">
+        <v>2</v>
+      </c>
+      <c r="AC32">
+        <v>3</v>
+      </c>
+      <c r="AE32">
+        <v>1</v>
+      </c>
+      <c r="AG32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>4</v>
+      </c>
+      <c r="J33">
+        <v>6</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>3</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <v>10</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+      <c r="R33">
+        <v>3</v>
+      </c>
+      <c r="S33">
+        <v>2</v>
+      </c>
+      <c r="T33">
+        <v>2</v>
+      </c>
+      <c r="V33">
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <v>2</v>
+      </c>
+      <c r="X33">
+        <v>4</v>
+      </c>
+      <c r="Y33">
+        <v>2</v>
+      </c>
+      <c r="Z33">
+        <v>4</v>
+      </c>
+      <c r="AA33">
+        <v>3</v>
+      </c>
+      <c r="AD33">
+        <v>9</v>
+      </c>
+      <c r="AE33">
+        <v>4</v>
+      </c>
+      <c r="AF33">
+        <v>4</v>
+      </c>
+      <c r="AG33">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34">
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>37</v>
+      </c>
+      <c r="D34">
+        <v>28</v>
+      </c>
+      <c r="E34">
+        <v>27</v>
+      </c>
+      <c r="F34">
+        <v>15</v>
+      </c>
+      <c r="H34">
+        <v>37</v>
+      </c>
+      <c r="I34">
+        <v>31</v>
+      </c>
+      <c r="J34">
+        <v>37</v>
+      </c>
+      <c r="L34">
+        <v>36</v>
+      </c>
+      <c r="M34">
+        <v>15</v>
+      </c>
+      <c r="O34">
+        <v>48</v>
+      </c>
+      <c r="P34">
+        <v>34</v>
+      </c>
+      <c r="Q34">
+        <v>41</v>
+      </c>
+      <c r="R34">
+        <v>35</v>
+      </c>
+      <c r="S34">
+        <v>14</v>
+      </c>
+      <c r="T34">
+        <v>16</v>
+      </c>
+      <c r="U34">
+        <v>1</v>
+      </c>
+      <c r="V34">
+        <v>19</v>
+      </c>
+      <c r="W34">
+        <v>30</v>
+      </c>
+      <c r="X34">
+        <v>25</v>
+      </c>
+      <c r="Y34">
+        <v>28</v>
+      </c>
+      <c r="Z34">
+        <v>32</v>
+      </c>
+      <c r="AA34">
+        <v>14</v>
+      </c>
+      <c r="AC34">
+        <v>47</v>
+      </c>
+      <c r="AD34">
+        <v>24</v>
+      </c>
+      <c r="AE34">
+        <v>31</v>
+      </c>
+      <c r="AF34">
+        <v>23</v>
+      </c>
+      <c r="AG34">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>24</v>
+      </c>
+      <c r="C35">
+        <v>20</v>
+      </c>
+      <c r="D35">
+        <v>17</v>
+      </c>
+      <c r="E35">
+        <v>15</v>
+      </c>
+      <c r="F35">
+        <v>8</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>23</v>
+      </c>
+      <c r="I35">
+        <v>22</v>
+      </c>
+      <c r="J35">
+        <v>20</v>
+      </c>
+      <c r="K35">
+        <v>4</v>
+      </c>
+      <c r="M35">
+        <v>11</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>52</v>
+      </c>
+      <c r="P35">
+        <v>23</v>
+      </c>
+      <c r="Q35">
+        <v>21</v>
+      </c>
+      <c r="R35">
+        <v>15</v>
+      </c>
+      <c r="S35">
+        <v>22</v>
+      </c>
+      <c r="T35">
+        <v>10</v>
+      </c>
+      <c r="U35">
+        <v>1</v>
+      </c>
+      <c r="V35">
+        <v>19</v>
+      </c>
+      <c r="W35">
+        <v>27</v>
+      </c>
+      <c r="X35">
+        <v>17</v>
+      </c>
+      <c r="Y35">
+        <v>22</v>
+      </c>
+      <c r="Z35">
+        <v>22</v>
+      </c>
+      <c r="AA35">
+        <v>7</v>
+      </c>
+      <c r="AB35">
+        <v>1</v>
+      </c>
+      <c r="AC35">
+        <v>35</v>
+      </c>
+      <c r="AD35">
+        <v>22</v>
+      </c>
+      <c r="AE35">
+        <v>19</v>
+      </c>
+      <c r="AF35">
+        <v>11</v>
+      </c>
+      <c r="AG35">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36">
+        <v>20</v>
+      </c>
+      <c r="C36">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>16</v>
+      </c>
+      <c r="E36">
+        <v>14</v>
+      </c>
+      <c r="F36">
+        <v>7</v>
+      </c>
+      <c r="H36">
+        <v>14</v>
+      </c>
+      <c r="I36">
+        <v>18</v>
+      </c>
+      <c r="J36">
+        <v>13</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>16</v>
+      </c>
+      <c r="M36">
+        <v>10</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>16</v>
+      </c>
+      <c r="P36">
+        <v>12</v>
+      </c>
+      <c r="Q36">
+        <v>8</v>
+      </c>
+      <c r="R36">
+        <v>19</v>
+      </c>
+      <c r="S36">
+        <v>14</v>
+      </c>
+      <c r="T36">
+        <v>8</v>
+      </c>
+      <c r="U36">
+        <v>1</v>
+      </c>
+      <c r="V36">
+        <v>13</v>
+      </c>
+      <c r="W36">
+        <v>13</v>
+      </c>
+      <c r="X36">
+        <v>15</v>
+      </c>
+      <c r="Y36">
+        <v>13</v>
+      </c>
+      <c r="Z36">
+        <v>13</v>
+      </c>
+      <c r="AA36">
+        <v>8</v>
+      </c>
+      <c r="AB36">
+        <v>2</v>
+      </c>
+      <c r="AC36">
+        <v>25</v>
+      </c>
+      <c r="AD36">
+        <v>12</v>
+      </c>
+      <c r="AE36">
+        <v>13</v>
+      </c>
+      <c r="AF36">
+        <v>17</v>
+      </c>
+      <c r="AG36">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <v>71</v>
+      </c>
+      <c r="C37">
+        <v>58</v>
+      </c>
+      <c r="D37">
+        <v>59</v>
+      </c>
+      <c r="E37">
+        <v>79</v>
+      </c>
+      <c r="F37">
+        <v>41</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>55</v>
+      </c>
+      <c r="I37">
+        <v>63</v>
+      </c>
+      <c r="J37">
+        <v>84</v>
+      </c>
+      <c r="K37">
+        <v>5</v>
+      </c>
+      <c r="L37">
+        <v>62</v>
+      </c>
+      <c r="M37">
+        <v>49</v>
+      </c>
+      <c r="N37">
+        <v>2</v>
+      </c>
+      <c r="O37">
+        <v>75</v>
+      </c>
+      <c r="P37">
+        <v>73</v>
+      </c>
+      <c r="Q37">
+        <v>63</v>
+      </c>
+      <c r="R37">
+        <v>64</v>
+      </c>
+      <c r="S37">
+        <v>49</v>
+      </c>
+      <c r="T37">
+        <v>26</v>
+      </c>
+      <c r="U37">
+        <v>2</v>
+      </c>
+      <c r="V37">
+        <v>62</v>
+      </c>
+      <c r="W37">
+        <v>76</v>
+      </c>
+      <c r="X37">
+        <v>59</v>
+      </c>
+      <c r="Y37">
+        <v>71</v>
+      </c>
+      <c r="Z37">
+        <v>98</v>
+      </c>
+      <c r="AA37">
+        <v>32</v>
+      </c>
+      <c r="AB37">
+        <v>3</v>
+      </c>
+      <c r="AC37">
+        <v>69</v>
+      </c>
+      <c r="AD37">
+        <v>49</v>
+      </c>
+      <c r="AE37">
+        <v>68</v>
+      </c>
+      <c r="AF37">
+        <v>63</v>
+      </c>
+      <c r="AG37">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>14</v>
+      </c>
+      <c r="E38">
+        <v>13</v>
+      </c>
+      <c r="F38">
+        <v>9</v>
+      </c>
+      <c r="H38">
+        <v>12</v>
+      </c>
+      <c r="I38">
+        <v>16</v>
+      </c>
+      <c r="J38">
+        <v>22</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+      <c r="L38">
+        <v>18</v>
+      </c>
+      <c r="M38">
+        <v>7</v>
+      </c>
+      <c r="O38">
+        <v>24</v>
+      </c>
+      <c r="P38">
+        <v>10</v>
+      </c>
+      <c r="Q38">
+        <v>19</v>
+      </c>
+      <c r="R38">
+        <v>13</v>
+      </c>
+      <c r="S38">
+        <v>22</v>
+      </c>
+      <c r="T38">
+        <v>8</v>
+      </c>
+      <c r="V38">
+        <v>11</v>
+      </c>
+      <c r="W38">
+        <v>16</v>
+      </c>
+      <c r="X38">
+        <v>15</v>
+      </c>
+      <c r="Y38">
+        <v>10</v>
+      </c>
+      <c r="Z38">
+        <v>9</v>
+      </c>
+      <c r="AA38">
+        <v>8</v>
+      </c>
+      <c r="AC38">
+        <v>14</v>
+      </c>
+      <c r="AD38">
+        <v>10</v>
+      </c>
+      <c r="AE38">
+        <v>17</v>
+      </c>
+      <c r="AF38">
+        <v>10</v>
+      </c>
+      <c r="AG38">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>37</v>
+      </c>
+      <c r="C39">
+        <v>28</v>
+      </c>
+      <c r="D39">
+        <v>47</v>
+      </c>
+      <c r="E39">
+        <v>28</v>
+      </c>
+      <c r="F39">
+        <v>22</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>37</v>
+      </c>
+      <c r="I39">
+        <v>38</v>
+      </c>
+      <c r="J39">
+        <v>48</v>
+      </c>
+      <c r="K39">
+        <v>3</v>
+      </c>
+      <c r="L39">
+        <v>39</v>
+      </c>
+      <c r="M39">
+        <v>31</v>
+      </c>
+      <c r="N39">
+        <v>2</v>
+      </c>
+      <c r="O39">
+        <v>42</v>
+      </c>
+      <c r="P39">
+        <v>50</v>
+      </c>
+      <c r="Q39">
+        <v>31</v>
+      </c>
+      <c r="R39">
+        <v>37</v>
+      </c>
+      <c r="S39">
+        <v>20</v>
+      </c>
+      <c r="T39">
+        <v>25</v>
+      </c>
+      <c r="U39">
+        <v>1</v>
+      </c>
+      <c r="V39">
+        <v>44</v>
+      </c>
+      <c r="W39">
+        <v>48</v>
+      </c>
+      <c r="X39">
+        <v>31</v>
+      </c>
+      <c r="Y39">
+        <v>40</v>
+      </c>
+      <c r="Z39">
+        <v>39</v>
+      </c>
+      <c r="AA39">
+        <v>23</v>
+      </c>
+      <c r="AB39">
+        <v>2</v>
+      </c>
+      <c r="AC39">
+        <v>38</v>
+      </c>
+      <c r="AD39">
+        <v>45</v>
+      </c>
+      <c r="AE39">
+        <v>25</v>
+      </c>
+      <c r="AF39">
+        <v>33</v>
+      </c>
+      <c r="AG39">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
+      <c r="M40">
+        <v>5</v>
+      </c>
+      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="R40">
+        <v>5</v>
+      </c>
+      <c r="W40">
+        <v>2</v>
+      </c>
+      <c r="X40">
+        <v>1</v>
+      </c>
+      <c r="Y40">
+        <v>3</v>
+      </c>
+      <c r="AA40">
+        <v>1</v>
+      </c>
+      <c r="AD40">
+        <v>3</v>
+      </c>
+      <c r="AF40">
+        <v>5</v>
+      </c>
+      <c r="AG40">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>6</v>
+      </c>
+      <c r="L41">
+        <v>7</v>
+      </c>
+      <c r="M41">
+        <v>2</v>
+      </c>
+      <c r="P41">
+        <v>8</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <v>3</v>
+      </c>
+      <c r="W41">
+        <v>4</v>
+      </c>
+      <c r="X41">
+        <v>4</v>
+      </c>
+      <c r="Y41">
+        <v>3</v>
+      </c>
+      <c r="Z41">
+        <v>5</v>
+      </c>
+      <c r="AA41">
+        <v>2</v>
+      </c>
+      <c r="AD41">
+        <v>3</v>
+      </c>
+      <c r="AE41">
+        <v>2</v>
+      </c>
+      <c r="AF41">
+        <v>4</v>
+      </c>
+      <c r="AG41">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42">
+        <v>13</v>
+      </c>
+      <c r="C42">
+        <v>19</v>
+      </c>
+      <c r="D42">
+        <v>13</v>
+      </c>
+      <c r="E42">
+        <v>15</v>
+      </c>
+      <c r="H42">
+        <v>21</v>
+      </c>
+      <c r="I42">
+        <v>7</v>
+      </c>
+      <c r="J42">
+        <v>9</v>
+      </c>
+      <c r="L42">
+        <v>12</v>
+      </c>
+      <c r="V42">
+        <v>13</v>
+      </c>
+      <c r="W42">
+        <v>4</v>
+      </c>
+      <c r="X42">
+        <v>14</v>
+      </c>
+      <c r="Y42">
+        <v>21</v>
+      </c>
+      <c r="Z42">
+        <v>11</v>
+      </c>
+      <c r="AD42">
+        <v>12</v>
+      </c>
+      <c r="AE42">
+        <v>15</v>
+      </c>
+      <c r="AF42">
+        <v>15</v>
+      </c>
+      <c r="AG42">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43">
+        <v>60</v>
+      </c>
+      <c r="C43">
+        <v>57</v>
+      </c>
+      <c r="D43">
+        <v>59</v>
+      </c>
+      <c r="E43">
+        <v>42</v>
+      </c>
+      <c r="H43">
+        <v>34</v>
+      </c>
+      <c r="I43">
+        <v>58</v>
+      </c>
+      <c r="J43">
+        <v>57</v>
+      </c>
+      <c r="L43">
+        <v>69</v>
+      </c>
+      <c r="V43">
+        <v>65</v>
+      </c>
+      <c r="W43">
+        <v>59</v>
+      </c>
+      <c r="X43">
+        <v>52</v>
+      </c>
+      <c r="Y43">
+        <v>67</v>
+      </c>
+      <c r="Z43">
+        <v>40</v>
+      </c>
+      <c r="AD43">
+        <v>67</v>
+      </c>
+      <c r="AE43">
+        <v>71</v>
+      </c>
+      <c r="AF43">
+        <v>86</v>
+      </c>
+      <c r="AG43">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>5</v>
+      </c>
+      <c r="V44">
+        <v>4</v>
+      </c>
+      <c r="W44">
+        <v>1</v>
+      </c>
+      <c r="Y44">
+        <v>3</v>
+      </c>
+      <c r="Z44">
+        <v>2</v>
+      </c>
+      <c r="AD44">
+        <v>2</v>
+      </c>
+      <c r="AE44">
+        <v>1</v>
+      </c>
+      <c r="AF44">
+        <v>3</v>
+      </c>
+      <c r="AG44">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45">
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="I45">
+        <v>6</v>
+      </c>
+      <c r="J45">
+        <v>5</v>
+      </c>
+      <c r="L45">
+        <v>8</v>
+      </c>
+      <c r="V45">
+        <v>10</v>
+      </c>
+      <c r="W45">
+        <v>9</v>
+      </c>
+      <c r="Y45">
+        <v>13</v>
+      </c>
+      <c r="Z45">
+        <v>3</v>
+      </c>
+      <c r="AD45">
+        <v>21</v>
+      </c>
+      <c r="AE45">
+        <v>5</v>
+      </c>
+      <c r="AG45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46">
+        <v>9</v>
+      </c>
+      <c r="C46">
+        <v>24</v>
+      </c>
+      <c r="D46">
+        <v>20</v>
+      </c>
+      <c r="E46">
+        <v>8</v>
+      </c>
+      <c r="I46">
+        <v>8</v>
+      </c>
+      <c r="J46">
+        <v>23</v>
+      </c>
+      <c r="L46">
+        <v>18</v>
+      </c>
+      <c r="V46">
+        <v>1</v>
+      </c>
+      <c r="W46">
+        <v>11</v>
+      </c>
+      <c r="X46">
+        <v>21</v>
+      </c>
+      <c r="Y46">
+        <v>22</v>
+      </c>
+      <c r="AD46">
+        <v>16</v>
+      </c>
+      <c r="AE46">
+        <v>24</v>
+      </c>
+      <c r="AF46">
+        <v>37</v>
+      </c>
+      <c r="AG46">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>9</v>
+      </c>
+      <c r="E47">
+        <v>7</v>
+      </c>
+      <c r="F47">
+        <v>7</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>8</v>
+      </c>
+      <c r="J47">
+        <v>12</v>
+      </c>
+      <c r="K47">
+        <v>5</v>
+      </c>
+      <c r="L47">
+        <v>6</v>
+      </c>
+      <c r="M47">
+        <v>5</v>
+      </c>
+      <c r="O47">
+        <v>8</v>
+      </c>
+      <c r="Q47">
+        <v>11</v>
+      </c>
+      <c r="R47">
+        <v>11</v>
+      </c>
+      <c r="S47">
+        <v>4</v>
+      </c>
+      <c r="T47">
+        <v>3</v>
+      </c>
+      <c r="V47">
+        <v>8</v>
+      </c>
+      <c r="W47">
+        <v>1</v>
+      </c>
+      <c r="X47">
+        <v>14</v>
+      </c>
+      <c r="Y47">
+        <v>8</v>
+      </c>
+      <c r="Z47">
+        <v>13</v>
+      </c>
+      <c r="AA47">
+        <v>3</v>
+      </c>
+      <c r="AC47">
+        <v>7</v>
+      </c>
+      <c r="AE47">
+        <v>8</v>
+      </c>
+      <c r="AF47">
+        <v>9</v>
+      </c>
+      <c r="AG47">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48">
+        <v>21</v>
+      </c>
+      <c r="C48">
+        <v>19</v>
+      </c>
+      <c r="D48">
+        <v>18</v>
+      </c>
+      <c r="E48">
+        <v>16</v>
+      </c>
+      <c r="F48">
+        <v>6</v>
+      </c>
+      <c r="H48">
+        <v>7</v>
+      </c>
+      <c r="I48">
+        <v>23</v>
+      </c>
+      <c r="J48">
+        <v>23</v>
+      </c>
+      <c r="L48">
+        <v>13</v>
+      </c>
+      <c r="M48">
+        <v>4</v>
+      </c>
+      <c r="O48">
+        <v>41</v>
+      </c>
+      <c r="P48">
+        <v>17</v>
+      </c>
+      <c r="Q48">
+        <v>24</v>
+      </c>
+      <c r="R48">
+        <v>15</v>
+      </c>
+      <c r="S48">
+        <v>16</v>
+      </c>
+      <c r="T48">
+        <v>7</v>
+      </c>
+      <c r="U48">
+        <v>3</v>
+      </c>
+      <c r="V48">
+        <v>18</v>
+      </c>
+      <c r="W48">
+        <v>21</v>
+      </c>
+      <c r="X48">
+        <v>20</v>
+      </c>
+      <c r="Y48">
+        <v>15</v>
+      </c>
+      <c r="Z48">
+        <v>20</v>
+      </c>
+      <c r="AA48">
+        <v>12</v>
+      </c>
+      <c r="AC48">
+        <v>16</v>
+      </c>
+      <c r="AD48">
+        <v>21</v>
+      </c>
+      <c r="AE48">
+        <v>17</v>
+      </c>
+      <c r="AF48">
+        <v>20</v>
+      </c>
+      <c r="AG48">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49">
+        <v>32</v>
+      </c>
+      <c r="C49">
+        <v>36</v>
+      </c>
+      <c r="D49">
+        <v>24</v>
+      </c>
+      <c r="E49">
+        <v>17</v>
+      </c>
+      <c r="F49">
+        <v>13</v>
+      </c>
+      <c r="H49">
+        <v>29</v>
+      </c>
+      <c r="I49">
+        <v>42</v>
+      </c>
+      <c r="J49">
+        <v>33</v>
+      </c>
+      <c r="K49">
+        <v>9</v>
+      </c>
+      <c r="L49">
+        <v>32</v>
+      </c>
+      <c r="M49">
+        <v>13</v>
+      </c>
+      <c r="N49">
+        <v>3</v>
+      </c>
+      <c r="O49">
+        <v>31</v>
+      </c>
+      <c r="P49">
+        <v>29</v>
+      </c>
+      <c r="Q49">
+        <v>28</v>
+      </c>
+      <c r="R49">
+        <v>35</v>
+      </c>
+      <c r="S49">
+        <v>26</v>
+      </c>
+      <c r="T49">
+        <v>18</v>
+      </c>
+      <c r="U49">
+        <v>2</v>
+      </c>
+      <c r="V49">
+        <v>42</v>
+      </c>
+      <c r="W49">
+        <v>30</v>
+      </c>
+      <c r="X49">
+        <v>29</v>
+      </c>
+      <c r="Y49">
+        <v>34</v>
+      </c>
+      <c r="Z49">
+        <v>32</v>
+      </c>
+      <c r="AA49">
+        <v>9</v>
+      </c>
+      <c r="AB49">
+        <v>2</v>
+      </c>
+      <c r="AC49">
+        <v>31</v>
+      </c>
+      <c r="AD49">
+        <v>25</v>
+      </c>
+      <c r="AE49">
+        <v>36</v>
+      </c>
+      <c r="AF49">
+        <v>33</v>
+      </c>
+      <c r="AG49">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50">
+        <v>19</v>
+      </c>
+      <c r="C50">
+        <v>21</v>
+      </c>
+      <c r="D50">
+        <v>40</v>
+      </c>
+      <c r="E50">
+        <v>18</v>
+      </c>
+      <c r="F50">
+        <v>12</v>
+      </c>
+      <c r="H50">
+        <v>22</v>
+      </c>
+      <c r="I50">
+        <v>26</v>
+      </c>
+      <c r="J50">
+        <v>38</v>
+      </c>
+      <c r="K50">
+        <v>2</v>
+      </c>
+      <c r="L50">
+        <v>21</v>
+      </c>
+      <c r="M50">
+        <v>11</v>
+      </c>
+      <c r="O50">
+        <v>35</v>
+      </c>
+      <c r="P50">
+        <v>26</v>
+      </c>
+      <c r="Q50">
+        <v>19</v>
+      </c>
+      <c r="R50">
+        <v>24</v>
+      </c>
+      <c r="S50">
+        <v>11</v>
+      </c>
+      <c r="T50">
+        <v>17</v>
+      </c>
+      <c r="U50">
+        <v>1</v>
+      </c>
+      <c r="V50">
+        <v>30</v>
+      </c>
+      <c r="W50">
+        <v>21</v>
+      </c>
+      <c r="X50">
+        <v>25</v>
+      </c>
+      <c r="Y50">
+        <v>22</v>
+      </c>
+      <c r="Z50">
+        <v>10</v>
+      </c>
+      <c r="AA50">
+        <v>4</v>
+      </c>
+      <c r="AC50">
+        <v>29</v>
+      </c>
+      <c r="AD50">
+        <v>25</v>
+      </c>
+      <c r="AE50">
+        <v>30</v>
+      </c>
+      <c r="AF50">
+        <v>23</v>
+      </c>
+      <c r="AG50">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51">
+        <v>23</v>
+      </c>
+      <c r="C51">
+        <v>33</v>
+      </c>
+      <c r="D51">
+        <v>23</v>
+      </c>
+      <c r="E51">
+        <v>20</v>
+      </c>
+      <c r="F51">
+        <v>5</v>
+      </c>
+      <c r="H51">
+        <v>22</v>
+      </c>
+      <c r="I51">
+        <v>21</v>
+      </c>
+      <c r="J51">
+        <v>18</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+      <c r="L51">
+        <v>21</v>
+      </c>
+      <c r="M51">
+        <v>2</v>
+      </c>
+      <c r="O51">
+        <v>31</v>
+      </c>
+      <c r="P51">
+        <v>25</v>
+      </c>
+      <c r="Q51">
+        <v>17</v>
+      </c>
+      <c r="R51">
+        <v>34</v>
+      </c>
+      <c r="S51">
+        <v>13</v>
+      </c>
+      <c r="T51">
+        <v>5</v>
+      </c>
+      <c r="V51">
+        <v>32</v>
+      </c>
+      <c r="W51">
+        <v>22</v>
+      </c>
+      <c r="X51">
+        <v>27</v>
+      </c>
+      <c r="Y51">
+        <v>29</v>
+      </c>
+      <c r="Z51">
+        <v>24</v>
+      </c>
+      <c r="AA51">
+        <v>4</v>
+      </c>
+      <c r="AC51">
+        <v>23</v>
+      </c>
+      <c r="AD51">
+        <v>24</v>
+      </c>
+      <c r="AE51">
+        <v>15</v>
+      </c>
+      <c r="AF51">
+        <v>16</v>
+      </c>
+      <c r="AG51">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52">
+        <v>46</v>
+      </c>
+      <c r="C52">
+        <v>42</v>
+      </c>
+      <c r="D52">
+        <v>33</v>
+      </c>
+      <c r="E52">
+        <v>37</v>
+      </c>
+      <c r="F52">
+        <v>20</v>
+      </c>
+      <c r="G52">
+        <v>6</v>
+      </c>
+      <c r="H52">
+        <v>33</v>
+      </c>
+      <c r="I52">
+        <v>48</v>
+      </c>
+      <c r="J52">
+        <v>63</v>
+      </c>
+      <c r="K52">
+        <v>5</v>
+      </c>
+      <c r="L52">
+        <v>36</v>
+      </c>
+      <c r="M52">
+        <v>15</v>
+      </c>
+      <c r="N52">
+        <v>21</v>
+      </c>
+      <c r="O52">
+        <v>52</v>
+      </c>
+      <c r="P52">
+        <v>36</v>
+      </c>
+      <c r="Q52">
+        <v>43</v>
+      </c>
+      <c r="R52">
+        <v>31</v>
+      </c>
+      <c r="S52">
+        <v>34</v>
+      </c>
+      <c r="T52">
+        <v>10</v>
+      </c>
+      <c r="U52">
+        <v>12</v>
+      </c>
+      <c r="V52">
+        <v>44</v>
+      </c>
+      <c r="W52">
+        <v>48</v>
+      </c>
+      <c r="X52">
+        <v>60</v>
+      </c>
+      <c r="Y52">
+        <v>37</v>
+      </c>
+      <c r="Z52">
+        <v>1</v>
+      </c>
+      <c r="AA52">
+        <v>33</v>
+      </c>
+      <c r="AB52">
+        <v>9</v>
+      </c>
+      <c r="AC52">
+        <v>47</v>
+      </c>
+      <c r="AD52">
+        <v>47</v>
+      </c>
+      <c r="AE52">
+        <v>38</v>
+      </c>
+      <c r="AF52">
+        <v>46</v>
+      </c>
+      <c r="AG52">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>8</v>
+      </c>
+      <c r="D53">
+        <v>4</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>10</v>
+      </c>
+      <c r="J53">
+        <v>10</v>
+      </c>
+      <c r="L53">
+        <v>4</v>
+      </c>
+      <c r="M53">
+        <v>5</v>
+      </c>
+      <c r="O53">
+        <v>9</v>
+      </c>
+      <c r="P53">
+        <v>8</v>
+      </c>
+      <c r="Q53">
+        <v>7</v>
+      </c>
+      <c r="R53">
+        <v>5</v>
+      </c>
+      <c r="S53">
+        <v>2</v>
+      </c>
+      <c r="T53">
+        <v>2</v>
+      </c>
+      <c r="V53">
+        <v>8</v>
+      </c>
+      <c r="W53">
+        <v>7</v>
+      </c>
+      <c r="X53">
+        <v>5</v>
+      </c>
+      <c r="Y53">
+        <v>9</v>
+      </c>
+      <c r="Z53">
+        <v>3</v>
+      </c>
+      <c r="AA53">
+        <v>4</v>
+      </c>
+      <c r="AC53">
+        <v>3</v>
+      </c>
+      <c r="AD53">
+        <v>4</v>
+      </c>
+      <c r="AE53">
+        <v>12</v>
+      </c>
+      <c r="AF53">
+        <v>6</v>
+      </c>
+      <c r="AG53">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54">
+        <v>16</v>
+      </c>
+      <c r="C54">
+        <v>19</v>
+      </c>
+      <c r="D54">
+        <v>12</v>
+      </c>
+      <c r="E54">
+        <v>12</v>
+      </c>
+      <c r="F54">
+        <v>9</v>
+      </c>
+      <c r="H54">
+        <v>16</v>
+      </c>
+      <c r="I54">
+        <v>18</v>
+      </c>
+      <c r="J54">
+        <v>33</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>14</v>
+      </c>
+      <c r="M54">
+        <v>4</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <v>15</v>
+      </c>
+      <c r="P54">
+        <v>18</v>
+      </c>
+      <c r="Q54">
+        <v>22</v>
+      </c>
+      <c r="R54">
+        <v>13</v>
+      </c>
+      <c r="S54">
+        <v>10</v>
+      </c>
+      <c r="T54">
+        <v>8</v>
+      </c>
+      <c r="U54">
+        <v>1</v>
+      </c>
+      <c r="V54">
+        <v>34</v>
+      </c>
+      <c r="W54">
+        <v>16</v>
+      </c>
+      <c r="X54">
+        <v>24</v>
+      </c>
+      <c r="Y54">
+        <v>7</v>
+      </c>
+      <c r="Z54">
+        <v>13</v>
+      </c>
+      <c r="AA54">
+        <v>8</v>
+      </c>
+      <c r="AC54">
+        <v>19</v>
+      </c>
+      <c r="AD54">
+        <v>19</v>
+      </c>
+      <c r="AE54">
+        <v>18</v>
+      </c>
+      <c r="AF54">
+        <v>17</v>
+      </c>
+      <c r="AG54">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55">
+        <v>5</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="H55">
+        <v>3</v>
+      </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>4</v>
+      </c>
+      <c r="M55">
+        <v>2</v>
+      </c>
+      <c r="O55">
+        <v>6</v>
+      </c>
+      <c r="P55">
+        <v>2</v>
+      </c>
+      <c r="Q55">
+        <v>4</v>
+      </c>
+      <c r="R55">
+        <v>1</v>
+      </c>
+      <c r="S55">
+        <v>5</v>
+      </c>
+      <c r="T55">
+        <v>3</v>
+      </c>
+      <c r="V55">
+        <v>4</v>
+      </c>
+      <c r="W55">
+        <v>2</v>
+      </c>
+      <c r="X55">
+        <v>4</v>
+      </c>
+      <c r="Y55">
+        <v>1</v>
+      </c>
+      <c r="Z55">
+        <v>8</v>
+      </c>
+      <c r="AC55">
+        <v>7</v>
+      </c>
+      <c r="AD55">
+        <v>1</v>
+      </c>
+      <c r="AE55">
+        <v>5</v>
+      </c>
+      <c r="AF55">
+        <v>4</v>
+      </c>
+      <c r="AG55">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <v>8</v>
+      </c>
+      <c r="D56">
+        <v>7</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <v>5</v>
+      </c>
+      <c r="I56">
+        <v>2</v>
+      </c>
+      <c r="J56">
+        <v>10</v>
+      </c>
+      <c r="K56">
+        <v>4</v>
+      </c>
+      <c r="M56">
+        <v>3</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
+      <c r="O56">
+        <v>5</v>
+      </c>
+      <c r="P56">
+        <v>4</v>
+      </c>
+      <c r="Q56">
+        <v>4</v>
+      </c>
+      <c r="R56">
+        <v>3</v>
+      </c>
+      <c r="T56">
+        <v>2</v>
+      </c>
+      <c r="V56">
+        <v>4</v>
+      </c>
+      <c r="W56">
+        <v>2</v>
+      </c>
+      <c r="X56">
+        <v>10</v>
+      </c>
+      <c r="Y56">
+        <v>1</v>
+      </c>
+      <c r="AA56">
+        <v>2</v>
+      </c>
+      <c r="AC56">
+        <v>3</v>
+      </c>
+      <c r="AD56">
+        <v>3</v>
+      </c>
+      <c r="AE56">
+        <v>8</v>
+      </c>
+      <c r="AF56">
+        <v>2</v>
+      </c>
+      <c r="AG56">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57">
+        <v>11</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57">
+        <v>11</v>
+      </c>
+      <c r="E57">
+        <v>5</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>7</v>
+      </c>
+      <c r="I57">
+        <v>6</v>
+      </c>
+      <c r="J57">
+        <v>6</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>8</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="O57">
+        <v>14</v>
+      </c>
+      <c r="P57">
+        <v>6</v>
+      </c>
+      <c r="Q57">
+        <v>5</v>
+      </c>
+      <c r="R57">
+        <v>7</v>
+      </c>
+      <c r="S57">
+        <v>8</v>
+      </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
+      <c r="V57">
+        <v>10</v>
+      </c>
+      <c r="W57">
+        <v>7</v>
+      </c>
+      <c r="X57">
+        <v>2</v>
+      </c>
+      <c r="Y57">
+        <v>5</v>
+      </c>
+      <c r="Z57">
+        <v>5</v>
+      </c>
+      <c r="AB57">
+        <v>2</v>
+      </c>
+      <c r="AC57">
+        <v>6</v>
+      </c>
+      <c r="AD57">
+        <v>2</v>
+      </c>
+      <c r="AE57">
+        <v>4</v>
+      </c>
+      <c r="AF57">
+        <v>4</v>
+      </c>
+      <c r="AG57">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:AG57" xr:uid="{34968F86-018E-44E2-A2A3-E904B7A2DFA5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Several april file updates
</commit_message>
<xml_diff>
--- a/statistics_files/2022/2022.d.monthly_circ_by_borrower.unique_borrowers.xlsx
+++ b/statistics_files/2022/2022.d.monthly_circ_by_borrower.unique_borrowers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B9A3B3-2BA5-4C8C-AED6-6E6B33046CFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0F917C-D0E0-4C7B-9F88-DD8C8D257BF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="894" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="894" activeTab="3" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="2" r:id="rId1"/>
@@ -27,6 +27,8 @@
     <sheet name="December" sheetId="13" r:id="rId12"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">April!$A$3:$AG$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">February!$A$3:$AG$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">January!$A$3:$AG$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">March!$A$3:$AG$57</definedName>
   </definedNames>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="71">
   <si>
     <t>branchname</t>
   </si>
@@ -250,6 +252,9 @@
   </si>
   <si>
     <t>2022-03-01 - 2022-03-30</t>
+  </si>
+  <si>
+    <t>2022-04-01 - 2022-04-30</t>
   </si>
 </sst>
 </file>
@@ -619,7 +624,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -9369,6 +9374,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:AG3" xr:uid="{D8399D67-E68B-42D7-AFC3-15C82B91E2D5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13948,9 +13954,9 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633557D5-54F2-4CB6-8A69-0FAA84994F48}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="B2:AF2"/>
+  <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -13963,40 +13969,4526 @@
     <col min="2" max="33" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44652</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44653</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44654</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44655</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44656</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44657</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44658</v>
+      </c>
+      <c r="I2" s="1">
+        <v>44659</v>
+      </c>
+      <c r="J2" s="1">
+        <v>44660</v>
+      </c>
+      <c r="K2" s="1">
+        <v>44661</v>
+      </c>
+      <c r="L2" s="1">
+        <v>44662</v>
+      </c>
+      <c r="M2" s="1">
+        <v>44663</v>
+      </c>
+      <c r="N2" s="1">
+        <v>44664</v>
+      </c>
+      <c r="O2" s="1">
+        <v>44665</v>
+      </c>
+      <c r="P2" s="1">
+        <v>44666</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>44667</v>
+      </c>
+      <c r="R2" s="1">
+        <v>44668</v>
+      </c>
+      <c r="S2" s="1">
+        <v>44669</v>
+      </c>
+      <c r="T2" s="1">
+        <v>44670</v>
+      </c>
+      <c r="U2" s="1">
+        <v>44671</v>
+      </c>
+      <c r="V2" s="1">
+        <v>44672</v>
+      </c>
+      <c r="W2" s="1">
+        <v>44673</v>
+      </c>
+      <c r="X2" s="1">
+        <v>44674</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>44675</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>44676</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>44677</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>44678</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>44679</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>44680</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>44681</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" t="s">
+        <v>8</v>
+      </c>
+      <c r="U3" t="s">
+        <v>9</v>
+      </c>
+      <c r="V3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" t="s">
+        <v>11</v>
+      </c>
+      <c r="X3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>38</v>
+      </c>
+      <c r="C4">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>70</v>
+      </c>
+      <c r="F4">
+        <v>52</v>
+      </c>
+      <c r="G4">
+        <v>53</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>54</v>
+      </c>
+      <c r="J4">
+        <v>27</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>69</v>
+      </c>
+      <c r="M4">
+        <v>67</v>
+      </c>
+      <c r="N4">
+        <v>55</v>
+      </c>
+      <c r="O4">
+        <v>88</v>
+      </c>
+      <c r="P4">
+        <v>41</v>
+      </c>
+      <c r="Q4">
+        <v>22</v>
+      </c>
+      <c r="S4">
+        <v>59</v>
+      </c>
+      <c r="T4">
+        <v>66</v>
+      </c>
+      <c r="U4">
+        <v>53</v>
+      </c>
+      <c r="V4">
+        <v>71</v>
+      </c>
+      <c r="W4">
+        <v>56</v>
+      </c>
+      <c r="X4">
+        <v>33</v>
+      </c>
+      <c r="Y4">
+        <v>4</v>
+      </c>
+      <c r="Z4">
+        <v>51</v>
+      </c>
+      <c r="AA4">
+        <v>66</v>
+      </c>
+      <c r="AB4">
+        <v>53</v>
+      </c>
+      <c r="AC4">
+        <v>60</v>
+      </c>
+      <c r="AD4">
+        <v>56</v>
+      </c>
+      <c r="AE4">
+        <v>38</v>
+      </c>
+      <c r="AG4">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>38</v>
+      </c>
+      <c r="C5">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>29</v>
+      </c>
+      <c r="F5">
+        <v>44</v>
+      </c>
+      <c r="G5">
+        <v>50</v>
+      </c>
+      <c r="H5">
+        <v>33</v>
+      </c>
+      <c r="I5">
+        <v>22</v>
+      </c>
+      <c r="J5">
+        <v>13</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>26</v>
+      </c>
+      <c r="M5">
+        <v>41</v>
+      </c>
+      <c r="N5">
+        <v>30</v>
+      </c>
+      <c r="O5">
+        <v>31</v>
+      </c>
+      <c r="P5">
+        <v>40</v>
+      </c>
+      <c r="Q5">
+        <v>20</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>41</v>
+      </c>
+      <c r="T5">
+        <v>40</v>
+      </c>
+      <c r="U5">
+        <v>29</v>
+      </c>
+      <c r="V5">
+        <v>26</v>
+      </c>
+      <c r="W5">
+        <v>23</v>
+      </c>
+      <c r="X5">
+        <v>12</v>
+      </c>
+      <c r="Y5">
+        <v>3</v>
+      </c>
+      <c r="Z5">
+        <v>41</v>
+      </c>
+      <c r="AA5">
+        <v>32</v>
+      </c>
+      <c r="AB5">
+        <v>35</v>
+      </c>
+      <c r="AC5">
+        <v>28</v>
+      </c>
+      <c r="AD5">
+        <v>27</v>
+      </c>
+      <c r="AE5">
+        <v>17</v>
+      </c>
+      <c r="AG5">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>66</v>
+      </c>
+      <c r="C6">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <v>43</v>
+      </c>
+      <c r="E6">
+        <v>78</v>
+      </c>
+      <c r="F6">
+        <v>71</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>57</v>
+      </c>
+      <c r="I6">
+        <v>52</v>
+      </c>
+      <c r="J6">
+        <v>60</v>
+      </c>
+      <c r="K6">
+        <v>30</v>
+      </c>
+      <c r="L6">
+        <v>74</v>
+      </c>
+      <c r="M6">
+        <v>77</v>
+      </c>
+      <c r="N6">
+        <v>85</v>
+      </c>
+      <c r="O6">
+        <v>79</v>
+      </c>
+      <c r="P6">
+        <v>51</v>
+      </c>
+      <c r="Q6">
+        <v>63</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>91</v>
+      </c>
+      <c r="T6">
+        <v>90</v>
+      </c>
+      <c r="U6">
+        <v>84</v>
+      </c>
+      <c r="V6">
+        <v>70</v>
+      </c>
+      <c r="W6">
+        <v>62</v>
+      </c>
+      <c r="X6">
+        <v>55</v>
+      </c>
+      <c r="Y6">
+        <v>29</v>
+      </c>
+      <c r="Z6">
+        <v>77</v>
+      </c>
+      <c r="AA6">
+        <v>91</v>
+      </c>
+      <c r="AB6">
+        <v>76</v>
+      </c>
+      <c r="AC6">
+        <v>68</v>
+      </c>
+      <c r="AD6">
+        <v>57</v>
+      </c>
+      <c r="AE6">
+        <v>48</v>
+      </c>
+      <c r="AG6">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7">
+        <v>3</v>
+      </c>
+      <c r="W7">
+        <v>4</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>2</v>
+      </c>
+      <c r="AB7">
+        <v>2</v>
+      </c>
+      <c r="AC7">
+        <v>4</v>
+      </c>
+      <c r="AD7">
+        <v>2</v>
+      </c>
+      <c r="AE7">
+        <v>4</v>
+      </c>
+      <c r="AG7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>47</v>
+      </c>
+      <c r="C8">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>64</v>
+      </c>
+      <c r="F8">
+        <v>47</v>
+      </c>
+      <c r="G8">
+        <v>42</v>
+      </c>
+      <c r="H8">
+        <v>48</v>
+      </c>
+      <c r="I8">
+        <v>47</v>
+      </c>
+      <c r="J8">
+        <v>43</v>
+      </c>
+      <c r="K8">
+        <v>11</v>
+      </c>
+      <c r="L8">
+        <v>61</v>
+      </c>
+      <c r="M8">
+        <v>50</v>
+      </c>
+      <c r="N8">
+        <v>38</v>
+      </c>
+      <c r="O8">
+        <v>46</v>
+      </c>
+      <c r="P8">
+        <v>43</v>
+      </c>
+      <c r="Q8">
+        <v>41</v>
+      </c>
+      <c r="R8">
+        <v>5</v>
+      </c>
+      <c r="S8">
+        <v>61</v>
+      </c>
+      <c r="T8">
+        <v>64</v>
+      </c>
+      <c r="U8">
+        <v>45</v>
+      </c>
+      <c r="V8">
+        <v>46</v>
+      </c>
+      <c r="W8">
+        <v>43</v>
+      </c>
+      <c r="X8">
+        <v>32</v>
+      </c>
+      <c r="Y8">
+        <v>23</v>
+      </c>
+      <c r="Z8">
+        <v>41</v>
+      </c>
+      <c r="AA8">
+        <v>52</v>
+      </c>
+      <c r="AB8">
+        <v>54</v>
+      </c>
+      <c r="AC8">
+        <v>61</v>
+      </c>
+      <c r="AD8">
+        <v>43</v>
+      </c>
+      <c r="AE8">
+        <v>40</v>
+      </c>
+      <c r="AG8">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>14</v>
+      </c>
+      <c r="H9">
+        <v>12</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>9</v>
+      </c>
+      <c r="N9">
+        <v>10</v>
+      </c>
+      <c r="O9">
+        <v>8</v>
+      </c>
+      <c r="P9">
+        <v>6</v>
+      </c>
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <v>9</v>
+      </c>
+      <c r="T9">
+        <v>13</v>
+      </c>
+      <c r="U9">
+        <v>6</v>
+      </c>
+      <c r="V9">
+        <v>4</v>
+      </c>
+      <c r="W9">
+        <v>12</v>
+      </c>
+      <c r="X9">
+        <v>2</v>
+      </c>
+      <c r="Z9">
+        <v>3</v>
+      </c>
+      <c r="AA9">
+        <v>6</v>
+      </c>
+      <c r="AB9">
+        <v>12</v>
+      </c>
+      <c r="AC9">
+        <v>11</v>
+      </c>
+      <c r="AD9">
+        <v>7</v>
+      </c>
+      <c r="AE9">
+        <v>8</v>
+      </c>
+      <c r="AG9">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>13</v>
+      </c>
+      <c r="H10">
+        <v>12</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>10</v>
+      </c>
+      <c r="M10">
+        <v>11</v>
+      </c>
+      <c r="N10">
+        <v>11</v>
+      </c>
+      <c r="O10">
+        <v>9</v>
+      </c>
+      <c r="P10">
+        <v>10</v>
+      </c>
+      <c r="Q10">
+        <v>10</v>
+      </c>
+      <c r="S10">
+        <v>13</v>
+      </c>
+      <c r="T10">
+        <v>10</v>
+      </c>
+      <c r="U10">
+        <v>17</v>
+      </c>
+      <c r="V10">
+        <v>5</v>
+      </c>
+      <c r="W10">
+        <v>11</v>
+      </c>
+      <c r="X10">
+        <v>6</v>
+      </c>
+      <c r="Z10">
+        <v>11</v>
+      </c>
+      <c r="AA10">
+        <v>8</v>
+      </c>
+      <c r="AB10">
+        <v>6</v>
+      </c>
+      <c r="AC10">
+        <v>10</v>
+      </c>
+      <c r="AD10">
+        <v>12</v>
+      </c>
+      <c r="AE10">
+        <v>6</v>
+      </c>
+      <c r="AG10">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <v>7</v>
+      </c>
+      <c r="O11">
+        <v>3</v>
+      </c>
+      <c r="P11">
+        <v>2</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>9</v>
+      </c>
+      <c r="U11">
+        <v>7</v>
+      </c>
+      <c r="V11">
+        <v>2</v>
+      </c>
+      <c r="W11">
+        <v>5</v>
+      </c>
+      <c r="Z11">
+        <v>9</v>
+      </c>
+      <c r="AB11">
+        <v>3</v>
+      </c>
+      <c r="AC11">
+        <v>2</v>
+      </c>
+      <c r="AD11">
+        <v>3</v>
+      </c>
+      <c r="AE11">
+        <v>2</v>
+      </c>
+      <c r="AG11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="AB12">
+        <v>1</v>
+      </c>
+      <c r="AE12">
+        <v>1</v>
+      </c>
+      <c r="AG12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>3</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>3</v>
+      </c>
+      <c r="V14">
+        <v>4</v>
+      </c>
+      <c r="W14">
+        <v>2</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+      <c r="AB14">
+        <v>2</v>
+      </c>
+      <c r="AC14">
+        <v>3</v>
+      </c>
+      <c r="AD14">
+        <v>2</v>
+      </c>
+      <c r="AG14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>8</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <v>8</v>
+      </c>
+      <c r="M15">
+        <v>10</v>
+      </c>
+      <c r="N15">
+        <v>8</v>
+      </c>
+      <c r="O15">
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <v>7</v>
+      </c>
+      <c r="S15">
+        <v>11</v>
+      </c>
+      <c r="T15">
+        <v>4</v>
+      </c>
+      <c r="U15">
+        <v>10</v>
+      </c>
+      <c r="V15">
+        <v>6</v>
+      </c>
+      <c r="W15">
+        <v>5</v>
+      </c>
+      <c r="Z15">
+        <v>7</v>
+      </c>
+      <c r="AA15">
+        <v>4</v>
+      </c>
+      <c r="AB15">
+        <v>5</v>
+      </c>
+      <c r="AC15">
+        <v>4</v>
+      </c>
+      <c r="AD15">
+        <v>5</v>
+      </c>
+      <c r="AG15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>17</v>
+      </c>
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
+      </c>
+      <c r="I16">
+        <v>17</v>
+      </c>
+      <c r="J16">
+        <v>5</v>
+      </c>
+      <c r="L16">
+        <v>13</v>
+      </c>
+      <c r="M16">
+        <v>8</v>
+      </c>
+      <c r="N16">
+        <v>12</v>
+      </c>
+      <c r="O16">
+        <v>10</v>
+      </c>
+      <c r="P16">
+        <v>14</v>
+      </c>
+      <c r="Q16">
+        <v>2</v>
+      </c>
+      <c r="S16">
+        <v>17</v>
+      </c>
+      <c r="T16">
+        <v>7</v>
+      </c>
+      <c r="U16">
+        <v>14</v>
+      </c>
+      <c r="V16">
+        <v>17</v>
+      </c>
+      <c r="W16">
+        <v>13</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>13</v>
+      </c>
+      <c r="AA16">
+        <v>12</v>
+      </c>
+      <c r="AB16">
+        <v>8</v>
+      </c>
+      <c r="AC16">
+        <v>15</v>
+      </c>
+      <c r="AD16">
+        <v>11</v>
+      </c>
+      <c r="AE16">
+        <v>4</v>
+      </c>
+      <c r="AG16">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>11</v>
+      </c>
+      <c r="M17">
+        <v>11</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="O17">
+        <v>8</v>
+      </c>
+      <c r="P17">
+        <v>8</v>
+      </c>
+      <c r="Q17">
+        <v>3</v>
+      </c>
+      <c r="S17">
+        <v>8</v>
+      </c>
+      <c r="T17">
+        <v>11</v>
+      </c>
+      <c r="U17">
+        <v>2</v>
+      </c>
+      <c r="V17">
+        <v>6</v>
+      </c>
+      <c r="W17">
+        <v>7</v>
+      </c>
+      <c r="X17">
+        <v>3</v>
+      </c>
+      <c r="Z17">
+        <v>6</v>
+      </c>
+      <c r="AA17">
+        <v>7</v>
+      </c>
+      <c r="AB17">
+        <v>4</v>
+      </c>
+      <c r="AC17">
+        <v>6</v>
+      </c>
+      <c r="AD17">
+        <v>8</v>
+      </c>
+      <c r="AE17">
+        <v>2</v>
+      </c>
+      <c r="AG17">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="O18">
+        <v>3</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="S18">
+        <v>2</v>
+      </c>
+      <c r="T18">
+        <v>4</v>
+      </c>
+      <c r="U18">
+        <v>5</v>
+      </c>
+      <c r="V18">
+        <v>2</v>
+      </c>
+      <c r="W18">
+        <v>3</v>
+      </c>
+      <c r="X18">
+        <v>3</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>8</v>
+      </c>
+      <c r="AA18">
+        <v>1</v>
+      </c>
+      <c r="AB18">
+        <v>7</v>
+      </c>
+      <c r="AD18">
+        <v>1</v>
+      </c>
+      <c r="AE18">
+        <v>1</v>
+      </c>
+      <c r="AG18">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <v>28</v>
+      </c>
+      <c r="F19">
+        <v>11</v>
+      </c>
+      <c r="G19">
+        <v>26</v>
+      </c>
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <v>18</v>
+      </c>
+      <c r="J19">
+        <v>16</v>
+      </c>
+      <c r="L19">
+        <v>36</v>
+      </c>
+      <c r="M19">
+        <v>16</v>
+      </c>
+      <c r="N19">
+        <v>28</v>
+      </c>
+      <c r="O19">
+        <v>25</v>
+      </c>
+      <c r="P19">
+        <v>15</v>
+      </c>
+      <c r="Q19">
+        <v>11</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>33</v>
+      </c>
+      <c r="T19">
+        <v>18</v>
+      </c>
+      <c r="U19">
+        <v>26</v>
+      </c>
+      <c r="V19">
+        <v>18</v>
+      </c>
+      <c r="W19">
+        <v>17</v>
+      </c>
+      <c r="X19">
+        <v>17</v>
+      </c>
+      <c r="Y19">
+        <v>3</v>
+      </c>
+      <c r="Z19">
+        <v>36</v>
+      </c>
+      <c r="AA19">
+        <v>18</v>
+      </c>
+      <c r="AB19">
+        <v>34</v>
+      </c>
+      <c r="AC19">
+        <v>11</v>
+      </c>
+      <c r="AD19">
+        <v>25</v>
+      </c>
+      <c r="AE19">
+        <v>18</v>
+      </c>
+      <c r="AG19">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>2</v>
+      </c>
+      <c r="S20">
+        <v>3</v>
+      </c>
+      <c r="U20">
+        <v>2</v>
+      </c>
+      <c r="V20">
+        <v>4</v>
+      </c>
+      <c r="W20">
+        <v>2</v>
+      </c>
+      <c r="X20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>1</v>
+      </c>
+      <c r="AA20">
+        <v>2</v>
+      </c>
+      <c r="AB20">
+        <v>3</v>
+      </c>
+      <c r="AC20">
+        <v>2</v>
+      </c>
+      <c r="AD20">
+        <v>3</v>
+      </c>
+      <c r="AG20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>13</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>49</v>
+      </c>
+      <c r="F21">
+        <v>27</v>
+      </c>
+      <c r="G21">
+        <v>21</v>
+      </c>
+      <c r="H21">
+        <v>36</v>
+      </c>
+      <c r="I21">
+        <v>22</v>
+      </c>
+      <c r="J21">
+        <v>13</v>
+      </c>
+      <c r="K21">
+        <v>9</v>
+      </c>
+      <c r="L21">
+        <v>32</v>
+      </c>
+      <c r="M21">
+        <v>29</v>
+      </c>
+      <c r="N21">
+        <v>21</v>
+      </c>
+      <c r="O21">
+        <v>36</v>
+      </c>
+      <c r="P21">
+        <v>28</v>
+      </c>
+      <c r="Q21">
+        <v>13</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>44</v>
+      </c>
+      <c r="T21">
+        <v>13</v>
+      </c>
+      <c r="U21">
+        <v>20</v>
+      </c>
+      <c r="V21">
+        <v>33</v>
+      </c>
+      <c r="W21">
+        <v>24</v>
+      </c>
+      <c r="X21">
+        <v>14</v>
+      </c>
+      <c r="Y21">
+        <v>4</v>
+      </c>
+      <c r="Z21">
+        <v>25</v>
+      </c>
+      <c r="AA21">
+        <v>22</v>
+      </c>
+      <c r="AB21">
+        <v>16</v>
+      </c>
+      <c r="AC21">
+        <v>36</v>
+      </c>
+      <c r="AD21">
+        <v>29</v>
+      </c>
+      <c r="AE21">
+        <v>18</v>
+      </c>
+      <c r="AG21">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>2</v>
+      </c>
+      <c r="U22">
+        <v>2</v>
+      </c>
+      <c r="V22">
+        <v>2</v>
+      </c>
+      <c r="W22">
+        <v>2</v>
+      </c>
+      <c r="Z22">
+        <v>1</v>
+      </c>
+      <c r="AA22">
+        <v>2</v>
+      </c>
+      <c r="AC22">
+        <v>2</v>
+      </c>
+      <c r="AD22">
+        <v>1</v>
+      </c>
+      <c r="AG22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>28</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+      <c r="E23">
+        <v>38</v>
+      </c>
+      <c r="F23">
+        <v>39</v>
+      </c>
+      <c r="G23">
+        <v>42</v>
+      </c>
+      <c r="H23">
+        <v>26</v>
+      </c>
+      <c r="I23">
+        <v>22</v>
+      </c>
+      <c r="J23">
+        <v>14</v>
+      </c>
+      <c r="K23">
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <v>45</v>
+      </c>
+      <c r="M23">
+        <v>36</v>
+      </c>
+      <c r="N23">
+        <v>39</v>
+      </c>
+      <c r="O23">
+        <v>29</v>
+      </c>
+      <c r="P23">
+        <v>22</v>
+      </c>
+      <c r="Q23">
+        <v>16</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>53</v>
+      </c>
+      <c r="T23">
+        <v>36</v>
+      </c>
+      <c r="U23">
+        <v>29</v>
+      </c>
+      <c r="V23">
+        <v>31</v>
+      </c>
+      <c r="W23">
+        <v>31</v>
+      </c>
+      <c r="X23">
+        <v>16</v>
+      </c>
+      <c r="Z23">
+        <v>34</v>
+      </c>
+      <c r="AA23">
+        <v>26</v>
+      </c>
+      <c r="AB23">
+        <v>38</v>
+      </c>
+      <c r="AC23">
+        <v>33</v>
+      </c>
+      <c r="AD23">
+        <v>19</v>
+      </c>
+      <c r="AE23">
+        <v>17</v>
+      </c>
+      <c r="AG23">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
+      </c>
+      <c r="M24">
+        <v>4</v>
+      </c>
+      <c r="N24">
+        <v>2</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>3</v>
+      </c>
+      <c r="T24">
+        <v>3</v>
+      </c>
+      <c r="U24">
+        <v>4</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <v>5</v>
+      </c>
+      <c r="Z24">
+        <v>4</v>
+      </c>
+      <c r="AB24">
+        <v>4</v>
+      </c>
+      <c r="AC24">
+        <v>1</v>
+      </c>
+      <c r="AD24">
+        <v>1</v>
+      </c>
+      <c r="AG24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>18</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>32</v>
+      </c>
+      <c r="F25">
+        <v>16</v>
+      </c>
+      <c r="G25">
+        <v>36</v>
+      </c>
+      <c r="H25">
+        <v>23</v>
+      </c>
+      <c r="I25">
+        <v>39</v>
+      </c>
+      <c r="J25">
+        <v>12</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <v>35</v>
+      </c>
+      <c r="M25">
+        <v>27</v>
+      </c>
+      <c r="N25">
+        <v>17</v>
+      </c>
+      <c r="O25">
+        <v>42</v>
+      </c>
+      <c r="P25">
+        <v>35</v>
+      </c>
+      <c r="Q25">
+        <v>14</v>
+      </c>
+      <c r="S25">
+        <v>39</v>
+      </c>
+      <c r="T25">
+        <v>25</v>
+      </c>
+      <c r="U25">
+        <v>13</v>
+      </c>
+      <c r="V25">
+        <v>21</v>
+      </c>
+      <c r="W25">
+        <v>30</v>
+      </c>
+      <c r="X25">
+        <v>1</v>
+      </c>
+      <c r="Y25">
+        <v>2</v>
+      </c>
+      <c r="Z25">
+        <v>25</v>
+      </c>
+      <c r="AA25">
+        <v>24</v>
+      </c>
+      <c r="AB25">
+        <v>29</v>
+      </c>
+      <c r="AC25">
+        <v>24</v>
+      </c>
+      <c r="AD25">
+        <v>20</v>
+      </c>
+      <c r="AE25">
+        <v>13</v>
+      </c>
+      <c r="AG25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>59</v>
+      </c>
+      <c r="C26">
+        <v>54</v>
+      </c>
+      <c r="D26">
+        <v>42</v>
+      </c>
+      <c r="E26">
+        <v>87</v>
+      </c>
+      <c r="F26">
+        <v>104</v>
+      </c>
+      <c r="G26">
+        <v>99</v>
+      </c>
+      <c r="H26">
+        <v>102</v>
+      </c>
+      <c r="I26">
+        <v>78</v>
+      </c>
+      <c r="J26">
+        <v>63</v>
+      </c>
+      <c r="K26">
+        <v>36</v>
+      </c>
+      <c r="L26">
+        <v>96</v>
+      </c>
+      <c r="M26">
+        <v>83</v>
+      </c>
+      <c r="N26">
+        <v>70</v>
+      </c>
+      <c r="O26">
+        <v>90</v>
+      </c>
+      <c r="P26">
+        <v>85</v>
+      </c>
+      <c r="Q26">
+        <v>65</v>
+      </c>
+      <c r="R26">
+        <v>8</v>
+      </c>
+      <c r="S26">
+        <v>93</v>
+      </c>
+      <c r="T26">
+        <v>98</v>
+      </c>
+      <c r="U26">
+        <v>103</v>
+      </c>
+      <c r="V26">
+        <v>79</v>
+      </c>
+      <c r="W26">
+        <v>59</v>
+      </c>
+      <c r="X26">
+        <v>56</v>
+      </c>
+      <c r="Y26">
+        <v>38</v>
+      </c>
+      <c r="Z26">
+        <v>89</v>
+      </c>
+      <c r="AA26">
+        <v>83</v>
+      </c>
+      <c r="AB26">
+        <v>102</v>
+      </c>
+      <c r="AC26">
+        <v>86</v>
+      </c>
+      <c r="AD26">
+        <v>81</v>
+      </c>
+      <c r="AE26">
+        <v>64</v>
+      </c>
+      <c r="AG26">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>12</v>
+      </c>
+      <c r="F27">
+        <v>8</v>
+      </c>
+      <c r="G27">
+        <v>8</v>
+      </c>
+      <c r="H27">
+        <v>9</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <v>7</v>
+      </c>
+      <c r="M27">
+        <v>8</v>
+      </c>
+      <c r="N27">
+        <v>5</v>
+      </c>
+      <c r="O27">
+        <v>16</v>
+      </c>
+      <c r="P27">
+        <v>5</v>
+      </c>
+      <c r="Q27">
+        <v>6</v>
+      </c>
+      <c r="S27">
+        <v>9</v>
+      </c>
+      <c r="T27">
+        <v>6</v>
+      </c>
+      <c r="U27">
+        <v>7</v>
+      </c>
+      <c r="V27">
+        <v>11</v>
+      </c>
+      <c r="W27">
+        <v>11</v>
+      </c>
+      <c r="X27">
+        <v>7</v>
+      </c>
+      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="Z27">
+        <v>7</v>
+      </c>
+      <c r="AA27">
+        <v>11</v>
+      </c>
+      <c r="AB27">
+        <v>11</v>
+      </c>
+      <c r="AC27">
+        <v>7</v>
+      </c>
+      <c r="AD27">
+        <v>5</v>
+      </c>
+      <c r="AE27">
+        <v>2</v>
+      </c>
+      <c r="AG27">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>13</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>14</v>
+      </c>
+      <c r="H29">
+        <v>9</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>6</v>
+      </c>
+      <c r="L29">
+        <v>15</v>
+      </c>
+      <c r="M29">
+        <v>12</v>
+      </c>
+      <c r="N29">
+        <v>10</v>
+      </c>
+      <c r="O29">
+        <v>9</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>4</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>26</v>
+      </c>
+      <c r="T29">
+        <v>7</v>
+      </c>
+      <c r="U29">
+        <v>11</v>
+      </c>
+      <c r="V29">
+        <v>7</v>
+      </c>
+      <c r="W29">
+        <v>3</v>
+      </c>
+      <c r="X29">
+        <v>4</v>
+      </c>
+      <c r="Z29">
+        <v>15</v>
+      </c>
+      <c r="AA29">
+        <v>5</v>
+      </c>
+      <c r="AB29">
+        <v>9</v>
+      </c>
+      <c r="AC29">
+        <v>8</v>
+      </c>
+      <c r="AE29">
+        <v>8</v>
+      </c>
+      <c r="AG29">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>6</v>
+      </c>
+      <c r="H30">
+        <v>3</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>3</v>
+      </c>
+      <c r="L30">
+        <v>7</v>
+      </c>
+      <c r="M30">
+        <v>5</v>
+      </c>
+      <c r="N30">
+        <v>4</v>
+      </c>
+      <c r="O30">
+        <v>6</v>
+      </c>
+      <c r="P30">
+        <v>4</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="T30">
+        <v>2</v>
+      </c>
+      <c r="U30">
+        <v>6</v>
+      </c>
+      <c r="V30">
+        <v>2</v>
+      </c>
+      <c r="W30">
+        <v>5</v>
+      </c>
+      <c r="X30">
+        <v>3</v>
+      </c>
+      <c r="Z30">
+        <v>3</v>
+      </c>
+      <c r="AA30">
+        <v>6</v>
+      </c>
+      <c r="AB30">
+        <v>5</v>
+      </c>
+      <c r="AC30">
+        <v>2</v>
+      </c>
+      <c r="AD30">
+        <v>2</v>
+      </c>
+      <c r="AG30">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>13</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>17</v>
+      </c>
+      <c r="F31">
+        <v>11</v>
+      </c>
+      <c r="G31">
+        <v>35</v>
+      </c>
+      <c r="H31">
+        <v>20</v>
+      </c>
+      <c r="I31">
+        <v>17</v>
+      </c>
+      <c r="J31">
+        <v>9</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>12</v>
+      </c>
+      <c r="M31">
+        <v>22</v>
+      </c>
+      <c r="N31">
+        <v>23</v>
+      </c>
+      <c r="O31">
+        <v>15</v>
+      </c>
+      <c r="P31">
+        <v>13</v>
+      </c>
+      <c r="Q31">
+        <v>8</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>2</v>
+      </c>
+      <c r="T31">
+        <v>23</v>
+      </c>
+      <c r="U31">
+        <v>18</v>
+      </c>
+      <c r="V31">
+        <v>18</v>
+      </c>
+      <c r="W31">
+        <v>21</v>
+      </c>
+      <c r="X31">
+        <v>10</v>
+      </c>
+      <c r="Z31">
+        <v>13</v>
+      </c>
+      <c r="AA31">
+        <v>14</v>
+      </c>
+      <c r="AB31">
+        <v>16</v>
+      </c>
+      <c r="AC31">
+        <v>18</v>
+      </c>
+      <c r="AD31">
+        <v>15</v>
+      </c>
+      <c r="AE31">
+        <v>8</v>
+      </c>
+      <c r="AG31">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>2</v>
+      </c>
+      <c r="O32">
+        <v>4</v>
+      </c>
+      <c r="P32">
+        <v>5</v>
+      </c>
+      <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <v>2</v>
+      </c>
+      <c r="V32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>1</v>
+      </c>
+      <c r="Z32">
+        <v>1</v>
+      </c>
+      <c r="AB32">
+        <v>3</v>
+      </c>
+      <c r="AC32">
+        <v>2</v>
+      </c>
+      <c r="AD32">
+        <v>1</v>
+      </c>
+      <c r="AG32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>4</v>
+      </c>
+      <c r="M33">
+        <v>6</v>
+      </c>
+      <c r="N33">
+        <v>4</v>
+      </c>
+      <c r="O33">
+        <v>4</v>
+      </c>
+      <c r="P33">
+        <v>5</v>
+      </c>
+      <c r="Q33">
+        <v>3</v>
+      </c>
+      <c r="T33">
+        <v>5</v>
+      </c>
+      <c r="U33">
+        <v>1</v>
+      </c>
+      <c r="V33">
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <v>4</v>
+      </c>
+      <c r="Z33">
+        <v>1</v>
+      </c>
+      <c r="AA33">
+        <v>6</v>
+      </c>
+      <c r="AC33">
+        <v>6</v>
+      </c>
+      <c r="AD33">
+        <v>4</v>
+      </c>
+      <c r="AG33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34">
+        <v>22</v>
+      </c>
+      <c r="C34">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>30</v>
+      </c>
+      <c r="F34">
+        <v>34</v>
+      </c>
+      <c r="G34">
+        <v>23</v>
+      </c>
+      <c r="H34">
+        <v>22</v>
+      </c>
+      <c r="I34">
+        <v>31</v>
+      </c>
+      <c r="J34">
+        <v>14</v>
+      </c>
+      <c r="L34">
+        <v>41</v>
+      </c>
+      <c r="M34">
+        <v>26</v>
+      </c>
+      <c r="N34">
+        <v>34</v>
+      </c>
+      <c r="O34">
+        <v>22</v>
+      </c>
+      <c r="P34">
+        <v>20</v>
+      </c>
+      <c r="Q34">
+        <v>10</v>
+      </c>
+      <c r="S34">
+        <v>36</v>
+      </c>
+      <c r="T34">
+        <v>35</v>
+      </c>
+      <c r="U34">
+        <v>29</v>
+      </c>
+      <c r="V34">
+        <v>18</v>
+      </c>
+      <c r="W34">
+        <v>20</v>
+      </c>
+      <c r="X34">
+        <v>22</v>
+      </c>
+      <c r="Z34">
+        <v>31</v>
+      </c>
+      <c r="AA34">
+        <v>26</v>
+      </c>
+      <c r="AB34">
+        <v>31</v>
+      </c>
+      <c r="AC34">
+        <v>27</v>
+      </c>
+      <c r="AD34">
+        <v>16</v>
+      </c>
+      <c r="AE34">
+        <v>14</v>
+      </c>
+      <c r="AG34">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>27</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>55</v>
+      </c>
+      <c r="F35">
+        <v>16</v>
+      </c>
+      <c r="G35">
+        <v>16</v>
+      </c>
+      <c r="H35">
+        <v>18</v>
+      </c>
+      <c r="I35">
+        <v>35</v>
+      </c>
+      <c r="J35">
+        <v>18</v>
+      </c>
+      <c r="L35">
+        <v>22</v>
+      </c>
+      <c r="M35">
+        <v>17</v>
+      </c>
+      <c r="N35">
+        <v>28</v>
+      </c>
+      <c r="O35">
+        <v>23</v>
+      </c>
+      <c r="P35">
+        <v>23</v>
+      </c>
+      <c r="Q35">
+        <v>17</v>
+      </c>
+      <c r="R35">
+        <v>1</v>
+      </c>
+      <c r="S35">
+        <v>28</v>
+      </c>
+      <c r="T35">
+        <v>25</v>
+      </c>
+      <c r="U35">
+        <v>18</v>
+      </c>
+      <c r="V35">
+        <v>20</v>
+      </c>
+      <c r="W35">
+        <v>31</v>
+      </c>
+      <c r="X35">
+        <v>6</v>
+      </c>
+      <c r="Z35">
+        <v>32</v>
+      </c>
+      <c r="AA35">
+        <v>27</v>
+      </c>
+      <c r="AB35">
+        <v>13</v>
+      </c>
+      <c r="AC35">
+        <v>16</v>
+      </c>
+      <c r="AD35">
+        <v>28</v>
+      </c>
+      <c r="AE35">
+        <v>12</v>
+      </c>
+      <c r="AG35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36">
+        <v>15</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>18</v>
+      </c>
+      <c r="F36">
+        <v>16</v>
+      </c>
+      <c r="G36">
+        <v>10</v>
+      </c>
+      <c r="H36">
+        <v>25</v>
+      </c>
+      <c r="I36">
+        <v>14</v>
+      </c>
+      <c r="J36">
+        <v>9</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>24</v>
+      </c>
+      <c r="M36">
+        <v>17</v>
+      </c>
+      <c r="N36">
+        <v>10</v>
+      </c>
+      <c r="O36">
+        <v>12</v>
+      </c>
+      <c r="P36">
+        <v>12</v>
+      </c>
+      <c r="Q36">
+        <v>14</v>
+      </c>
+      <c r="R36">
+        <v>4</v>
+      </c>
+      <c r="S36">
+        <v>13</v>
+      </c>
+      <c r="T36">
+        <v>16</v>
+      </c>
+      <c r="U36">
+        <v>17</v>
+      </c>
+      <c r="V36">
+        <v>14</v>
+      </c>
+      <c r="W36">
+        <v>12</v>
+      </c>
+      <c r="X36">
+        <v>7</v>
+      </c>
+      <c r="Y36">
+        <v>2</v>
+      </c>
+      <c r="Z36">
+        <v>21</v>
+      </c>
+      <c r="AA36">
+        <v>17</v>
+      </c>
+      <c r="AB36">
+        <v>20</v>
+      </c>
+      <c r="AC36">
+        <v>15</v>
+      </c>
+      <c r="AD36">
+        <v>15</v>
+      </c>
+      <c r="AE36">
+        <v>7</v>
+      </c>
+      <c r="AG36">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <v>82</v>
+      </c>
+      <c r="C37">
+        <v>28</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>69</v>
+      </c>
+      <c r="F37">
+        <v>58</v>
+      </c>
+      <c r="G37">
+        <v>47</v>
+      </c>
+      <c r="H37">
+        <v>44</v>
+      </c>
+      <c r="I37">
+        <v>69</v>
+      </c>
+      <c r="J37">
+        <v>34</v>
+      </c>
+      <c r="K37">
+        <v>2</v>
+      </c>
+      <c r="L37">
+        <v>63</v>
+      </c>
+      <c r="M37">
+        <v>69</v>
+      </c>
+      <c r="N37">
+        <v>54</v>
+      </c>
+      <c r="O37">
+        <v>70</v>
+      </c>
+      <c r="P37">
+        <v>52</v>
+      </c>
+      <c r="Q37">
+        <v>35</v>
+      </c>
+      <c r="R37">
+        <v>3</v>
+      </c>
+      <c r="S37">
+        <v>70</v>
+      </c>
+      <c r="T37">
+        <v>46</v>
+      </c>
+      <c r="U37">
+        <v>51</v>
+      </c>
+      <c r="V37">
+        <v>52</v>
+      </c>
+      <c r="W37">
+        <v>65</v>
+      </c>
+      <c r="X37">
+        <v>25</v>
+      </c>
+      <c r="Y37">
+        <v>5</v>
+      </c>
+      <c r="Z37">
+        <v>71</v>
+      </c>
+      <c r="AA37">
+        <v>75</v>
+      </c>
+      <c r="AB37">
+        <v>55</v>
+      </c>
+      <c r="AC37">
+        <v>56</v>
+      </c>
+      <c r="AD37">
+        <v>51</v>
+      </c>
+      <c r="AE37">
+        <v>29</v>
+      </c>
+      <c r="AG37">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>16</v>
+      </c>
+      <c r="F38">
+        <v>11</v>
+      </c>
+      <c r="G38">
+        <v>10</v>
+      </c>
+      <c r="H38">
+        <v>11</v>
+      </c>
+      <c r="I38">
+        <v>8</v>
+      </c>
+      <c r="J38">
+        <v>4</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+      <c r="L38">
+        <v>13</v>
+      </c>
+      <c r="M38">
+        <v>17</v>
+      </c>
+      <c r="N38">
+        <v>10</v>
+      </c>
+      <c r="O38">
+        <v>7</v>
+      </c>
+      <c r="P38">
+        <v>11</v>
+      </c>
+      <c r="Q38">
+        <v>8</v>
+      </c>
+      <c r="S38">
+        <v>20</v>
+      </c>
+      <c r="T38">
+        <v>24</v>
+      </c>
+      <c r="U38">
+        <v>12</v>
+      </c>
+      <c r="V38">
+        <v>12</v>
+      </c>
+      <c r="W38">
+        <v>18</v>
+      </c>
+      <c r="X38">
+        <v>7</v>
+      </c>
+      <c r="Z38">
+        <v>8</v>
+      </c>
+      <c r="AA38">
+        <v>12</v>
+      </c>
+      <c r="AB38">
+        <v>12</v>
+      </c>
+      <c r="AC38">
+        <v>11</v>
+      </c>
+      <c r="AD38">
+        <v>13</v>
+      </c>
+      <c r="AE38">
+        <v>5</v>
+      </c>
+      <c r="AG38">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>45</v>
+      </c>
+      <c r="C39">
+        <v>16</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>49</v>
+      </c>
+      <c r="F39">
+        <v>45</v>
+      </c>
+      <c r="G39">
+        <v>31</v>
+      </c>
+      <c r="H39">
+        <v>42</v>
+      </c>
+      <c r="I39">
+        <v>24</v>
+      </c>
+      <c r="J39">
+        <v>20</v>
+      </c>
+      <c r="L39">
+        <v>46</v>
+      </c>
+      <c r="M39">
+        <v>37</v>
+      </c>
+      <c r="N39">
+        <v>32</v>
+      </c>
+      <c r="O39">
+        <v>28</v>
+      </c>
+      <c r="P39">
+        <v>34</v>
+      </c>
+      <c r="Q39">
+        <v>17</v>
+      </c>
+      <c r="R39">
+        <v>3</v>
+      </c>
+      <c r="S39">
+        <v>48</v>
+      </c>
+      <c r="T39">
+        <v>41</v>
+      </c>
+      <c r="U39">
+        <v>35</v>
+      </c>
+      <c r="V39">
+        <v>41</v>
+      </c>
+      <c r="W39">
+        <v>15</v>
+      </c>
+      <c r="X39">
+        <v>25</v>
+      </c>
+      <c r="Z39">
+        <v>41</v>
+      </c>
+      <c r="AA39">
+        <v>33</v>
+      </c>
+      <c r="AB39">
+        <v>39</v>
+      </c>
+      <c r="AC39">
+        <v>46</v>
+      </c>
+      <c r="AD39">
+        <v>35</v>
+      </c>
+      <c r="AE39">
+        <v>22</v>
+      </c>
+      <c r="AG39">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>5</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>6</v>
+      </c>
+      <c r="O40">
+        <v>6</v>
+      </c>
+      <c r="T40">
+        <v>2</v>
+      </c>
+      <c r="V40">
+        <v>3</v>
+      </c>
+      <c r="W40">
+        <v>1</v>
+      </c>
+      <c r="X40">
+        <v>2</v>
+      </c>
+      <c r="AA40">
+        <v>5</v>
+      </c>
+      <c r="AC40">
+        <v>1</v>
+      </c>
+      <c r="AD40">
+        <v>1</v>
+      </c>
+      <c r="AE40">
+        <v>2</v>
+      </c>
+      <c r="AG40">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>4</v>
+      </c>
+      <c r="G41">
+        <v>5</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>2</v>
+      </c>
+      <c r="N41">
+        <v>4</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="P41">
+        <v>4</v>
+      </c>
+      <c r="T41">
+        <v>3</v>
+      </c>
+      <c r="U41">
+        <v>4</v>
+      </c>
+      <c r="V41">
+        <v>8</v>
+      </c>
+      <c r="W41">
+        <v>3</v>
+      </c>
+      <c r="X41">
+        <v>1</v>
+      </c>
+      <c r="AA41">
+        <v>4</v>
+      </c>
+      <c r="AB41">
+        <v>3</v>
+      </c>
+      <c r="AC41">
+        <v>1</v>
+      </c>
+      <c r="AD41">
+        <v>5</v>
+      </c>
+      <c r="AE41">
+        <v>4</v>
+      </c>
+      <c r="AG41">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42">
+        <v>18</v>
+      </c>
+      <c r="E42">
+        <v>15</v>
+      </c>
+      <c r="F42">
+        <v>15</v>
+      </c>
+      <c r="G42">
+        <v>8</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42">
+        <v>17</v>
+      </c>
+      <c r="L42">
+        <v>3</v>
+      </c>
+      <c r="M42">
+        <v>11</v>
+      </c>
+      <c r="N42">
+        <v>9</v>
+      </c>
+      <c r="O42">
+        <v>20</v>
+      </c>
+      <c r="S42">
+        <v>11</v>
+      </c>
+      <c r="T42">
+        <v>5</v>
+      </c>
+      <c r="U42">
+        <v>16</v>
+      </c>
+      <c r="V42">
+        <v>5</v>
+      </c>
+      <c r="W42">
+        <v>8</v>
+      </c>
+      <c r="Z42">
+        <v>19</v>
+      </c>
+      <c r="AA42">
+        <v>13</v>
+      </c>
+      <c r="AB42">
+        <v>12</v>
+      </c>
+      <c r="AC42">
+        <v>21</v>
+      </c>
+      <c r="AD42">
+        <v>11</v>
+      </c>
+      <c r="AG42">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43">
+        <v>54</v>
+      </c>
+      <c r="E43">
+        <v>74</v>
+      </c>
+      <c r="F43">
+        <v>57</v>
+      </c>
+      <c r="G43">
+        <v>51</v>
+      </c>
+      <c r="H43">
+        <v>68</v>
+      </c>
+      <c r="I43">
+        <v>40</v>
+      </c>
+      <c r="L43">
+        <v>63</v>
+      </c>
+      <c r="M43">
+        <v>73</v>
+      </c>
+      <c r="N43">
+        <v>67</v>
+      </c>
+      <c r="O43">
+        <v>66</v>
+      </c>
+      <c r="S43">
+        <v>1</v>
+      </c>
+      <c r="T43">
+        <v>3</v>
+      </c>
+      <c r="V43">
+        <v>1</v>
+      </c>
+      <c r="Z43">
+        <v>59</v>
+      </c>
+      <c r="AA43">
+        <v>52</v>
+      </c>
+      <c r="AB43">
+        <v>58</v>
+      </c>
+      <c r="AC43">
+        <v>57</v>
+      </c>
+      <c r="AD43">
+        <v>45</v>
+      </c>
+      <c r="AG43">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="W44">
+        <v>3</v>
+      </c>
+      <c r="AB44">
+        <v>1</v>
+      </c>
+      <c r="AD44">
+        <v>2</v>
+      </c>
+      <c r="AG44">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45">
+        <v>11</v>
+      </c>
+      <c r="E45">
+        <v>8</v>
+      </c>
+      <c r="F45">
+        <v>9</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>7</v>
+      </c>
+      <c r="I45">
+        <v>8</v>
+      </c>
+      <c r="L45">
+        <v>16</v>
+      </c>
+      <c r="M45">
+        <v>9</v>
+      </c>
+      <c r="N45">
+        <v>10</v>
+      </c>
+      <c r="O45">
+        <v>5</v>
+      </c>
+      <c r="S45">
+        <v>3</v>
+      </c>
+      <c r="T45">
+        <v>2</v>
+      </c>
+      <c r="U45">
+        <v>2</v>
+      </c>
+      <c r="V45">
+        <v>1</v>
+      </c>
+      <c r="W45">
+        <v>30</v>
+      </c>
+      <c r="Z45">
+        <v>16</v>
+      </c>
+      <c r="AA45">
+        <v>3</v>
+      </c>
+      <c r="AB45">
+        <v>1</v>
+      </c>
+      <c r="AC45">
+        <v>2</v>
+      </c>
+      <c r="AD45">
+        <v>4</v>
+      </c>
+      <c r="AG45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>21</v>
+      </c>
+      <c r="G46">
+        <v>8</v>
+      </c>
+      <c r="H46">
+        <v>22</v>
+      </c>
+      <c r="I46">
+        <v>9</v>
+      </c>
+      <c r="L46">
+        <v>2</v>
+      </c>
+      <c r="M46">
+        <v>13</v>
+      </c>
+      <c r="N46">
+        <v>22</v>
+      </c>
+      <c r="O46">
+        <v>23</v>
+      </c>
+      <c r="S46">
+        <v>1</v>
+      </c>
+      <c r="T46">
+        <v>9</v>
+      </c>
+      <c r="U46">
+        <v>24</v>
+      </c>
+      <c r="V46">
+        <v>19</v>
+      </c>
+      <c r="W46">
+        <v>8</v>
+      </c>
+      <c r="AA46">
+        <v>16</v>
+      </c>
+      <c r="AB46">
+        <v>27</v>
+      </c>
+      <c r="AC46">
+        <v>23</v>
+      </c>
+      <c r="AG46">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>6</v>
+      </c>
+      <c r="G47">
+        <v>8</v>
+      </c>
+      <c r="H47">
+        <v>6</v>
+      </c>
+      <c r="I47">
+        <v>12</v>
+      </c>
+      <c r="J47">
+        <v>6</v>
+      </c>
+      <c r="L47">
+        <v>8</v>
+      </c>
+      <c r="N47">
+        <v>10</v>
+      </c>
+      <c r="O47">
+        <v>8</v>
+      </c>
+      <c r="P47">
+        <v>7</v>
+      </c>
+      <c r="Q47">
+        <v>3</v>
+      </c>
+      <c r="S47">
+        <v>9</v>
+      </c>
+      <c r="U47">
+        <v>11</v>
+      </c>
+      <c r="V47">
+        <v>6</v>
+      </c>
+      <c r="W47">
+        <v>8</v>
+      </c>
+      <c r="X47">
+        <v>1</v>
+      </c>
+      <c r="Z47">
+        <v>11</v>
+      </c>
+      <c r="AA47">
+        <v>1</v>
+      </c>
+      <c r="AB47">
+        <v>10</v>
+      </c>
+      <c r="AC47">
+        <v>9</v>
+      </c>
+      <c r="AD47">
+        <v>5</v>
+      </c>
+      <c r="AE47">
+        <v>4</v>
+      </c>
+      <c r="AG47">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48">
+        <v>21</v>
+      </c>
+      <c r="C48">
+        <v>6</v>
+      </c>
+      <c r="E48">
+        <v>12</v>
+      </c>
+      <c r="F48">
+        <v>16</v>
+      </c>
+      <c r="G48">
+        <v>17</v>
+      </c>
+      <c r="H48">
+        <v>15</v>
+      </c>
+      <c r="I48">
+        <v>17</v>
+      </c>
+      <c r="J48">
+        <v>4</v>
+      </c>
+      <c r="L48">
+        <v>37</v>
+      </c>
+      <c r="M48">
+        <v>20</v>
+      </c>
+      <c r="N48">
+        <v>20</v>
+      </c>
+      <c r="O48">
+        <v>32</v>
+      </c>
+      <c r="P48">
+        <v>18</v>
+      </c>
+      <c r="Q48">
+        <v>4</v>
+      </c>
+      <c r="S48">
+        <v>3</v>
+      </c>
+      <c r="T48">
+        <v>29</v>
+      </c>
+      <c r="U48">
+        <v>17</v>
+      </c>
+      <c r="V48">
+        <v>23</v>
+      </c>
+      <c r="W48">
+        <v>12</v>
+      </c>
+      <c r="X48">
+        <v>13</v>
+      </c>
+      <c r="Y48">
+        <v>1</v>
+      </c>
+      <c r="Z48">
+        <v>11</v>
+      </c>
+      <c r="AA48">
+        <v>16</v>
+      </c>
+      <c r="AB48">
+        <v>21</v>
+      </c>
+      <c r="AC48">
+        <v>16</v>
+      </c>
+      <c r="AD48">
+        <v>27</v>
+      </c>
+      <c r="AE48">
+        <v>14</v>
+      </c>
+      <c r="AG48">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49">
+        <v>31</v>
+      </c>
+      <c r="C49">
+        <v>16</v>
+      </c>
+      <c r="E49">
+        <v>31</v>
+      </c>
+      <c r="F49">
+        <v>30</v>
+      </c>
+      <c r="G49">
+        <v>35</v>
+      </c>
+      <c r="H49">
+        <v>20</v>
+      </c>
+      <c r="I49">
+        <v>23</v>
+      </c>
+      <c r="J49">
+        <v>15</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <v>33</v>
+      </c>
+      <c r="M49">
+        <v>24</v>
+      </c>
+      <c r="N49">
+        <v>33</v>
+      </c>
+      <c r="O49">
+        <v>26</v>
+      </c>
+      <c r="P49">
+        <v>37</v>
+      </c>
+      <c r="Q49">
+        <v>19</v>
+      </c>
+      <c r="S49">
+        <v>39</v>
+      </c>
+      <c r="T49">
+        <v>32</v>
+      </c>
+      <c r="U49">
+        <v>35</v>
+      </c>
+      <c r="V49">
+        <v>15</v>
+      </c>
+      <c r="W49">
+        <v>35</v>
+      </c>
+      <c r="X49">
+        <v>14</v>
+      </c>
+      <c r="Y49">
+        <v>2</v>
+      </c>
+      <c r="Z49">
+        <v>38</v>
+      </c>
+      <c r="AA49">
+        <v>22</v>
+      </c>
+      <c r="AB49">
+        <v>27</v>
+      </c>
+      <c r="AC49">
+        <v>28</v>
+      </c>
+      <c r="AD49">
+        <v>34</v>
+      </c>
+      <c r="AE49">
+        <v>14</v>
+      </c>
+      <c r="AG49">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50">
+        <v>19</v>
+      </c>
+      <c r="C50">
+        <v>13</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>29</v>
+      </c>
+      <c r="F50">
+        <v>19</v>
+      </c>
+      <c r="G50">
+        <v>31</v>
+      </c>
+      <c r="H50">
+        <v>20</v>
+      </c>
+      <c r="I50">
+        <v>16</v>
+      </c>
+      <c r="J50">
+        <v>10</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>25</v>
+      </c>
+      <c r="M50">
+        <v>26</v>
+      </c>
+      <c r="N50">
+        <v>26</v>
+      </c>
+      <c r="O50">
+        <v>20</v>
+      </c>
+      <c r="P50">
+        <v>6</v>
+      </c>
+      <c r="Q50">
+        <v>1</v>
+      </c>
+      <c r="R50">
+        <v>1</v>
+      </c>
+      <c r="S50">
+        <v>31</v>
+      </c>
+      <c r="T50">
+        <v>22</v>
+      </c>
+      <c r="U50">
+        <v>21</v>
+      </c>
+      <c r="V50">
+        <v>20</v>
+      </c>
+      <c r="W50">
+        <v>14</v>
+      </c>
+      <c r="X50">
+        <v>17</v>
+      </c>
+      <c r="Y50">
+        <v>1</v>
+      </c>
+      <c r="Z50">
+        <v>28</v>
+      </c>
+      <c r="AA50">
+        <v>21</v>
+      </c>
+      <c r="AB50">
+        <v>23</v>
+      </c>
+      <c r="AC50">
+        <v>24</v>
+      </c>
+      <c r="AD50">
+        <v>14</v>
+      </c>
+      <c r="AE50">
+        <v>13</v>
+      </c>
+      <c r="AG50">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51">
+        <v>23</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>24</v>
+      </c>
+      <c r="F51">
+        <v>26</v>
+      </c>
+      <c r="G51">
+        <v>16</v>
+      </c>
+      <c r="H51">
+        <v>30</v>
+      </c>
+      <c r="I51">
+        <v>9</v>
+      </c>
+      <c r="J51">
+        <v>7</v>
+      </c>
+      <c r="L51">
+        <v>17</v>
+      </c>
+      <c r="M51">
+        <v>37</v>
+      </c>
+      <c r="N51">
+        <v>23</v>
+      </c>
+      <c r="O51">
+        <v>10</v>
+      </c>
+      <c r="P51">
+        <v>12</v>
+      </c>
+      <c r="Q51">
+        <v>7</v>
+      </c>
+      <c r="R51">
+        <v>1</v>
+      </c>
+      <c r="S51">
+        <v>11</v>
+      </c>
+      <c r="T51">
+        <v>20</v>
+      </c>
+      <c r="U51">
+        <v>21</v>
+      </c>
+      <c r="V51">
+        <v>5</v>
+      </c>
+      <c r="W51">
+        <v>20</v>
+      </c>
+      <c r="X51">
+        <v>37</v>
+      </c>
+      <c r="Z51">
+        <v>12</v>
+      </c>
+      <c r="AA51">
+        <v>20</v>
+      </c>
+      <c r="AB51">
+        <v>18</v>
+      </c>
+      <c r="AC51">
+        <v>16</v>
+      </c>
+      <c r="AD51">
+        <v>26</v>
+      </c>
+      <c r="AE51">
+        <v>4</v>
+      </c>
+      <c r="AG51">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52">
+        <v>41</v>
+      </c>
+      <c r="C52">
+        <v>20</v>
+      </c>
+      <c r="D52">
+        <v>17</v>
+      </c>
+      <c r="E52">
+        <v>34</v>
+      </c>
+      <c r="F52">
+        <v>58</v>
+      </c>
+      <c r="G52">
+        <v>49</v>
+      </c>
+      <c r="H52">
+        <v>47</v>
+      </c>
+      <c r="I52">
+        <v>32</v>
+      </c>
+      <c r="J52">
+        <v>11</v>
+      </c>
+      <c r="K52">
+        <v>4</v>
+      </c>
+      <c r="L52">
+        <v>37</v>
+      </c>
+      <c r="M52">
+        <v>35</v>
+      </c>
+      <c r="N52">
+        <v>48</v>
+      </c>
+      <c r="O52">
+        <v>32</v>
+      </c>
+      <c r="P52">
+        <v>36</v>
+      </c>
+      <c r="Q52">
+        <v>18</v>
+      </c>
+      <c r="S52">
+        <v>37</v>
+      </c>
+      <c r="T52">
+        <v>52</v>
+      </c>
+      <c r="U52">
+        <v>41</v>
+      </c>
+      <c r="V52">
+        <v>40</v>
+      </c>
+      <c r="W52">
+        <v>40</v>
+      </c>
+      <c r="X52">
+        <v>26</v>
+      </c>
+      <c r="Y52">
+        <v>14</v>
+      </c>
+      <c r="Z52">
+        <v>41</v>
+      </c>
+      <c r="AA52">
+        <v>47</v>
+      </c>
+      <c r="AB52">
+        <v>32</v>
+      </c>
+      <c r="AC52">
+        <v>38</v>
+      </c>
+      <c r="AD52">
+        <v>36</v>
+      </c>
+      <c r="AE52">
+        <v>29</v>
+      </c>
+      <c r="AG52">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>7</v>
+      </c>
+      <c r="E53">
+        <v>5</v>
+      </c>
+      <c r="F53">
+        <v>4</v>
+      </c>
+      <c r="G53">
+        <v>7</v>
+      </c>
+      <c r="H53">
+        <v>5</v>
+      </c>
+      <c r="I53">
+        <v>4</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>6</v>
+      </c>
+      <c r="M53">
+        <v>5</v>
+      </c>
+      <c r="N53">
+        <v>8</v>
+      </c>
+      <c r="O53">
+        <v>4</v>
+      </c>
+      <c r="P53">
+        <v>5</v>
+      </c>
+      <c r="Q53">
+        <v>3</v>
+      </c>
+      <c r="S53">
+        <v>5</v>
+      </c>
+      <c r="T53">
+        <v>5</v>
+      </c>
+      <c r="U53">
+        <v>8</v>
+      </c>
+      <c r="V53">
+        <v>4</v>
+      </c>
+      <c r="W53">
+        <v>3</v>
+      </c>
+      <c r="X53">
+        <v>7</v>
+      </c>
+      <c r="Z53">
+        <v>4</v>
+      </c>
+      <c r="AA53">
+        <v>6</v>
+      </c>
+      <c r="AB53">
+        <v>9</v>
+      </c>
+      <c r="AC53">
+        <v>2</v>
+      </c>
+      <c r="AD53">
+        <v>5</v>
+      </c>
+      <c r="AE53">
+        <v>5</v>
+      </c>
+      <c r="AG53">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54">
+        <v>10</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <v>19</v>
+      </c>
+      <c r="F54">
+        <v>13</v>
+      </c>
+      <c r="G54">
+        <v>29</v>
+      </c>
+      <c r="H54">
+        <v>17</v>
+      </c>
+      <c r="I54">
+        <v>18</v>
+      </c>
+      <c r="J54">
+        <v>5</v>
+      </c>
+      <c r="L54">
+        <v>13</v>
+      </c>
+      <c r="M54">
+        <v>16</v>
+      </c>
+      <c r="N54">
+        <v>19</v>
+      </c>
+      <c r="O54">
+        <v>10</v>
+      </c>
+      <c r="P54">
+        <v>14</v>
+      </c>
+      <c r="Q54">
+        <v>6</v>
+      </c>
+      <c r="R54">
+        <v>2</v>
+      </c>
+      <c r="S54">
+        <v>21</v>
+      </c>
+      <c r="T54">
+        <v>17</v>
+      </c>
+      <c r="U54">
+        <v>19</v>
+      </c>
+      <c r="V54">
+        <v>5</v>
+      </c>
+      <c r="W54">
+        <v>13</v>
+      </c>
+      <c r="X54">
+        <v>7</v>
+      </c>
+      <c r="Z54">
+        <v>24</v>
+      </c>
+      <c r="AA54">
+        <v>9</v>
+      </c>
+      <c r="AB54">
+        <v>19</v>
+      </c>
+      <c r="AC54">
+        <v>8</v>
+      </c>
+      <c r="AD54">
+        <v>14</v>
+      </c>
+      <c r="AE54">
+        <v>5</v>
+      </c>
+      <c r="AG54">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
+      <c r="L55">
+        <v>4</v>
+      </c>
+      <c r="M55">
+        <v>3</v>
+      </c>
+      <c r="N55">
+        <v>5</v>
+      </c>
+      <c r="O55">
+        <v>5</v>
+      </c>
+      <c r="P55">
+        <v>2</v>
+      </c>
+      <c r="Q55">
+        <v>3</v>
+      </c>
+      <c r="S55">
+        <v>4</v>
+      </c>
+      <c r="U55">
+        <v>2</v>
+      </c>
+      <c r="V55">
+        <v>4</v>
+      </c>
+      <c r="W55">
+        <v>5</v>
+      </c>
+      <c r="X55">
+        <v>1</v>
+      </c>
+      <c r="Z55">
+        <v>2</v>
+      </c>
+      <c r="AA55">
+        <v>1</v>
+      </c>
+      <c r="AB55">
+        <v>2</v>
+      </c>
+      <c r="AC55">
+        <v>1</v>
+      </c>
+      <c r="AD55">
+        <v>2</v>
+      </c>
+      <c r="AE55">
+        <v>3</v>
+      </c>
+      <c r="AG55">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+      <c r="G56">
+        <v>15</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>3</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="M56">
+        <v>4</v>
+      </c>
+      <c r="N56">
+        <v>8</v>
+      </c>
+      <c r="O56">
+        <v>5</v>
+      </c>
+      <c r="Q56">
+        <v>2</v>
+      </c>
+      <c r="S56">
+        <v>2</v>
+      </c>
+      <c r="U56">
+        <v>10</v>
+      </c>
+      <c r="V56">
+        <v>3</v>
+      </c>
+      <c r="X56">
+        <v>1</v>
+      </c>
+      <c r="Y56">
+        <v>1</v>
+      </c>
+      <c r="Z56">
+        <v>4</v>
+      </c>
+      <c r="AA56">
+        <v>2</v>
+      </c>
+      <c r="AB56">
+        <v>4</v>
+      </c>
+      <c r="AE56">
+        <v>3</v>
+      </c>
+      <c r="AG56">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57">
+        <v>6</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>12</v>
+      </c>
+      <c r="F57">
+        <v>4</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>6</v>
+      </c>
+      <c r="I57">
+        <v>8</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>4</v>
+      </c>
+      <c r="M57">
+        <v>7</v>
+      </c>
+      <c r="N57">
+        <v>8</v>
+      </c>
+      <c r="O57">
+        <v>6</v>
+      </c>
+      <c r="P57">
+        <v>9</v>
+      </c>
+      <c r="R57">
+        <v>1</v>
+      </c>
+      <c r="S57">
+        <v>8</v>
+      </c>
+      <c r="T57">
+        <v>5</v>
+      </c>
+      <c r="U57">
+        <v>2</v>
+      </c>
+      <c r="V57">
+        <v>5</v>
+      </c>
+      <c r="W57">
+        <v>5</v>
+      </c>
+      <c r="X57">
+        <v>1</v>
+      </c>
+      <c r="Z57">
+        <v>4</v>
+      </c>
+      <c r="AA57">
+        <v>5</v>
+      </c>
+      <c r="AB57">
+        <v>5</v>
+      </c>
+      <c r="AC57">
+        <v>6</v>
+      </c>
+      <c r="AD57">
+        <v>4</v>
+      </c>
+      <c r="AE57">
+        <v>1</v>
+      </c>
+      <c r="AG57">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:AG3" xr:uid="{9030ABEF-4467-42E7-BCDA-FF968810D030}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update data for June
</commit_message>
<xml_diff>
--- a/statistics_files/2022/2022.d.monthly_circ_by_borrower.unique_borrowers.xlsx
+++ b/statistics_files/2022/2022.d.monthly_circ_by_borrower.unique_borrowers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BB1981-64EF-4970-90FB-F64D5BE7B410}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B0B007-88BC-4247-9833-230D668C9E9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="894" activeTab="4" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="894" activeTab="5" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="2" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">April!$A$3:$AG$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">February!$A$3:$AG$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">January!$A$3:$AG$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">June!$A$3:$AG$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">March!$A$3:$AG$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">May!$A$3:$AG$57</definedName>
   </definedNames>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="73">
   <si>
     <t>branchname</t>
   </si>
@@ -259,6 +260,9 @@
   </si>
   <si>
     <t>2022-05-01 - 2022-05-30</t>
+  </si>
+  <si>
+    <t>2022-06-01 - 2022-06-30</t>
   </si>
 </sst>
 </file>
@@ -18502,7 +18506,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -22829,10 +22833,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC7559C5-98A6-49B7-ABC7-2F44371F9A3D}">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="B2:AF2"/>
+  <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
@@ -22844,38 +22848,4304 @@
     <col min="2" max="33" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44713</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44714</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44715</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44716</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44717</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44718</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44719</v>
+      </c>
+      <c r="I2" s="1">
+        <v>44720</v>
+      </c>
+      <c r="J2" s="1">
+        <v>44721</v>
+      </c>
+      <c r="K2" s="1">
+        <v>44722</v>
+      </c>
+      <c r="L2" s="1">
+        <v>44723</v>
+      </c>
+      <c r="M2" s="1">
+        <v>44724</v>
+      </c>
+      <c r="N2" s="1">
+        <v>44725</v>
+      </c>
+      <c r="O2" s="1">
+        <v>44726</v>
+      </c>
+      <c r="P2" s="1">
+        <v>44727</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>44728</v>
+      </c>
+      <c r="R2" s="1">
+        <v>44729</v>
+      </c>
+      <c r="S2" s="1">
+        <v>44730</v>
+      </c>
+      <c r="T2" s="1">
+        <v>44731</v>
+      </c>
+      <c r="U2" s="1">
+        <v>44732</v>
+      </c>
+      <c r="V2" s="1">
+        <v>44733</v>
+      </c>
+      <c r="W2" s="1">
+        <v>44734</v>
+      </c>
+      <c r="X2" s="1">
+        <v>44735</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>44736</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>44737</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>44738</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>44739</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>44740</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>44741</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>44742</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U3" t="s">
+        <v>7</v>
+      </c>
+      <c r="V3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>67</v>
+      </c>
+      <c r="C4">
+        <v>68</v>
+      </c>
+      <c r="D4">
+        <v>67</v>
+      </c>
+      <c r="E4">
+        <v>24</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>76</v>
+      </c>
+      <c r="H4">
+        <v>87</v>
+      </c>
+      <c r="I4">
+        <v>91</v>
+      </c>
+      <c r="J4">
+        <v>92</v>
+      </c>
+      <c r="K4">
+        <v>53</v>
+      </c>
+      <c r="L4">
+        <v>48</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>79</v>
+      </c>
+      <c r="O4">
+        <v>75</v>
+      </c>
+      <c r="P4">
+        <v>75</v>
+      </c>
+      <c r="Q4">
+        <v>77</v>
+      </c>
+      <c r="R4">
+        <v>66</v>
+      </c>
+      <c r="S4">
+        <v>37</v>
+      </c>
+      <c r="T4">
+        <v>9</v>
+      </c>
+      <c r="U4">
+        <v>70</v>
+      </c>
+      <c r="V4">
+        <v>80</v>
+      </c>
+      <c r="W4">
+        <v>83</v>
+      </c>
+      <c r="X4">
+        <v>73</v>
+      </c>
+      <c r="Y4">
+        <v>56</v>
+      </c>
+      <c r="Z4">
+        <v>32</v>
+      </c>
+      <c r="AA4">
+        <v>7</v>
+      </c>
+      <c r="AB4">
+        <v>74</v>
+      </c>
+      <c r="AC4">
+        <v>78</v>
+      </c>
+      <c r="AD4">
+        <v>88</v>
+      </c>
+      <c r="AE4">
+        <v>74</v>
+      </c>
+      <c r="AG4">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>46</v>
+      </c>
+      <c r="D5">
+        <v>33</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>52</v>
+      </c>
+      <c r="H5">
+        <v>48</v>
+      </c>
+      <c r="I5">
+        <v>50</v>
+      </c>
+      <c r="J5">
+        <v>38</v>
+      </c>
+      <c r="K5">
+        <v>35</v>
+      </c>
+      <c r="L5">
+        <v>25</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>36</v>
+      </c>
+      <c r="O5">
+        <v>54</v>
+      </c>
+      <c r="P5">
+        <v>52</v>
+      </c>
+      <c r="Q5">
+        <v>47</v>
+      </c>
+      <c r="R5">
+        <v>31</v>
+      </c>
+      <c r="S5">
+        <v>30</v>
+      </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
+      <c r="U5">
+        <v>49</v>
+      </c>
+      <c r="V5">
+        <v>49</v>
+      </c>
+      <c r="W5">
+        <v>46</v>
+      </c>
+      <c r="X5">
+        <v>38</v>
+      </c>
+      <c r="Y5">
+        <v>38</v>
+      </c>
+      <c r="Z5">
+        <v>24</v>
+      </c>
+      <c r="AB5">
+        <v>43</v>
+      </c>
+      <c r="AC5">
+        <v>55</v>
+      </c>
+      <c r="AD5">
+        <v>49</v>
+      </c>
+      <c r="AE5">
+        <v>42</v>
+      </c>
+      <c r="AG5">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>115</v>
+      </c>
+      <c r="C6">
+        <v>102</v>
+      </c>
+      <c r="D6">
+        <v>87</v>
+      </c>
+      <c r="E6">
+        <v>67</v>
+      </c>
+      <c r="F6">
+        <v>32</v>
+      </c>
+      <c r="G6">
+        <v>102</v>
+      </c>
+      <c r="H6">
+        <v>126</v>
+      </c>
+      <c r="I6">
+        <v>124</v>
+      </c>
+      <c r="J6">
+        <v>101</v>
+      </c>
+      <c r="K6">
+        <v>63</v>
+      </c>
+      <c r="L6">
+        <v>59</v>
+      </c>
+      <c r="M6">
+        <v>41</v>
+      </c>
+      <c r="N6">
+        <v>112</v>
+      </c>
+      <c r="O6">
+        <v>110</v>
+      </c>
+      <c r="P6">
+        <v>125</v>
+      </c>
+      <c r="Q6">
+        <v>95</v>
+      </c>
+      <c r="R6">
+        <v>95</v>
+      </c>
+      <c r="S6">
+        <v>57</v>
+      </c>
+      <c r="T6">
+        <v>6</v>
+      </c>
+      <c r="U6">
+        <v>90</v>
+      </c>
+      <c r="V6">
+        <v>96</v>
+      </c>
+      <c r="W6">
+        <v>133</v>
+      </c>
+      <c r="X6">
+        <v>94</v>
+      </c>
+      <c r="Y6">
+        <v>78</v>
+      </c>
+      <c r="Z6">
+        <v>64</v>
+      </c>
+      <c r="AA6">
+        <v>41</v>
+      </c>
+      <c r="AB6">
+        <v>96</v>
+      </c>
+      <c r="AC6">
+        <v>107</v>
+      </c>
+      <c r="AD6">
+        <v>144</v>
+      </c>
+      <c r="AE6">
+        <v>97</v>
+      </c>
+      <c r="AG6">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>3</v>
+      </c>
+      <c r="U7">
+        <v>2</v>
+      </c>
+      <c r="V7">
+        <v>2</v>
+      </c>
+      <c r="W7">
+        <v>8</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>3</v>
+      </c>
+      <c r="AB7">
+        <v>2</v>
+      </c>
+      <c r="AC7">
+        <v>5</v>
+      </c>
+      <c r="AD7">
+        <v>4</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>80</v>
+      </c>
+      <c r="C8">
+        <v>62</v>
+      </c>
+      <c r="D8">
+        <v>58</v>
+      </c>
+      <c r="E8">
+        <v>51</v>
+      </c>
+      <c r="F8">
+        <v>17</v>
+      </c>
+      <c r="G8">
+        <v>94</v>
+      </c>
+      <c r="H8">
+        <v>70</v>
+      </c>
+      <c r="I8">
+        <v>75</v>
+      </c>
+      <c r="J8">
+        <v>60</v>
+      </c>
+      <c r="K8">
+        <v>48</v>
+      </c>
+      <c r="L8">
+        <v>39</v>
+      </c>
+      <c r="M8">
+        <v>29</v>
+      </c>
+      <c r="N8">
+        <v>68</v>
+      </c>
+      <c r="O8">
+        <v>80</v>
+      </c>
+      <c r="P8">
+        <v>88</v>
+      </c>
+      <c r="Q8">
+        <v>60</v>
+      </c>
+      <c r="R8">
+        <v>56</v>
+      </c>
+      <c r="S8">
+        <v>51</v>
+      </c>
+      <c r="T8">
+        <v>5</v>
+      </c>
+      <c r="U8">
+        <v>71</v>
+      </c>
+      <c r="V8">
+        <v>98</v>
+      </c>
+      <c r="W8">
+        <v>74</v>
+      </c>
+      <c r="X8">
+        <v>72</v>
+      </c>
+      <c r="Y8">
+        <v>43</v>
+      </c>
+      <c r="Z8">
+        <v>35</v>
+      </c>
+      <c r="AA8">
+        <v>22</v>
+      </c>
+      <c r="AB8">
+        <v>68</v>
+      </c>
+      <c r="AC8">
+        <v>63</v>
+      </c>
+      <c r="AD8">
+        <v>95</v>
+      </c>
+      <c r="AE8">
+        <v>61</v>
+      </c>
+      <c r="AG8">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>3</v>
+      </c>
+      <c r="P9">
+        <v>15</v>
+      </c>
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="R9">
+        <v>7</v>
+      </c>
+      <c r="S9">
+        <v>4</v>
+      </c>
+      <c r="U9">
+        <v>14</v>
+      </c>
+      <c r="V9">
+        <v>2</v>
+      </c>
+      <c r="W9">
+        <v>17</v>
+      </c>
+      <c r="X9">
+        <v>14</v>
+      </c>
+      <c r="Y9">
+        <v>7</v>
+      </c>
+      <c r="Z9">
+        <v>3</v>
+      </c>
+      <c r="AB9">
+        <v>8</v>
+      </c>
+      <c r="AC9">
+        <v>4</v>
+      </c>
+      <c r="AD9">
+        <v>7</v>
+      </c>
+      <c r="AE9">
+        <v>15</v>
+      </c>
+      <c r="AG9">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
+      <c r="J10">
+        <v>15</v>
+      </c>
+      <c r="K10">
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <v>10</v>
+      </c>
+      <c r="N10">
+        <v>7</v>
+      </c>
+      <c r="O10">
+        <v>14</v>
+      </c>
+      <c r="P10">
+        <v>11</v>
+      </c>
+      <c r="Q10">
+        <v>7</v>
+      </c>
+      <c r="R10">
+        <v>7</v>
+      </c>
+      <c r="S10">
+        <v>9</v>
+      </c>
+      <c r="U10">
+        <v>16</v>
+      </c>
+      <c r="V10">
+        <v>9</v>
+      </c>
+      <c r="W10">
+        <v>20</v>
+      </c>
+      <c r="X10">
+        <v>6</v>
+      </c>
+      <c r="Y10">
+        <v>14</v>
+      </c>
+      <c r="Z10">
+        <v>5</v>
+      </c>
+      <c r="AB10">
+        <v>11</v>
+      </c>
+      <c r="AC10">
+        <v>15</v>
+      </c>
+      <c r="AD10">
+        <v>11</v>
+      </c>
+      <c r="AE10">
+        <v>11</v>
+      </c>
+      <c r="AG10">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>16</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>11</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>7</v>
+      </c>
+      <c r="P11">
+        <v>27</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="U11">
+        <v>2</v>
+      </c>
+      <c r="W11">
+        <v>13</v>
+      </c>
+      <c r="X11">
+        <v>4</v>
+      </c>
+      <c r="Y11">
+        <v>7</v>
+      </c>
+      <c r="Z11">
+        <v>3</v>
+      </c>
+      <c r="AB11">
+        <v>2</v>
+      </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
+      <c r="AD11">
+        <v>16</v>
+      </c>
+      <c r="AE11">
+        <v>3</v>
+      </c>
+      <c r="AG11">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>18</v>
+      </c>
+      <c r="O12">
+        <v>18</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>12</v>
+      </c>
+      <c r="W12">
+        <v>3</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AB12">
+        <v>4</v>
+      </c>
+      <c r="AC12">
+        <v>16</v>
+      </c>
+      <c r="AD12">
+        <v>3</v>
+      </c>
+      <c r="AG12">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>7</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>3</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>2</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>2</v>
+      </c>
+      <c r="Y14">
+        <v>5</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14">
+        <v>1</v>
+      </c>
+      <c r="AD14">
+        <v>4</v>
+      </c>
+      <c r="AE14">
+        <v>4</v>
+      </c>
+      <c r="AG14">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>12</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>9</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <v>5</v>
+      </c>
+      <c r="L15">
+        <v>5</v>
+      </c>
+      <c r="N15">
+        <v>8</v>
+      </c>
+      <c r="O15">
+        <v>5</v>
+      </c>
+      <c r="P15">
+        <v>10</v>
+      </c>
+      <c r="Q15">
+        <v>5</v>
+      </c>
+      <c r="R15">
+        <v>11</v>
+      </c>
+      <c r="S15">
+        <v>3</v>
+      </c>
+      <c r="U15">
+        <v>8</v>
+      </c>
+      <c r="V15">
+        <v>11</v>
+      </c>
+      <c r="W15">
+        <v>7</v>
+      </c>
+      <c r="X15">
+        <v>5</v>
+      </c>
+      <c r="Y15">
+        <v>9</v>
+      </c>
+      <c r="Z15">
+        <v>4</v>
+      </c>
+      <c r="AA15">
+        <v>1</v>
+      </c>
+      <c r="AB15">
+        <v>5</v>
+      </c>
+      <c r="AC15">
+        <v>5</v>
+      </c>
+      <c r="AD15">
+        <v>14</v>
+      </c>
+      <c r="AE15">
+        <v>11</v>
+      </c>
+      <c r="AG15">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>22</v>
+      </c>
+      <c r="H16">
+        <v>23</v>
+      </c>
+      <c r="I16">
+        <v>18</v>
+      </c>
+      <c r="J16">
+        <v>19</v>
+      </c>
+      <c r="K16">
+        <v>8</v>
+      </c>
+      <c r="L16">
+        <v>6</v>
+      </c>
+      <c r="N16">
+        <v>11</v>
+      </c>
+      <c r="O16">
+        <v>12</v>
+      </c>
+      <c r="P16">
+        <v>17</v>
+      </c>
+      <c r="Q16">
+        <v>16</v>
+      </c>
+      <c r="R16">
+        <v>16</v>
+      </c>
+      <c r="S16">
+        <v>5</v>
+      </c>
+      <c r="U16">
+        <v>11</v>
+      </c>
+      <c r="V16">
+        <v>12</v>
+      </c>
+      <c r="W16">
+        <v>22</v>
+      </c>
+      <c r="X16">
+        <v>23</v>
+      </c>
+      <c r="Y16">
+        <v>15</v>
+      </c>
+      <c r="Z16">
+        <v>8</v>
+      </c>
+      <c r="AB16">
+        <v>12</v>
+      </c>
+      <c r="AC16">
+        <v>19</v>
+      </c>
+      <c r="AD16">
+        <v>12</v>
+      </c>
+      <c r="AE16">
+        <v>6</v>
+      </c>
+      <c r="AG16">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>3</v>
+      </c>
+      <c r="N17">
+        <v>18</v>
+      </c>
+      <c r="O17">
+        <v>3</v>
+      </c>
+      <c r="P17">
+        <v>5</v>
+      </c>
+      <c r="Q17">
+        <v>24</v>
+      </c>
+      <c r="R17">
+        <v>8</v>
+      </c>
+      <c r="S17">
+        <v>6</v>
+      </c>
+      <c r="U17">
+        <v>4</v>
+      </c>
+      <c r="V17">
+        <v>9</v>
+      </c>
+      <c r="W17">
+        <v>6</v>
+      </c>
+      <c r="X17">
+        <v>5</v>
+      </c>
+      <c r="Y17">
+        <v>6</v>
+      </c>
+      <c r="Z17">
+        <v>2</v>
+      </c>
+      <c r="AB17">
+        <v>9</v>
+      </c>
+      <c r="AC17">
+        <v>7</v>
+      </c>
+      <c r="AD17">
+        <v>5</v>
+      </c>
+      <c r="AE17">
+        <v>8</v>
+      </c>
+      <c r="AG17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>13</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>11</v>
+      </c>
+      <c r="Q18">
+        <v>3</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>5</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>14</v>
+      </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
+      <c r="Y18">
+        <v>5</v>
+      </c>
+      <c r="Z18">
+        <v>4</v>
+      </c>
+      <c r="AB18">
+        <v>4</v>
+      </c>
+      <c r="AC18">
+        <v>6</v>
+      </c>
+      <c r="AD18">
+        <v>11</v>
+      </c>
+      <c r="AE18">
+        <v>2</v>
+      </c>
+      <c r="AG18">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>48</v>
+      </c>
+      <c r="C19">
+        <v>31</v>
+      </c>
+      <c r="D19">
+        <v>17</v>
+      </c>
+      <c r="E19">
+        <v>19</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>34</v>
+      </c>
+      <c r="H19">
+        <v>28</v>
+      </c>
+      <c r="I19">
+        <v>37</v>
+      </c>
+      <c r="J19">
+        <v>25</v>
+      </c>
+      <c r="K19">
+        <v>19</v>
+      </c>
+      <c r="L19">
+        <v>10</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>37</v>
+      </c>
+      <c r="O19">
+        <v>28</v>
+      </c>
+      <c r="P19">
+        <v>44</v>
+      </c>
+      <c r="Q19">
+        <v>20</v>
+      </c>
+      <c r="R19">
+        <v>16</v>
+      </c>
+      <c r="S19">
+        <v>17</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>2</v>
+      </c>
+      <c r="V19">
+        <v>41</v>
+      </c>
+      <c r="W19">
+        <v>38</v>
+      </c>
+      <c r="X19">
+        <v>23</v>
+      </c>
+      <c r="Y19">
+        <v>25</v>
+      </c>
+      <c r="Z19">
+        <v>17</v>
+      </c>
+      <c r="AA19">
+        <v>1</v>
+      </c>
+      <c r="AB19">
+        <v>29</v>
+      </c>
+      <c r="AC19">
+        <v>23</v>
+      </c>
+      <c r="AD19">
+        <v>38</v>
+      </c>
+      <c r="AE19">
+        <v>25</v>
+      </c>
+      <c r="AG19">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>7</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>2</v>
+      </c>
+      <c r="R20">
+        <v>6</v>
+      </c>
+      <c r="V20">
+        <v>2</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>3</v>
+      </c>
+      <c r="Z20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <v>5</v>
+      </c>
+      <c r="AD20">
+        <v>2</v>
+      </c>
+      <c r="AE20">
+        <v>2</v>
+      </c>
+      <c r="AG20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>45</v>
+      </c>
+      <c r="C21">
+        <v>33</v>
+      </c>
+      <c r="D21">
+        <v>29</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>47</v>
+      </c>
+      <c r="H21">
+        <v>38</v>
+      </c>
+      <c r="I21">
+        <v>36</v>
+      </c>
+      <c r="J21">
+        <v>54</v>
+      </c>
+      <c r="K21">
+        <v>36</v>
+      </c>
+      <c r="L21">
+        <v>13</v>
+      </c>
+      <c r="M21">
+        <v>10</v>
+      </c>
+      <c r="N21">
+        <v>35</v>
+      </c>
+      <c r="O21">
+        <v>46</v>
+      </c>
+      <c r="P21">
+        <v>4</v>
+      </c>
+      <c r="Q21">
+        <v>42</v>
+      </c>
+      <c r="R21">
+        <v>32</v>
+      </c>
+      <c r="S21">
+        <v>13</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>41</v>
+      </c>
+      <c r="V21">
+        <v>26</v>
+      </c>
+      <c r="W21">
+        <v>39</v>
+      </c>
+      <c r="X21">
+        <v>42</v>
+      </c>
+      <c r="Y21">
+        <v>27</v>
+      </c>
+      <c r="Z21">
+        <v>16</v>
+      </c>
+      <c r="AA21">
+        <v>7</v>
+      </c>
+      <c r="AB21">
+        <v>46</v>
+      </c>
+      <c r="AC21">
+        <v>33</v>
+      </c>
+      <c r="AD21">
+        <v>24</v>
+      </c>
+      <c r="AE21">
+        <v>44</v>
+      </c>
+      <c r="AG21">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>3</v>
+      </c>
+      <c r="Q22">
+        <v>2</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22">
+        <v>1</v>
+      </c>
+      <c r="AB22">
+        <v>2</v>
+      </c>
+      <c r="AC22">
+        <v>1</v>
+      </c>
+      <c r="AE22">
+        <v>1</v>
+      </c>
+      <c r="AG22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>40</v>
+      </c>
+      <c r="C23">
+        <v>49</v>
+      </c>
+      <c r="D23">
+        <v>39</v>
+      </c>
+      <c r="E23">
+        <v>16</v>
+      </c>
+      <c r="G23">
+        <v>42</v>
+      </c>
+      <c r="H23">
+        <v>43</v>
+      </c>
+      <c r="I23">
+        <v>42</v>
+      </c>
+      <c r="J23">
+        <v>49</v>
+      </c>
+      <c r="K23">
+        <v>30</v>
+      </c>
+      <c r="L23">
+        <v>12</v>
+      </c>
+      <c r="N23">
+        <v>45</v>
+      </c>
+      <c r="O23">
+        <v>51</v>
+      </c>
+      <c r="P23">
+        <v>37</v>
+      </c>
+      <c r="Q23">
+        <v>42</v>
+      </c>
+      <c r="R23">
+        <v>33</v>
+      </c>
+      <c r="S23">
+        <v>17</v>
+      </c>
+      <c r="U23">
+        <v>49</v>
+      </c>
+      <c r="V23">
+        <v>41</v>
+      </c>
+      <c r="W23">
+        <v>50</v>
+      </c>
+      <c r="X23">
+        <v>31</v>
+      </c>
+      <c r="Y23">
+        <v>37</v>
+      </c>
+      <c r="Z23">
+        <v>14</v>
+      </c>
+      <c r="AB23">
+        <v>44</v>
+      </c>
+      <c r="AC23">
+        <v>39</v>
+      </c>
+      <c r="AD23">
+        <v>32</v>
+      </c>
+      <c r="AE23">
+        <v>43</v>
+      </c>
+      <c r="AG23">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <v>5</v>
+      </c>
+      <c r="N24">
+        <v>5</v>
+      </c>
+      <c r="O24">
+        <v>2</v>
+      </c>
+      <c r="P24">
+        <v>8</v>
+      </c>
+      <c r="Q24">
+        <v>4</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="U24">
+        <v>3</v>
+      </c>
+      <c r="V24">
+        <v>2</v>
+      </c>
+      <c r="W24">
+        <v>8</v>
+      </c>
+      <c r="X24">
+        <v>5</v>
+      </c>
+      <c r="Y24">
+        <v>4</v>
+      </c>
+      <c r="AB24">
+        <v>4</v>
+      </c>
+      <c r="AC24">
+        <v>5</v>
+      </c>
+      <c r="AD24">
+        <v>7</v>
+      </c>
+      <c r="AE24">
+        <v>2</v>
+      </c>
+      <c r="AG24">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>69</v>
+      </c>
+      <c r="C25">
+        <v>45</v>
+      </c>
+      <c r="D25">
+        <v>41</v>
+      </c>
+      <c r="E25">
+        <v>35</v>
+      </c>
+      <c r="F25">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>52</v>
+      </c>
+      <c r="H25">
+        <v>34</v>
+      </c>
+      <c r="I25">
+        <v>30</v>
+      </c>
+      <c r="J25">
+        <v>35</v>
+      </c>
+      <c r="K25">
+        <v>40</v>
+      </c>
+      <c r="L25">
+        <v>13</v>
+      </c>
+      <c r="M25">
+        <v>3</v>
+      </c>
+      <c r="N25">
+        <v>41</v>
+      </c>
+      <c r="O25">
+        <v>46</v>
+      </c>
+      <c r="P25">
+        <v>37</v>
+      </c>
+      <c r="Q25">
+        <v>28</v>
+      </c>
+      <c r="R25">
+        <v>36</v>
+      </c>
+      <c r="S25">
+        <v>19</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>33</v>
+      </c>
+      <c r="V25">
+        <v>51</v>
+      </c>
+      <c r="W25">
+        <v>53</v>
+      </c>
+      <c r="X25">
+        <v>40</v>
+      </c>
+      <c r="Y25">
+        <v>45</v>
+      </c>
+      <c r="Z25">
+        <v>20</v>
+      </c>
+      <c r="AA25">
+        <v>2</v>
+      </c>
+      <c r="AB25">
+        <v>42</v>
+      </c>
+      <c r="AC25">
+        <v>43</v>
+      </c>
+      <c r="AD25">
+        <v>35</v>
+      </c>
+      <c r="AE25">
+        <v>35</v>
+      </c>
+      <c r="AG25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>108</v>
+      </c>
+      <c r="C26">
+        <v>109</v>
+      </c>
+      <c r="D26">
+        <v>94</v>
+      </c>
+      <c r="E26">
+        <v>74</v>
+      </c>
+      <c r="F26">
+        <v>11</v>
+      </c>
+      <c r="G26">
+        <v>118</v>
+      </c>
+      <c r="H26">
+        <v>130</v>
+      </c>
+      <c r="I26">
+        <v>107</v>
+      </c>
+      <c r="J26">
+        <v>102</v>
+      </c>
+      <c r="K26">
+        <v>72</v>
+      </c>
+      <c r="L26">
+        <v>57</v>
+      </c>
+      <c r="M26">
+        <v>10</v>
+      </c>
+      <c r="N26">
+        <v>103</v>
+      </c>
+      <c r="O26">
+        <v>106</v>
+      </c>
+      <c r="P26">
+        <v>110</v>
+      </c>
+      <c r="Q26">
+        <v>96</v>
+      </c>
+      <c r="R26">
+        <v>75</v>
+      </c>
+      <c r="S26">
+        <v>61</v>
+      </c>
+      <c r="U26">
+        <v>14</v>
+      </c>
+      <c r="V26">
+        <v>167</v>
+      </c>
+      <c r="W26">
+        <v>145</v>
+      </c>
+      <c r="X26">
+        <v>90</v>
+      </c>
+      <c r="Y26">
+        <v>83</v>
+      </c>
+      <c r="Z26">
+        <v>77</v>
+      </c>
+      <c r="AA26">
+        <v>7</v>
+      </c>
+      <c r="AB26">
+        <v>91</v>
+      </c>
+      <c r="AC26">
+        <v>116</v>
+      </c>
+      <c r="AD26">
+        <v>83</v>
+      </c>
+      <c r="AE26">
+        <v>100</v>
+      </c>
+      <c r="AG26">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>13</v>
+      </c>
+      <c r="D27">
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <v>12</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <v>11</v>
+      </c>
+      <c r="K27">
+        <v>12</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>8</v>
+      </c>
+      <c r="O27">
+        <v>15</v>
+      </c>
+      <c r="P27">
+        <v>13</v>
+      </c>
+      <c r="Q27">
+        <v>11</v>
+      </c>
+      <c r="R27">
+        <v>10</v>
+      </c>
+      <c r="S27">
+        <v>4</v>
+      </c>
+      <c r="U27">
+        <v>10</v>
+      </c>
+      <c r="V27">
+        <v>6</v>
+      </c>
+      <c r="W27">
+        <v>10</v>
+      </c>
+      <c r="X27">
+        <v>15</v>
+      </c>
+      <c r="Y27">
+        <v>9</v>
+      </c>
+      <c r="AB27">
+        <v>11</v>
+      </c>
+      <c r="AC27">
+        <v>14</v>
+      </c>
+      <c r="AD27">
+        <v>10</v>
+      </c>
+      <c r="AE27">
+        <v>8</v>
+      </c>
+      <c r="AG27">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>15</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>12</v>
+      </c>
+      <c r="G29">
+        <v>18</v>
+      </c>
+      <c r="H29">
+        <v>13</v>
+      </c>
+      <c r="I29">
+        <v>12</v>
+      </c>
+      <c r="J29">
+        <v>13</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>6</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>13</v>
+      </c>
+      <c r="O29">
+        <v>13</v>
+      </c>
+      <c r="P29">
+        <v>9</v>
+      </c>
+      <c r="Q29">
+        <v>10</v>
+      </c>
+      <c r="S29">
+        <v>6</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <v>19</v>
+      </c>
+      <c r="V29">
+        <v>14</v>
+      </c>
+      <c r="W29">
+        <v>10</v>
+      </c>
+      <c r="X29">
+        <v>14</v>
+      </c>
+      <c r="Z29">
+        <v>10</v>
+      </c>
+      <c r="AA29">
+        <v>2</v>
+      </c>
+      <c r="AB29">
+        <v>16</v>
+      </c>
+      <c r="AC29">
+        <v>13</v>
+      </c>
+      <c r="AD29">
+        <v>17</v>
+      </c>
+      <c r="AE29">
+        <v>13</v>
+      </c>
+      <c r="AG29">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>6</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="J30">
+        <v>6</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>3</v>
+      </c>
+      <c r="N30">
+        <v>4</v>
+      </c>
+      <c r="O30">
+        <v>2</v>
+      </c>
+      <c r="P30">
+        <v>9</v>
+      </c>
+      <c r="Q30">
+        <v>4</v>
+      </c>
+      <c r="R30">
+        <v>6</v>
+      </c>
+      <c r="S30">
+        <v>3</v>
+      </c>
+      <c r="U30">
+        <v>3</v>
+      </c>
+      <c r="V30">
+        <v>7</v>
+      </c>
+      <c r="W30">
+        <v>5</v>
+      </c>
+      <c r="X30">
+        <v>4</v>
+      </c>
+      <c r="Y30">
+        <v>11</v>
+      </c>
+      <c r="Z30">
+        <v>2</v>
+      </c>
+      <c r="AB30">
+        <v>9</v>
+      </c>
+      <c r="AC30">
+        <v>2</v>
+      </c>
+      <c r="AD30">
+        <v>8</v>
+      </c>
+      <c r="AE30">
+        <v>5</v>
+      </c>
+      <c r="AG30">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>34</v>
+      </c>
+      <c r="C31">
+        <v>37</v>
+      </c>
+      <c r="D31">
+        <v>22</v>
+      </c>
+      <c r="E31">
+        <v>13</v>
+      </c>
+      <c r="G31">
+        <v>33</v>
+      </c>
+      <c r="H31">
+        <v>39</v>
+      </c>
+      <c r="I31">
+        <v>31</v>
+      </c>
+      <c r="J31">
+        <v>33</v>
+      </c>
+      <c r="K31">
+        <v>25</v>
+      </c>
+      <c r="L31">
+        <v>8</v>
+      </c>
+      <c r="N31">
+        <v>24</v>
+      </c>
+      <c r="O31">
+        <v>31</v>
+      </c>
+      <c r="P31">
+        <v>33</v>
+      </c>
+      <c r="Q31">
+        <v>39</v>
+      </c>
+      <c r="R31">
+        <v>21</v>
+      </c>
+      <c r="S31">
+        <v>6</v>
+      </c>
+      <c r="T31">
+        <v>1</v>
+      </c>
+      <c r="U31">
+        <v>24</v>
+      </c>
+      <c r="V31">
+        <v>33</v>
+      </c>
+      <c r="W31">
+        <v>25</v>
+      </c>
+      <c r="X31">
+        <v>25</v>
+      </c>
+      <c r="Y31">
+        <v>16</v>
+      </c>
+      <c r="Z31">
+        <v>5</v>
+      </c>
+      <c r="AA31">
+        <v>3</v>
+      </c>
+      <c r="AB31">
+        <v>25</v>
+      </c>
+      <c r="AC31">
+        <v>16</v>
+      </c>
+      <c r="AD31">
+        <v>25</v>
+      </c>
+      <c r="AE31">
+        <v>29</v>
+      </c>
+      <c r="AG31">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>3</v>
+      </c>
+      <c r="Q32">
+        <v>6</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+      <c r="V32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>3</v>
+      </c>
+      <c r="X32">
+        <v>5</v>
+      </c>
+      <c r="Y32">
+        <v>1</v>
+      </c>
+      <c r="AB32">
+        <v>2</v>
+      </c>
+      <c r="AC32">
+        <v>1</v>
+      </c>
+      <c r="AD32">
+        <v>4</v>
+      </c>
+      <c r="AG32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>14</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>17</v>
+      </c>
+      <c r="I33">
+        <v>7</v>
+      </c>
+      <c r="J33">
+        <v>20</v>
+      </c>
+      <c r="K33">
+        <v>13</v>
+      </c>
+      <c r="L33">
+        <v>5</v>
+      </c>
+      <c r="O33">
+        <v>13</v>
+      </c>
+      <c r="P33">
+        <v>5</v>
+      </c>
+      <c r="Q33">
+        <v>6</v>
+      </c>
+      <c r="R33">
+        <v>8</v>
+      </c>
+      <c r="V33">
+        <v>15</v>
+      </c>
+      <c r="W33">
+        <v>3</v>
+      </c>
+      <c r="X33">
+        <v>7</v>
+      </c>
+      <c r="Y33">
+        <v>7</v>
+      </c>
+      <c r="AA33">
+        <v>1</v>
+      </c>
+      <c r="AB33">
+        <v>1</v>
+      </c>
+      <c r="AC33">
+        <v>14</v>
+      </c>
+      <c r="AD33">
+        <v>3</v>
+      </c>
+      <c r="AE33">
+        <v>7</v>
+      </c>
+      <c r="AG33">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34">
+        <v>46</v>
+      </c>
+      <c r="C34">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>24</v>
+      </c>
+      <c r="E34">
+        <v>22</v>
+      </c>
+      <c r="G34">
+        <v>46</v>
+      </c>
+      <c r="H34">
+        <v>47</v>
+      </c>
+      <c r="I34">
+        <v>41</v>
+      </c>
+      <c r="J34">
+        <v>25</v>
+      </c>
+      <c r="K34">
+        <v>42</v>
+      </c>
+      <c r="L34">
+        <v>16</v>
+      </c>
+      <c r="M34">
+        <v>2</v>
+      </c>
+      <c r="N34">
+        <v>42</v>
+      </c>
+      <c r="O34">
+        <v>54</v>
+      </c>
+      <c r="P34">
+        <v>39</v>
+      </c>
+      <c r="Q34">
+        <v>30</v>
+      </c>
+      <c r="R34">
+        <v>35</v>
+      </c>
+      <c r="S34">
+        <v>12</v>
+      </c>
+      <c r="U34">
+        <v>40</v>
+      </c>
+      <c r="V34">
+        <v>33</v>
+      </c>
+      <c r="W34">
+        <v>36</v>
+      </c>
+      <c r="X34">
+        <v>26</v>
+      </c>
+      <c r="Y34">
+        <v>36</v>
+      </c>
+      <c r="Z34">
+        <v>14</v>
+      </c>
+      <c r="AB34">
+        <v>37</v>
+      </c>
+      <c r="AC34">
+        <v>38</v>
+      </c>
+      <c r="AD34">
+        <v>53</v>
+      </c>
+      <c r="AE34">
+        <v>34</v>
+      </c>
+      <c r="AG34">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>32</v>
+      </c>
+      <c r="C35">
+        <v>33</v>
+      </c>
+      <c r="D35">
+        <v>19</v>
+      </c>
+      <c r="E35">
+        <v>13</v>
+      </c>
+      <c r="G35">
+        <v>31</v>
+      </c>
+      <c r="H35">
+        <v>36</v>
+      </c>
+      <c r="I35">
+        <v>36</v>
+      </c>
+      <c r="J35">
+        <v>19</v>
+      </c>
+      <c r="K35">
+        <v>22</v>
+      </c>
+      <c r="L35">
+        <v>5</v>
+      </c>
+      <c r="M35">
+        <v>4</v>
+      </c>
+      <c r="N35">
+        <v>31</v>
+      </c>
+      <c r="O35">
+        <v>34</v>
+      </c>
+      <c r="P35">
+        <v>34</v>
+      </c>
+      <c r="Q35">
+        <v>14</v>
+      </c>
+      <c r="R35">
+        <v>35</v>
+      </c>
+      <c r="S35">
+        <v>16</v>
+      </c>
+      <c r="T35">
+        <v>1</v>
+      </c>
+      <c r="U35">
+        <v>2</v>
+      </c>
+      <c r="V35">
+        <v>60</v>
+      </c>
+      <c r="W35">
+        <v>37</v>
+      </c>
+      <c r="X35">
+        <v>27</v>
+      </c>
+      <c r="Y35">
+        <v>26</v>
+      </c>
+      <c r="Z35">
+        <v>9</v>
+      </c>
+      <c r="AA35">
+        <v>2</v>
+      </c>
+      <c r="AB35">
+        <v>38</v>
+      </c>
+      <c r="AC35">
+        <v>40</v>
+      </c>
+      <c r="AD35">
+        <v>32</v>
+      </c>
+      <c r="AE35">
+        <v>50</v>
+      </c>
+      <c r="AG35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36">
+        <v>14</v>
+      </c>
+      <c r="C36">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>24</v>
+      </c>
+      <c r="E36">
+        <v>10</v>
+      </c>
+      <c r="G36">
+        <v>27</v>
+      </c>
+      <c r="H36">
+        <v>22</v>
+      </c>
+      <c r="I36">
+        <v>20</v>
+      </c>
+      <c r="J36">
+        <v>20</v>
+      </c>
+      <c r="K36">
+        <v>16</v>
+      </c>
+      <c r="L36">
+        <v>9</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>26</v>
+      </c>
+      <c r="O36">
+        <v>21</v>
+      </c>
+      <c r="P36">
+        <v>20</v>
+      </c>
+      <c r="Q36">
+        <v>13</v>
+      </c>
+      <c r="R36">
+        <v>18</v>
+      </c>
+      <c r="S36">
+        <v>5</v>
+      </c>
+      <c r="U36">
+        <v>12</v>
+      </c>
+      <c r="V36">
+        <v>20</v>
+      </c>
+      <c r="W36">
+        <v>14</v>
+      </c>
+      <c r="X36">
+        <v>14</v>
+      </c>
+      <c r="Y36">
+        <v>19</v>
+      </c>
+      <c r="Z36">
+        <v>7</v>
+      </c>
+      <c r="AB36">
+        <v>17</v>
+      </c>
+      <c r="AC36">
+        <v>16</v>
+      </c>
+      <c r="AD36">
+        <v>14</v>
+      </c>
+      <c r="AE36">
+        <v>30</v>
+      </c>
+      <c r="AG36">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <v>103</v>
+      </c>
+      <c r="C37">
+        <v>119</v>
+      </c>
+      <c r="D37">
+        <v>87</v>
+      </c>
+      <c r="E37">
+        <v>34</v>
+      </c>
+      <c r="G37">
+        <v>110</v>
+      </c>
+      <c r="H37">
+        <v>105</v>
+      </c>
+      <c r="I37">
+        <v>84</v>
+      </c>
+      <c r="J37">
+        <v>101</v>
+      </c>
+      <c r="K37">
+        <v>87</v>
+      </c>
+      <c r="L37">
+        <v>41</v>
+      </c>
+      <c r="M37">
+        <v>2</v>
+      </c>
+      <c r="N37">
+        <v>98</v>
+      </c>
+      <c r="O37">
+        <v>87</v>
+      </c>
+      <c r="P37">
+        <v>84</v>
+      </c>
+      <c r="Q37">
+        <v>100</v>
+      </c>
+      <c r="R37">
+        <v>62</v>
+      </c>
+      <c r="S37">
+        <v>27</v>
+      </c>
+      <c r="T37">
+        <v>4</v>
+      </c>
+      <c r="U37">
+        <v>104</v>
+      </c>
+      <c r="V37">
+        <v>121</v>
+      </c>
+      <c r="W37">
+        <v>81</v>
+      </c>
+      <c r="X37">
+        <v>95</v>
+      </c>
+      <c r="Y37">
+        <v>78</v>
+      </c>
+      <c r="Z37">
+        <v>28</v>
+      </c>
+      <c r="AA37">
+        <v>2</v>
+      </c>
+      <c r="AB37">
+        <v>116</v>
+      </c>
+      <c r="AC37">
+        <v>102</v>
+      </c>
+      <c r="AD37">
+        <v>84</v>
+      </c>
+      <c r="AE37">
+        <v>85</v>
+      </c>
+      <c r="AG37">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38">
+        <v>16</v>
+      </c>
+      <c r="C38">
+        <v>20</v>
+      </c>
+      <c r="D38">
+        <v>23</v>
+      </c>
+      <c r="E38">
+        <v>9</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>15</v>
+      </c>
+      <c r="H38">
+        <v>15</v>
+      </c>
+      <c r="I38">
+        <v>21</v>
+      </c>
+      <c r="J38">
+        <v>22</v>
+      </c>
+      <c r="K38">
+        <v>11</v>
+      </c>
+      <c r="L38">
+        <v>8</v>
+      </c>
+      <c r="N38">
+        <v>15</v>
+      </c>
+      <c r="O38">
+        <v>14</v>
+      </c>
+      <c r="P38">
+        <v>16</v>
+      </c>
+      <c r="Q38">
+        <v>19</v>
+      </c>
+      <c r="R38">
+        <v>17</v>
+      </c>
+      <c r="S38">
+        <v>3</v>
+      </c>
+      <c r="U38">
+        <v>17</v>
+      </c>
+      <c r="V38">
+        <v>33</v>
+      </c>
+      <c r="W38">
+        <v>23</v>
+      </c>
+      <c r="X38">
+        <v>20</v>
+      </c>
+      <c r="Y38">
+        <v>13</v>
+      </c>
+      <c r="Z38">
+        <v>11</v>
+      </c>
+      <c r="AA38">
+        <v>1</v>
+      </c>
+      <c r="AB38">
+        <v>15</v>
+      </c>
+      <c r="AC38">
+        <v>12</v>
+      </c>
+      <c r="AD38">
+        <v>7</v>
+      </c>
+      <c r="AE38">
+        <v>26</v>
+      </c>
+      <c r="AG38">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>46</v>
+      </c>
+      <c r="C39">
+        <v>68</v>
+      </c>
+      <c r="D39">
+        <v>43</v>
+      </c>
+      <c r="E39">
+        <v>9</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>46</v>
+      </c>
+      <c r="H39">
+        <v>48</v>
+      </c>
+      <c r="I39">
+        <v>52</v>
+      </c>
+      <c r="J39">
+        <v>43</v>
+      </c>
+      <c r="K39">
+        <v>33</v>
+      </c>
+      <c r="L39">
+        <v>26</v>
+      </c>
+      <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="N39">
+        <v>83</v>
+      </c>
+      <c r="O39">
+        <v>63</v>
+      </c>
+      <c r="P39">
+        <v>64</v>
+      </c>
+      <c r="Q39">
+        <v>70</v>
+      </c>
+      <c r="R39">
+        <v>49</v>
+      </c>
+      <c r="S39">
+        <v>26</v>
+      </c>
+      <c r="T39">
+        <v>1</v>
+      </c>
+      <c r="U39">
+        <v>2</v>
+      </c>
+      <c r="V39">
+        <v>93</v>
+      </c>
+      <c r="W39">
+        <v>65</v>
+      </c>
+      <c r="X39">
+        <v>71</v>
+      </c>
+      <c r="Y39">
+        <v>45</v>
+      </c>
+      <c r="Z39">
+        <v>29</v>
+      </c>
+      <c r="AA39">
+        <v>1</v>
+      </c>
+      <c r="AB39">
+        <v>54</v>
+      </c>
+      <c r="AC39">
+        <v>61</v>
+      </c>
+      <c r="AD39">
+        <v>57</v>
+      </c>
+      <c r="AE39">
+        <v>66</v>
+      </c>
+      <c r="AG39">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40">
+        <v>18</v>
+      </c>
+      <c r="H40">
+        <v>12</v>
+      </c>
+      <c r="J40">
+        <v>19</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>9</v>
+      </c>
+      <c r="Q40">
+        <v>18</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
+      <c r="V40">
+        <v>14</v>
+      </c>
+      <c r="X40">
+        <v>13</v>
+      </c>
+      <c r="Y40">
+        <v>1</v>
+      </c>
+      <c r="Z40">
+        <v>1</v>
+      </c>
+      <c r="AC40">
+        <v>11</v>
+      </c>
+      <c r="AE40">
+        <v>21</v>
+      </c>
+      <c r="AG40">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>7</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>12</v>
+      </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41">
+        <v>7</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="P41">
+        <v>2</v>
+      </c>
+      <c r="Q41">
+        <v>2</v>
+      </c>
+      <c r="R41">
+        <v>6</v>
+      </c>
+      <c r="V41">
+        <v>3</v>
+      </c>
+      <c r="W41">
+        <v>3</v>
+      </c>
+      <c r="Y41">
+        <v>1</v>
+      </c>
+      <c r="Z41">
+        <v>2</v>
+      </c>
+      <c r="AC41">
+        <v>4</v>
+      </c>
+      <c r="AD41">
+        <v>3</v>
+      </c>
+      <c r="AE41">
+        <v>2</v>
+      </c>
+      <c r="AG41">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB42">
+        <v>1</v>
+      </c>
+      <c r="AG42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47">
+        <v>14</v>
+      </c>
+      <c r="C47">
+        <v>12</v>
+      </c>
+      <c r="D47">
+        <v>10</v>
+      </c>
+      <c r="E47">
+        <v>11</v>
+      </c>
+      <c r="G47">
+        <v>12</v>
+      </c>
+      <c r="I47">
+        <v>12</v>
+      </c>
+      <c r="J47">
+        <v>11</v>
+      </c>
+      <c r="K47">
+        <v>10</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>10</v>
+      </c>
+      <c r="P47">
+        <v>7</v>
+      </c>
+      <c r="Q47">
+        <v>5</v>
+      </c>
+      <c r="R47">
+        <v>9</v>
+      </c>
+      <c r="S47">
+        <v>2</v>
+      </c>
+      <c r="U47">
+        <v>9</v>
+      </c>
+      <c r="W47">
+        <v>14</v>
+      </c>
+      <c r="X47">
+        <v>9</v>
+      </c>
+      <c r="Y47">
+        <v>10</v>
+      </c>
+      <c r="Z47">
+        <v>2</v>
+      </c>
+      <c r="AB47">
+        <v>11</v>
+      </c>
+      <c r="AD47">
+        <v>10</v>
+      </c>
+      <c r="AE47">
+        <v>5</v>
+      </c>
+      <c r="AG47">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48">
+        <v>22</v>
+      </c>
+      <c r="C48">
+        <v>16</v>
+      </c>
+      <c r="D48">
+        <v>23</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>22</v>
+      </c>
+      <c r="H48">
+        <v>34</v>
+      </c>
+      <c r="I48">
+        <v>12</v>
+      </c>
+      <c r="J48">
+        <v>23</v>
+      </c>
+      <c r="K48">
+        <v>23</v>
+      </c>
+      <c r="L48">
+        <v>5</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>44</v>
+      </c>
+      <c r="O48">
+        <v>15</v>
+      </c>
+      <c r="P48">
+        <v>22</v>
+      </c>
+      <c r="Q48">
+        <v>23</v>
+      </c>
+      <c r="R48">
+        <v>17</v>
+      </c>
+      <c r="S48">
+        <v>6</v>
+      </c>
+      <c r="T48">
+        <v>1</v>
+      </c>
+      <c r="U48">
+        <v>18</v>
+      </c>
+      <c r="V48">
+        <v>29</v>
+      </c>
+      <c r="W48">
+        <v>21</v>
+      </c>
+      <c r="X48">
+        <v>29</v>
+      </c>
+      <c r="Y48">
+        <v>26</v>
+      </c>
+      <c r="Z48">
+        <v>6</v>
+      </c>
+      <c r="AB48">
+        <v>20</v>
+      </c>
+      <c r="AC48">
+        <v>23</v>
+      </c>
+      <c r="AD48">
+        <v>11</v>
+      </c>
+      <c r="AE48">
+        <v>19</v>
+      </c>
+      <c r="AG48">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49">
+        <v>35</v>
+      </c>
+      <c r="C49">
+        <v>42</v>
+      </c>
+      <c r="D49">
+        <v>40</v>
+      </c>
+      <c r="E49">
+        <v>19</v>
+      </c>
+      <c r="G49">
+        <v>27</v>
+      </c>
+      <c r="H49">
+        <v>44</v>
+      </c>
+      <c r="I49">
+        <v>36</v>
+      </c>
+      <c r="J49">
+        <v>32</v>
+      </c>
+      <c r="K49">
+        <v>26</v>
+      </c>
+      <c r="L49">
+        <v>9</v>
+      </c>
+      <c r="N49">
+        <v>42</v>
+      </c>
+      <c r="O49">
+        <v>35</v>
+      </c>
+      <c r="P49">
+        <v>36</v>
+      </c>
+      <c r="Q49">
+        <v>36</v>
+      </c>
+      <c r="R49">
+        <v>38</v>
+      </c>
+      <c r="S49">
+        <v>13</v>
+      </c>
+      <c r="U49">
+        <v>28</v>
+      </c>
+      <c r="V49">
+        <v>41</v>
+      </c>
+      <c r="W49">
+        <v>32</v>
+      </c>
+      <c r="X49">
+        <v>52</v>
+      </c>
+      <c r="Y49">
+        <v>43</v>
+      </c>
+      <c r="Z49">
+        <v>9</v>
+      </c>
+      <c r="AA49">
+        <v>2</v>
+      </c>
+      <c r="AB49">
+        <v>27</v>
+      </c>
+      <c r="AC49">
+        <v>41</v>
+      </c>
+      <c r="AD49">
+        <v>28</v>
+      </c>
+      <c r="AE49">
+        <v>35</v>
+      </c>
+      <c r="AG49">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50">
+        <v>46</v>
+      </c>
+      <c r="C50">
+        <v>33</v>
+      </c>
+      <c r="D50">
+        <v>26</v>
+      </c>
+      <c r="E50">
+        <v>14</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>46</v>
+      </c>
+      <c r="H50">
+        <v>47</v>
+      </c>
+      <c r="I50">
+        <v>33</v>
+      </c>
+      <c r="J50">
+        <v>30</v>
+      </c>
+      <c r="K50">
+        <v>18</v>
+      </c>
+      <c r="L50">
+        <v>17</v>
+      </c>
+      <c r="N50">
+        <v>40</v>
+      </c>
+      <c r="O50">
+        <v>36</v>
+      </c>
+      <c r="P50">
+        <v>34</v>
+      </c>
+      <c r="Q50">
+        <v>31</v>
+      </c>
+      <c r="R50">
+        <v>25</v>
+      </c>
+      <c r="S50">
+        <v>15</v>
+      </c>
+      <c r="U50">
+        <v>38</v>
+      </c>
+      <c r="V50">
+        <v>41</v>
+      </c>
+      <c r="W50">
+        <v>36</v>
+      </c>
+      <c r="X50">
+        <v>24</v>
+      </c>
+      <c r="Y50">
+        <v>26</v>
+      </c>
+      <c r="Z50">
+        <v>14</v>
+      </c>
+      <c r="AB50">
+        <v>34</v>
+      </c>
+      <c r="AC50">
+        <v>34</v>
+      </c>
+      <c r="AD50">
+        <v>37</v>
+      </c>
+      <c r="AE50">
+        <v>40</v>
+      </c>
+      <c r="AG50">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51">
+        <v>28</v>
+      </c>
+      <c r="C51">
+        <v>23</v>
+      </c>
+      <c r="D51">
+        <v>18</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>24</v>
+      </c>
+      <c r="H51">
+        <v>31</v>
+      </c>
+      <c r="I51">
+        <v>25</v>
+      </c>
+      <c r="J51">
+        <v>15</v>
+      </c>
+      <c r="K51">
+        <v>6</v>
+      </c>
+      <c r="L51">
+        <v>35</v>
+      </c>
+      <c r="N51">
+        <v>25</v>
+      </c>
+      <c r="O51">
+        <v>31</v>
+      </c>
+      <c r="P51">
+        <v>17</v>
+      </c>
+      <c r="Q51">
+        <v>21</v>
+      </c>
+      <c r="R51">
+        <v>18</v>
+      </c>
+      <c r="S51">
+        <v>5</v>
+      </c>
+      <c r="U51">
+        <v>21</v>
+      </c>
+      <c r="V51">
+        <v>21</v>
+      </c>
+      <c r="W51">
+        <v>24</v>
+      </c>
+      <c r="X51">
+        <v>44</v>
+      </c>
+      <c r="Y51">
+        <v>22</v>
+      </c>
+      <c r="Z51">
+        <v>7</v>
+      </c>
+      <c r="AB51">
+        <v>17</v>
+      </c>
+      <c r="AC51">
+        <v>31</v>
+      </c>
+      <c r="AD51">
+        <v>21</v>
+      </c>
+      <c r="AE51">
+        <v>34</v>
+      </c>
+      <c r="AG51">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52">
+        <v>69</v>
+      </c>
+      <c r="C52">
+        <v>54</v>
+      </c>
+      <c r="D52">
+        <v>58</v>
+      </c>
+      <c r="E52">
+        <v>24</v>
+      </c>
+      <c r="F52">
+        <v>19</v>
+      </c>
+      <c r="G52">
+        <v>73</v>
+      </c>
+      <c r="H52">
+        <v>47</v>
+      </c>
+      <c r="I52">
+        <v>53</v>
+      </c>
+      <c r="J52">
+        <v>75</v>
+      </c>
+      <c r="K52">
+        <v>47</v>
+      </c>
+      <c r="L52">
+        <v>21</v>
+      </c>
+      <c r="M52">
+        <v>9</v>
+      </c>
+      <c r="N52">
+        <v>66</v>
+      </c>
+      <c r="O52">
+        <v>66</v>
+      </c>
+      <c r="P52">
+        <v>66</v>
+      </c>
+      <c r="Q52">
+        <v>76</v>
+      </c>
+      <c r="R52">
+        <v>50</v>
+      </c>
+      <c r="S52">
+        <v>20</v>
+      </c>
+      <c r="T52">
+        <v>14</v>
+      </c>
+      <c r="U52">
+        <v>53</v>
+      </c>
+      <c r="V52">
+        <v>47</v>
+      </c>
+      <c r="W52">
+        <v>51</v>
+      </c>
+      <c r="X52">
+        <v>81</v>
+      </c>
+      <c r="Y52">
+        <v>42</v>
+      </c>
+      <c r="Z52">
+        <v>30</v>
+      </c>
+      <c r="AA52">
+        <v>11</v>
+      </c>
+      <c r="AB52">
+        <v>43</v>
+      </c>
+      <c r="AC52">
+        <v>49</v>
+      </c>
+      <c r="AD52">
+        <v>51</v>
+      </c>
+      <c r="AE52">
+        <v>66</v>
+      </c>
+      <c r="AG52">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53">
+        <v>12</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+      <c r="D53">
+        <v>12</v>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+      <c r="G53">
+        <v>4</v>
+      </c>
+      <c r="H53">
+        <v>6</v>
+      </c>
+      <c r="I53">
+        <v>6</v>
+      </c>
+      <c r="J53">
+        <v>3</v>
+      </c>
+      <c r="K53">
+        <v>9</v>
+      </c>
+      <c r="L53">
+        <v>5</v>
+      </c>
+      <c r="N53">
+        <v>8</v>
+      </c>
+      <c r="O53">
+        <v>7</v>
+      </c>
+      <c r="P53">
+        <v>11</v>
+      </c>
+      <c r="Q53">
+        <v>4</v>
+      </c>
+      <c r="R53">
+        <v>11</v>
+      </c>
+      <c r="S53">
+        <v>4</v>
+      </c>
+      <c r="U53">
+        <v>7</v>
+      </c>
+      <c r="V53">
+        <v>7</v>
+      </c>
+      <c r="W53">
+        <v>10</v>
+      </c>
+      <c r="X53">
+        <v>4</v>
+      </c>
+      <c r="Y53">
+        <v>5</v>
+      </c>
+      <c r="Z53">
+        <v>3</v>
+      </c>
+      <c r="AA53">
+        <v>1</v>
+      </c>
+      <c r="AB53">
+        <v>8</v>
+      </c>
+      <c r="AC53">
+        <v>5</v>
+      </c>
+      <c r="AD53">
+        <v>8</v>
+      </c>
+      <c r="AE53">
+        <v>5</v>
+      </c>
+      <c r="AG53">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>18</v>
+      </c>
+      <c r="D54">
+        <v>19</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="G54">
+        <v>26</v>
+      </c>
+      <c r="H54">
+        <v>24</v>
+      </c>
+      <c r="I54">
+        <v>47</v>
+      </c>
+      <c r="J54">
+        <v>11</v>
+      </c>
+      <c r="K54">
+        <v>22</v>
+      </c>
+      <c r="L54">
+        <v>7</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>20</v>
+      </c>
+      <c r="O54">
+        <v>17</v>
+      </c>
+      <c r="P54">
+        <v>46</v>
+      </c>
+      <c r="Q54">
+        <v>17</v>
+      </c>
+      <c r="R54">
+        <v>23</v>
+      </c>
+      <c r="S54">
+        <v>5</v>
+      </c>
+      <c r="T54">
+        <v>1</v>
+      </c>
+      <c r="U54">
+        <v>21</v>
+      </c>
+      <c r="V54">
+        <v>14</v>
+      </c>
+      <c r="W54">
+        <v>36</v>
+      </c>
+      <c r="X54">
+        <v>18</v>
+      </c>
+      <c r="Y54">
+        <v>28</v>
+      </c>
+      <c r="Z54">
+        <v>4</v>
+      </c>
+      <c r="AB54">
+        <v>24</v>
+      </c>
+      <c r="AC54">
+        <v>25</v>
+      </c>
+      <c r="AD54">
+        <v>30</v>
+      </c>
+      <c r="AE54">
+        <v>12</v>
+      </c>
+      <c r="AG54">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>5</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+      <c r="H55">
+        <v>5</v>
+      </c>
+      <c r="I55">
+        <v>12</v>
+      </c>
+      <c r="J55">
+        <v>2</v>
+      </c>
+      <c r="K55">
+        <v>2</v>
+      </c>
+      <c r="L55">
+        <v>2</v>
+      </c>
+      <c r="N55">
+        <v>5</v>
+      </c>
+      <c r="O55">
+        <v>5</v>
+      </c>
+      <c r="P55">
+        <v>8</v>
+      </c>
+      <c r="Q55">
+        <v>3</v>
+      </c>
+      <c r="R55">
+        <v>6</v>
+      </c>
+      <c r="S55">
+        <v>2</v>
+      </c>
+      <c r="U55">
+        <v>2</v>
+      </c>
+      <c r="V55">
+        <v>3</v>
+      </c>
+      <c r="W55">
+        <v>9</v>
+      </c>
+      <c r="X55">
+        <v>1</v>
+      </c>
+      <c r="Y55">
+        <v>7</v>
+      </c>
+      <c r="AB55">
+        <v>5</v>
+      </c>
+      <c r="AC55">
+        <v>3</v>
+      </c>
+      <c r="AD55">
+        <v>9</v>
+      </c>
+      <c r="AE55">
+        <v>1</v>
+      </c>
+      <c r="AG55">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56">
+        <v>7</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>5</v>
+      </c>
+      <c r="G56">
+        <v>13</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>9</v>
+      </c>
+      <c r="J56">
+        <v>2</v>
+      </c>
+      <c r="K56">
+        <v>2</v>
+      </c>
+      <c r="L56">
+        <v>4</v>
+      </c>
+      <c r="M56">
+        <v>2</v>
+      </c>
+      <c r="N56">
+        <v>6</v>
+      </c>
+      <c r="O56">
+        <v>3</v>
+      </c>
+      <c r="P56">
+        <v>7</v>
+      </c>
+      <c r="S56">
+        <v>4</v>
+      </c>
+      <c r="U56">
+        <v>5</v>
+      </c>
+      <c r="V56">
+        <v>4</v>
+      </c>
+      <c r="W56">
+        <v>6</v>
+      </c>
+      <c r="Z56">
+        <v>2</v>
+      </c>
+      <c r="AB56">
+        <v>10</v>
+      </c>
+      <c r="AC56">
+        <v>3</v>
+      </c>
+      <c r="AD56">
+        <v>5</v>
+      </c>
+      <c r="AE56">
+        <v>1</v>
+      </c>
+      <c r="AG56">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57">
+        <v>6</v>
+      </c>
+      <c r="C57">
+        <v>11</v>
+      </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>13</v>
+      </c>
+      <c r="H57">
+        <v>10</v>
+      </c>
+      <c r="I57">
+        <v>8</v>
+      </c>
+      <c r="J57">
+        <v>11</v>
+      </c>
+      <c r="K57">
+        <v>11</v>
+      </c>
+      <c r="N57">
+        <v>8</v>
+      </c>
+      <c r="O57">
+        <v>4</v>
+      </c>
+      <c r="P57">
+        <v>9</v>
+      </c>
+      <c r="Q57">
+        <v>3</v>
+      </c>
+      <c r="R57">
+        <v>4</v>
+      </c>
+      <c r="S57">
+        <v>3</v>
+      </c>
+      <c r="U57">
+        <v>11</v>
+      </c>
+      <c r="V57">
+        <v>4</v>
+      </c>
+      <c r="W57">
+        <v>6</v>
+      </c>
+      <c r="X57">
+        <v>4</v>
+      </c>
+      <c r="Y57">
+        <v>10</v>
+      </c>
+      <c r="Z57">
+        <v>6</v>
+      </c>
+      <c r="AA57">
+        <v>1</v>
+      </c>
+      <c r="AB57">
+        <v>7</v>
+      </c>
+      <c r="AC57">
+        <v>6</v>
+      </c>
+      <c r="AD57">
+        <v>4</v>
+      </c>
+      <c r="AE57">
+        <v>11</v>
+      </c>
+      <c r="AG57">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates for November 2022
</commit_message>
<xml_diff>
--- a/statistics_files/2022/2022.d.monthly_circ_by_borrower.unique_borrowers.xlsx
+++ b/statistics_files/2022/2022.d.monthly_circ_by_borrower.unique_borrowers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1A9F66-5C1A-42C3-9667-C1D87F062C5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC54789-C9F6-4901-A93B-E8B2C27BEA5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="719" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="719" activeTab="10" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="78">
   <si>
     <t>branchname</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>2022-10-01 - 2022-10-30</t>
+  </si>
+  <si>
+    <t>2022-11-01 - 2022-11-30</t>
   </si>
 </sst>
 </file>
@@ -645,7 +648,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -9573,9 +9576,9 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E281BB9B-3635-450C-9750-AAA8261D8A1F}">
   <sheetPr codeName="Sheet22"/>
-  <dimension ref="B2:AF2"/>
+  <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -9588,38 +9591,4322 @@
     <col min="2" max="33" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44866</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44867</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44868</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44869</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44870</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44871</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44872</v>
+      </c>
+      <c r="I2" s="1">
+        <v>44873</v>
+      </c>
+      <c r="J2" s="1">
+        <v>44874</v>
+      </c>
+      <c r="K2" s="1">
+        <v>44875</v>
+      </c>
+      <c r="L2" s="1">
+        <v>44876</v>
+      </c>
+      <c r="M2" s="1">
+        <v>44877</v>
+      </c>
+      <c r="N2" s="1">
+        <v>44878</v>
+      </c>
+      <c r="O2" s="1">
+        <v>44879</v>
+      </c>
+      <c r="P2" s="1">
+        <v>44880</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>44881</v>
+      </c>
+      <c r="R2" s="1">
+        <v>44882</v>
+      </c>
+      <c r="S2" s="1">
+        <v>44883</v>
+      </c>
+      <c r="T2" s="1">
+        <v>44884</v>
+      </c>
+      <c r="U2" s="1">
+        <v>44885</v>
+      </c>
+      <c r="V2" s="1">
+        <v>44886</v>
+      </c>
+      <c r="W2" s="1">
+        <v>44887</v>
+      </c>
+      <c r="X2" s="1">
+        <v>44888</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>44889</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>44890</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>44891</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>44892</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>44893</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>44894</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>44895</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>53</v>
+      </c>
+      <c r="C4">
+        <v>64</v>
+      </c>
+      <c r="D4">
+        <v>66</v>
+      </c>
+      <c r="E4">
+        <v>41</v>
+      </c>
+      <c r="F4">
+        <v>33</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>64</v>
+      </c>
+      <c r="I4">
+        <v>71</v>
+      </c>
+      <c r="J4">
+        <v>54</v>
+      </c>
+      <c r="K4">
+        <v>64</v>
+      </c>
+      <c r="L4">
+        <v>53</v>
+      </c>
+      <c r="M4">
+        <v>36</v>
+      </c>
+      <c r="N4">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>72</v>
+      </c>
+      <c r="P4">
+        <v>55</v>
+      </c>
+      <c r="Q4">
+        <v>46</v>
+      </c>
+      <c r="R4">
+        <v>68</v>
+      </c>
+      <c r="S4">
+        <v>70</v>
+      </c>
+      <c r="T4">
+        <v>29</v>
+      </c>
+      <c r="U4">
+        <v>3</v>
+      </c>
+      <c r="V4">
+        <v>82</v>
+      </c>
+      <c r="W4">
+        <v>49</v>
+      </c>
+      <c r="X4">
+        <v>45</v>
+      </c>
+      <c r="Y4">
+        <v>3</v>
+      </c>
+      <c r="Z4">
+        <v>3</v>
+      </c>
+      <c r="AA4">
+        <v>37</v>
+      </c>
+      <c r="AB4">
+        <v>5</v>
+      </c>
+      <c r="AC4">
+        <v>93</v>
+      </c>
+      <c r="AD4">
+        <v>56</v>
+      </c>
+      <c r="AE4">
+        <v>59</v>
+      </c>
+      <c r="AG4">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <v>43</v>
+      </c>
+      <c r="D5">
+        <v>31</v>
+      </c>
+      <c r="E5">
+        <v>31</v>
+      </c>
+      <c r="F5">
+        <v>24</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>43</v>
+      </c>
+      <c r="I5">
+        <v>32</v>
+      </c>
+      <c r="J5">
+        <v>17</v>
+      </c>
+      <c r="K5">
+        <v>34</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>24</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>47</v>
+      </c>
+      <c r="P5">
+        <v>22</v>
+      </c>
+      <c r="Q5">
+        <v>38</v>
+      </c>
+      <c r="R5">
+        <v>36</v>
+      </c>
+      <c r="S5">
+        <v>32</v>
+      </c>
+      <c r="T5">
+        <v>12</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>41</v>
+      </c>
+      <c r="W5">
+        <v>42</v>
+      </c>
+      <c r="X5">
+        <v>24</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>5</v>
+      </c>
+      <c r="AA5">
+        <v>25</v>
+      </c>
+      <c r="AB5">
+        <v>4</v>
+      </c>
+      <c r="AC5">
+        <v>38</v>
+      </c>
+      <c r="AD5">
+        <v>36</v>
+      </c>
+      <c r="AE5">
+        <v>36</v>
+      </c>
+      <c r="AG5">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>109</v>
+      </c>
+      <c r="C6">
+        <v>96</v>
+      </c>
+      <c r="D6">
+        <v>68</v>
+      </c>
+      <c r="E6">
+        <v>43</v>
+      </c>
+      <c r="F6">
+        <v>66</v>
+      </c>
+      <c r="G6">
+        <v>42</v>
+      </c>
+      <c r="H6">
+        <v>95</v>
+      </c>
+      <c r="I6">
+        <v>71</v>
+      </c>
+      <c r="J6">
+        <v>82</v>
+      </c>
+      <c r="K6">
+        <v>84</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <v>67</v>
+      </c>
+      <c r="N6">
+        <v>43</v>
+      </c>
+      <c r="O6">
+        <v>90</v>
+      </c>
+      <c r="P6">
+        <v>88</v>
+      </c>
+      <c r="Q6">
+        <v>68</v>
+      </c>
+      <c r="R6">
+        <v>74</v>
+      </c>
+      <c r="S6">
+        <v>52</v>
+      </c>
+      <c r="T6">
+        <v>65</v>
+      </c>
+      <c r="U6">
+        <v>37</v>
+      </c>
+      <c r="V6">
+        <v>92</v>
+      </c>
+      <c r="W6">
+        <v>72</v>
+      </c>
+      <c r="X6">
+        <v>79</v>
+      </c>
+      <c r="Y6">
+        <v>3</v>
+      </c>
+      <c r="Z6">
+        <v>9</v>
+      </c>
+      <c r="AA6">
+        <v>60</v>
+      </c>
+      <c r="AB6">
+        <v>32</v>
+      </c>
+      <c r="AC6">
+        <v>75</v>
+      </c>
+      <c r="AD6">
+        <v>72</v>
+      </c>
+      <c r="AE6">
+        <v>95</v>
+      </c>
+      <c r="AG6">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>4</v>
+      </c>
+      <c r="T7">
+        <v>2</v>
+      </c>
+      <c r="V7">
+        <v>2</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>2</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AD7">
+        <v>1</v>
+      </c>
+      <c r="AE7">
+        <v>2</v>
+      </c>
+      <c r="AG7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>77</v>
+      </c>
+      <c r="C8">
+        <v>71</v>
+      </c>
+      <c r="D8">
+        <v>47</v>
+      </c>
+      <c r="E8">
+        <v>36</v>
+      </c>
+      <c r="F8">
+        <v>40</v>
+      </c>
+      <c r="G8">
+        <v>27</v>
+      </c>
+      <c r="H8">
+        <v>56</v>
+      </c>
+      <c r="I8">
+        <v>49</v>
+      </c>
+      <c r="J8">
+        <v>68</v>
+      </c>
+      <c r="K8">
+        <v>63</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>52</v>
+      </c>
+      <c r="N8">
+        <v>21</v>
+      </c>
+      <c r="O8">
+        <v>57</v>
+      </c>
+      <c r="P8">
+        <v>61</v>
+      </c>
+      <c r="Q8">
+        <v>72</v>
+      </c>
+      <c r="R8">
+        <v>50</v>
+      </c>
+      <c r="S8">
+        <v>51</v>
+      </c>
+      <c r="T8">
+        <v>24</v>
+      </c>
+      <c r="U8">
+        <v>24</v>
+      </c>
+      <c r="V8">
+        <v>59</v>
+      </c>
+      <c r="W8">
+        <v>44</v>
+      </c>
+      <c r="X8">
+        <v>56</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>6</v>
+      </c>
+      <c r="AA8">
+        <v>45</v>
+      </c>
+      <c r="AB8">
+        <v>18</v>
+      </c>
+      <c r="AC8">
+        <v>47</v>
+      </c>
+      <c r="AD8">
+        <v>62</v>
+      </c>
+      <c r="AE8">
+        <v>68</v>
+      </c>
+      <c r="AG8">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>16</v>
+      </c>
+      <c r="I9">
+        <v>24</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>6</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>14</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9">
+        <v>11</v>
+      </c>
+      <c r="R9">
+        <v>13</v>
+      </c>
+      <c r="S9">
+        <v>11</v>
+      </c>
+      <c r="T9">
+        <v>6</v>
+      </c>
+      <c r="V9">
+        <v>14</v>
+      </c>
+      <c r="W9">
+        <v>7</v>
+      </c>
+      <c r="X9">
+        <v>13</v>
+      </c>
+      <c r="Z9">
+        <v>5</v>
+      </c>
+      <c r="AA9">
+        <v>8</v>
+      </c>
+      <c r="AB9">
+        <v>1</v>
+      </c>
+      <c r="AC9">
+        <v>13</v>
+      </c>
+      <c r="AD9">
+        <v>7</v>
+      </c>
+      <c r="AE9">
+        <v>9</v>
+      </c>
+      <c r="AG9">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>7</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <v>12</v>
+      </c>
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
+      </c>
+      <c r="P10">
+        <v>8</v>
+      </c>
+      <c r="Q10">
+        <v>9</v>
+      </c>
+      <c r="R10">
+        <v>11</v>
+      </c>
+      <c r="S10">
+        <v>9</v>
+      </c>
+      <c r="T10">
+        <v>6</v>
+      </c>
+      <c r="V10">
+        <v>7</v>
+      </c>
+      <c r="W10">
+        <v>15</v>
+      </c>
+      <c r="X10">
+        <v>9</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>5</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <v>9</v>
+      </c>
+      <c r="AD10">
+        <v>7</v>
+      </c>
+      <c r="AE10">
+        <v>15</v>
+      </c>
+      <c r="AG10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>11</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
+      <c r="O11">
+        <v>6</v>
+      </c>
+      <c r="Q11">
+        <v>11</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>2</v>
+      </c>
+      <c r="V11">
+        <v>9</v>
+      </c>
+      <c r="X11">
+        <v>9</v>
+      </c>
+      <c r="Z11">
+        <v>3</v>
+      </c>
+      <c r="AC11">
+        <v>7</v>
+      </c>
+      <c r="AE11">
+        <v>7</v>
+      </c>
+      <c r="AG11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="X12">
+        <v>1</v>
+      </c>
+      <c r="AA12">
+        <v>1</v>
+      </c>
+      <c r="AC12">
+        <v>4</v>
+      </c>
+      <c r="AG12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>3</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>3</v>
+      </c>
+      <c r="V14">
+        <v>4</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>4</v>
+      </c>
+      <c r="AC14">
+        <v>3</v>
+      </c>
+      <c r="AE14">
+        <v>6</v>
+      </c>
+      <c r="AG14">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <v>7</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <v>5</v>
+      </c>
+      <c r="M15">
+        <v>5</v>
+      </c>
+      <c r="O15">
+        <v>5</v>
+      </c>
+      <c r="P15">
+        <v>8</v>
+      </c>
+      <c r="Q15">
+        <v>11</v>
+      </c>
+      <c r="R15">
+        <v>8</v>
+      </c>
+      <c r="S15">
+        <v>5</v>
+      </c>
+      <c r="T15">
+        <v>3</v>
+      </c>
+      <c r="V15">
+        <v>12</v>
+      </c>
+      <c r="W15">
+        <v>6</v>
+      </c>
+      <c r="X15">
+        <v>12</v>
+      </c>
+      <c r="AC15">
+        <v>7</v>
+      </c>
+      <c r="AD15">
+        <v>5</v>
+      </c>
+      <c r="AE15">
+        <v>8</v>
+      </c>
+      <c r="AG15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>22</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>11</v>
+      </c>
+      <c r="K16">
+        <v>9</v>
+      </c>
+      <c r="L16">
+        <v>13</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>10</v>
+      </c>
+      <c r="P16">
+        <v>13</v>
+      </c>
+      <c r="Q16">
+        <v>13</v>
+      </c>
+      <c r="R16">
+        <v>12</v>
+      </c>
+      <c r="S16">
+        <v>6</v>
+      </c>
+      <c r="T16">
+        <v>5</v>
+      </c>
+      <c r="V16">
+        <v>11</v>
+      </c>
+      <c r="W16">
+        <v>25</v>
+      </c>
+      <c r="X16">
+        <v>14</v>
+      </c>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
+        <v>13</v>
+      </c>
+      <c r="AD16">
+        <v>13</v>
+      </c>
+      <c r="AE16">
+        <v>8</v>
+      </c>
+      <c r="AG16">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>6</v>
+      </c>
+      <c r="K17">
+        <v>6</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>10</v>
+      </c>
+      <c r="P17">
+        <v>4</v>
+      </c>
+      <c r="Q17">
+        <v>2</v>
+      </c>
+      <c r="R17">
+        <v>6</v>
+      </c>
+      <c r="S17">
+        <v>5</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>7</v>
+      </c>
+      <c r="W17">
+        <v>7</v>
+      </c>
+      <c r="X17">
+        <v>2</v>
+      </c>
+      <c r="AC17">
+        <v>10</v>
+      </c>
+      <c r="AD17">
+        <v>30</v>
+      </c>
+      <c r="AE17">
+        <v>4</v>
+      </c>
+      <c r="AG17">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>12</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+      <c r="O18">
+        <v>3</v>
+      </c>
+      <c r="P18">
+        <v>3</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <v>5</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>6</v>
+      </c>
+      <c r="V18">
+        <v>4</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18">
+        <v>4</v>
+      </c>
+      <c r="AA18">
+        <v>2</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18">
+        <v>4</v>
+      </c>
+      <c r="AD18">
+        <v>2</v>
+      </c>
+      <c r="AE18">
+        <v>2</v>
+      </c>
+      <c r="AG18">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>25</v>
+      </c>
+      <c r="I19">
+        <v>33</v>
+      </c>
+      <c r="J19">
+        <v>23</v>
+      </c>
+      <c r="K19">
+        <v>12</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+      <c r="M19">
+        <v>28</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>29</v>
+      </c>
+      <c r="P19">
+        <v>19</v>
+      </c>
+      <c r="Q19">
+        <v>25</v>
+      </c>
+      <c r="R19">
+        <v>40</v>
+      </c>
+      <c r="S19">
+        <v>14</v>
+      </c>
+      <c r="T19">
+        <v>15</v>
+      </c>
+      <c r="U19">
+        <v>2</v>
+      </c>
+      <c r="V19">
+        <v>31</v>
+      </c>
+      <c r="W19">
+        <v>22</v>
+      </c>
+      <c r="X19">
+        <v>1</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <v>3</v>
+      </c>
+      <c r="AB19">
+        <v>3</v>
+      </c>
+      <c r="AC19">
+        <v>41</v>
+      </c>
+      <c r="AD19">
+        <v>23</v>
+      </c>
+      <c r="AE19">
+        <v>17</v>
+      </c>
+      <c r="AG19">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>4</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>4</v>
+      </c>
+      <c r="V20">
+        <v>6</v>
+      </c>
+      <c r="W20">
+        <v>2</v>
+      </c>
+      <c r="X20">
+        <v>2</v>
+      </c>
+      <c r="AC20">
+        <v>1</v>
+      </c>
+      <c r="AD20">
+        <v>5</v>
+      </c>
+      <c r="AE20">
+        <v>1</v>
+      </c>
+      <c r="AG20">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>39</v>
+      </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>31</v>
+      </c>
+      <c r="E21">
+        <v>27</v>
+      </c>
+      <c r="F21">
+        <v>22</v>
+      </c>
+      <c r="G21">
+        <v>11</v>
+      </c>
+      <c r="H21">
+        <v>26</v>
+      </c>
+      <c r="I21">
+        <v>34</v>
+      </c>
+      <c r="J21">
+        <v>23</v>
+      </c>
+      <c r="K21">
+        <v>40</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21">
+        <v>16</v>
+      </c>
+      <c r="N21">
+        <v>12</v>
+      </c>
+      <c r="O21">
+        <v>29</v>
+      </c>
+      <c r="P21">
+        <v>27</v>
+      </c>
+      <c r="Q21">
+        <v>26</v>
+      </c>
+      <c r="R21">
+        <v>29</v>
+      </c>
+      <c r="S21">
+        <v>23</v>
+      </c>
+      <c r="T21">
+        <v>11</v>
+      </c>
+      <c r="U21">
+        <v>18</v>
+      </c>
+      <c r="V21">
+        <v>23</v>
+      </c>
+      <c r="W21">
+        <v>32</v>
+      </c>
+      <c r="X21">
+        <v>13</v>
+      </c>
+      <c r="Y21">
+        <v>2</v>
+      </c>
+      <c r="Z21">
+        <v>3</v>
+      </c>
+      <c r="AA21">
+        <v>15</v>
+      </c>
+      <c r="AB21">
+        <v>10</v>
+      </c>
+      <c r="AC21">
+        <v>34</v>
+      </c>
+      <c r="AD21">
+        <v>30</v>
+      </c>
+      <c r="AE21">
+        <v>18</v>
+      </c>
+      <c r="AG21">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <v>6</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>5</v>
+      </c>
+      <c r="Q22">
+        <v>5</v>
+      </c>
+      <c r="AC22">
+        <v>2</v>
+      </c>
+      <c r="AD22">
+        <v>1</v>
+      </c>
+      <c r="AE22">
+        <v>4</v>
+      </c>
+      <c r="AG22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>27</v>
+      </c>
+      <c r="D23">
+        <v>35</v>
+      </c>
+      <c r="E23">
+        <v>27</v>
+      </c>
+      <c r="F23">
+        <v>14</v>
+      </c>
+      <c r="H23">
+        <v>23</v>
+      </c>
+      <c r="I23">
+        <v>35</v>
+      </c>
+      <c r="J23">
+        <v>27</v>
+      </c>
+      <c r="K23">
+        <v>43</v>
+      </c>
+      <c r="L23">
+        <v>4</v>
+      </c>
+      <c r="O23">
+        <v>41</v>
+      </c>
+      <c r="P23">
+        <v>30</v>
+      </c>
+      <c r="Q23">
+        <v>32</v>
+      </c>
+      <c r="R23">
+        <v>41</v>
+      </c>
+      <c r="S23">
+        <v>29</v>
+      </c>
+      <c r="T23">
+        <v>17</v>
+      </c>
+      <c r="V23">
+        <v>32</v>
+      </c>
+      <c r="W23">
+        <v>36</v>
+      </c>
+      <c r="X23">
+        <v>38</v>
+      </c>
+      <c r="AC23">
+        <v>58</v>
+      </c>
+      <c r="AD23">
+        <v>42</v>
+      </c>
+      <c r="AE23">
+        <v>38</v>
+      </c>
+      <c r="AG23">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>2</v>
+      </c>
+      <c r="S24">
+        <v>4</v>
+      </c>
+      <c r="V24">
+        <v>3</v>
+      </c>
+      <c r="W24">
+        <v>7</v>
+      </c>
+      <c r="X24">
+        <v>9</v>
+      </c>
+      <c r="AC24">
+        <v>4</v>
+      </c>
+      <c r="AD24">
+        <v>3</v>
+      </c>
+      <c r="AE24">
+        <v>2</v>
+      </c>
+      <c r="AG24">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>39</v>
+      </c>
+      <c r="D25">
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <v>26</v>
+      </c>
+      <c r="F25">
+        <v>18</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>26</v>
+      </c>
+      <c r="I25">
+        <v>28</v>
+      </c>
+      <c r="J25">
+        <v>27</v>
+      </c>
+      <c r="K25">
+        <v>21</v>
+      </c>
+      <c r="L25">
+        <v>4</v>
+      </c>
+      <c r="M25">
+        <v>23</v>
+      </c>
+      <c r="N25">
+        <v>4</v>
+      </c>
+      <c r="O25">
+        <v>27</v>
+      </c>
+      <c r="P25">
+        <v>27</v>
+      </c>
+      <c r="Q25">
+        <v>23</v>
+      </c>
+      <c r="R25">
+        <v>34</v>
+      </c>
+      <c r="S25">
+        <v>30</v>
+      </c>
+      <c r="T25">
+        <v>18</v>
+      </c>
+      <c r="U25">
+        <v>7</v>
+      </c>
+      <c r="V25">
+        <v>27</v>
+      </c>
+      <c r="W25">
+        <v>21</v>
+      </c>
+      <c r="X25">
+        <v>31</v>
+      </c>
+      <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="Z25">
+        <v>23</v>
+      </c>
+      <c r="AA25">
+        <v>19</v>
+      </c>
+      <c r="AB25">
+        <v>1</v>
+      </c>
+      <c r="AC25">
+        <v>29</v>
+      </c>
+      <c r="AD25">
+        <v>26</v>
+      </c>
+      <c r="AE25">
+        <v>19</v>
+      </c>
+      <c r="AG25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>101</v>
+      </c>
+      <c r="C26">
+        <v>106</v>
+      </c>
+      <c r="D26">
+        <v>85</v>
+      </c>
+      <c r="E26">
+        <v>82</v>
+      </c>
+      <c r="F26">
+        <v>57</v>
+      </c>
+      <c r="G26">
+        <v>39</v>
+      </c>
+      <c r="H26">
+        <v>98</v>
+      </c>
+      <c r="I26">
+        <v>99</v>
+      </c>
+      <c r="J26">
+        <v>92</v>
+      </c>
+      <c r="K26">
+        <v>70</v>
+      </c>
+      <c r="L26">
+        <v>8</v>
+      </c>
+      <c r="M26">
+        <v>87</v>
+      </c>
+      <c r="N26">
+        <v>34</v>
+      </c>
+      <c r="O26">
+        <v>132</v>
+      </c>
+      <c r="P26">
+        <v>108</v>
+      </c>
+      <c r="Q26">
+        <v>107</v>
+      </c>
+      <c r="R26">
+        <v>102</v>
+      </c>
+      <c r="S26">
+        <v>76</v>
+      </c>
+      <c r="T26">
+        <v>67</v>
+      </c>
+      <c r="U26">
+        <v>40</v>
+      </c>
+      <c r="V26">
+        <v>108</v>
+      </c>
+      <c r="W26">
+        <v>92</v>
+      </c>
+      <c r="X26">
+        <v>77</v>
+      </c>
+      <c r="Y26">
+        <v>5</v>
+      </c>
+      <c r="Z26">
+        <v>17</v>
+      </c>
+      <c r="AA26">
+        <v>90</v>
+      </c>
+      <c r="AB26">
+        <v>30</v>
+      </c>
+      <c r="AC26">
+        <v>127</v>
+      </c>
+      <c r="AD26">
+        <v>93</v>
+      </c>
+      <c r="AE26">
+        <v>101</v>
+      </c>
+      <c r="AG26">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <v>9</v>
+      </c>
+      <c r="I27">
+        <v>7</v>
+      </c>
+      <c r="J27">
+        <v>7</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <v>13</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>6</v>
+      </c>
+      <c r="P27">
+        <v>6</v>
+      </c>
+      <c r="Q27">
+        <v>4</v>
+      </c>
+      <c r="R27">
+        <v>4</v>
+      </c>
+      <c r="S27">
+        <v>5</v>
+      </c>
+      <c r="U27">
+        <v>2</v>
+      </c>
+      <c r="V27">
+        <v>5</v>
+      </c>
+      <c r="W27">
+        <v>8</v>
+      </c>
+      <c r="X27">
+        <v>10</v>
+      </c>
+      <c r="AB27">
+        <v>2</v>
+      </c>
+      <c r="AC27">
+        <v>11</v>
+      </c>
+      <c r="AD27">
+        <v>10</v>
+      </c>
+      <c r="AE27">
+        <v>3</v>
+      </c>
+      <c r="AG27">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+      <c r="F29">
+        <v>7</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>15</v>
+      </c>
+      <c r="I29">
+        <v>13</v>
+      </c>
+      <c r="J29">
+        <v>15</v>
+      </c>
+      <c r="K29">
+        <v>10</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>5</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>18</v>
+      </c>
+      <c r="P29">
+        <v>7</v>
+      </c>
+      <c r="Q29">
+        <v>20</v>
+      </c>
+      <c r="R29">
+        <v>11</v>
+      </c>
+      <c r="T29">
+        <v>4</v>
+      </c>
+      <c r="V29">
+        <v>12</v>
+      </c>
+      <c r="W29">
+        <v>13</v>
+      </c>
+      <c r="X29">
+        <v>9</v>
+      </c>
+      <c r="Y29">
+        <v>2</v>
+      </c>
+      <c r="Z29">
+        <v>1</v>
+      </c>
+      <c r="AA29">
+        <v>9</v>
+      </c>
+      <c r="AC29">
+        <v>11</v>
+      </c>
+      <c r="AD29">
+        <v>11</v>
+      </c>
+      <c r="AE29">
+        <v>8</v>
+      </c>
+      <c r="AG29">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>6</v>
+      </c>
+      <c r="I30">
+        <v>8</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>3</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>2</v>
+      </c>
+      <c r="O30">
+        <v>6</v>
+      </c>
+      <c r="P30">
+        <v>3</v>
+      </c>
+      <c r="Q30">
+        <v>5</v>
+      </c>
+      <c r="R30">
+        <v>5</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="V30">
+        <v>3</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <v>3</v>
+      </c>
+      <c r="AC30">
+        <v>3</v>
+      </c>
+      <c r="AD30">
+        <v>3</v>
+      </c>
+      <c r="AE30">
+        <v>3</v>
+      </c>
+      <c r="AG30">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>15</v>
+      </c>
+      <c r="D31">
+        <v>31</v>
+      </c>
+      <c r="E31">
+        <v>12</v>
+      </c>
+      <c r="F31">
+        <v>12</v>
+      </c>
+      <c r="H31">
+        <v>28</v>
+      </c>
+      <c r="I31">
+        <v>24</v>
+      </c>
+      <c r="J31">
+        <v>22</v>
+      </c>
+      <c r="K31">
+        <v>23</v>
+      </c>
+      <c r="L31">
+        <v>18</v>
+      </c>
+      <c r="M31">
+        <v>10</v>
+      </c>
+      <c r="O31">
+        <v>16</v>
+      </c>
+      <c r="P31">
+        <v>23</v>
+      </c>
+      <c r="Q31">
+        <v>17</v>
+      </c>
+      <c r="R31">
+        <v>15</v>
+      </c>
+      <c r="S31">
+        <v>19</v>
+      </c>
+      <c r="T31">
+        <v>11</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31">
+        <v>21</v>
+      </c>
+      <c r="W31">
+        <v>12</v>
+      </c>
+      <c r="X31">
+        <v>39</v>
+      </c>
+      <c r="Y31">
+        <v>1</v>
+      </c>
+      <c r="AA31">
+        <v>1</v>
+      </c>
+      <c r="AB31">
+        <v>1</v>
+      </c>
+      <c r="AC31">
+        <v>25</v>
+      </c>
+      <c r="AD31">
+        <v>18</v>
+      </c>
+      <c r="AE31">
+        <v>23</v>
+      </c>
+      <c r="AG31">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>2</v>
+      </c>
+      <c r="O32">
+        <v>4</v>
+      </c>
+      <c r="R32">
+        <v>4</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>2</v>
+      </c>
+      <c r="AC32">
+        <v>3</v>
+      </c>
+      <c r="AD32">
+        <v>1</v>
+      </c>
+      <c r="AE32">
+        <v>1</v>
+      </c>
+      <c r="AG32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="K33">
+        <v>4</v>
+      </c>
+      <c r="L33">
+        <v>2</v>
+      </c>
+      <c r="M33">
+        <v>4</v>
+      </c>
+      <c r="P33">
+        <v>5</v>
+      </c>
+      <c r="Q33">
+        <v>7</v>
+      </c>
+      <c r="R33">
+        <v>3</v>
+      </c>
+      <c r="S33">
+        <v>4</v>
+      </c>
+      <c r="T33">
+        <v>1</v>
+      </c>
+      <c r="V33">
+        <v>3</v>
+      </c>
+      <c r="W33">
+        <v>7</v>
+      </c>
+      <c r="X33">
+        <v>3</v>
+      </c>
+      <c r="Y33">
+        <v>1</v>
+      </c>
+      <c r="AA33">
+        <v>1</v>
+      </c>
+      <c r="AD33">
+        <v>6</v>
+      </c>
+      <c r="AE33">
+        <v>5</v>
+      </c>
+      <c r="AG33">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34">
+        <v>30</v>
+      </c>
+      <c r="C34">
+        <v>45</v>
+      </c>
+      <c r="D34">
+        <v>42</v>
+      </c>
+      <c r="E34">
+        <v>18</v>
+      </c>
+      <c r="F34">
+        <v>21</v>
+      </c>
+      <c r="H34">
+        <v>27</v>
+      </c>
+      <c r="I34">
+        <v>35</v>
+      </c>
+      <c r="J34">
+        <v>43</v>
+      </c>
+      <c r="K34">
+        <v>37</v>
+      </c>
+      <c r="M34">
+        <v>26</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>35</v>
+      </c>
+      <c r="P34">
+        <v>29</v>
+      </c>
+      <c r="Q34">
+        <v>24</v>
+      </c>
+      <c r="R34">
+        <v>31</v>
+      </c>
+      <c r="S34">
+        <v>34</v>
+      </c>
+      <c r="T34">
+        <v>19</v>
+      </c>
+      <c r="V34">
+        <v>33</v>
+      </c>
+      <c r="W34">
+        <v>34</v>
+      </c>
+      <c r="X34">
+        <v>35</v>
+      </c>
+      <c r="Z34">
+        <v>1</v>
+      </c>
+      <c r="AA34">
+        <v>22</v>
+      </c>
+      <c r="AC34">
+        <v>51</v>
+      </c>
+      <c r="AD34">
+        <v>46</v>
+      </c>
+      <c r="AE34">
+        <v>26</v>
+      </c>
+      <c r="AG34">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>27</v>
+      </c>
+      <c r="C35">
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <v>15</v>
+      </c>
+      <c r="E35">
+        <v>15</v>
+      </c>
+      <c r="F35">
+        <v>14</v>
+      </c>
+      <c r="H35">
+        <v>26</v>
+      </c>
+      <c r="I35">
+        <v>19</v>
+      </c>
+      <c r="J35">
+        <v>29</v>
+      </c>
+      <c r="K35">
+        <v>14</v>
+      </c>
+      <c r="M35">
+        <v>21</v>
+      </c>
+      <c r="O35">
+        <v>33</v>
+      </c>
+      <c r="P35">
+        <v>15</v>
+      </c>
+      <c r="Q35">
+        <v>9</v>
+      </c>
+      <c r="R35">
+        <v>16</v>
+      </c>
+      <c r="S35">
+        <v>20</v>
+      </c>
+      <c r="T35">
+        <v>15</v>
+      </c>
+      <c r="U35">
+        <v>1</v>
+      </c>
+      <c r="V35">
+        <v>29</v>
+      </c>
+      <c r="W35">
+        <v>20</v>
+      </c>
+      <c r="X35">
+        <v>23</v>
+      </c>
+      <c r="AB35">
+        <v>1</v>
+      </c>
+      <c r="AC35">
+        <v>38</v>
+      </c>
+      <c r="AD35">
+        <v>9</v>
+      </c>
+      <c r="AE35">
+        <v>17</v>
+      </c>
+      <c r="AG35">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>15</v>
+      </c>
+      <c r="D36">
+        <v>15</v>
+      </c>
+      <c r="E36">
+        <v>11</v>
+      </c>
+      <c r="F36">
+        <v>7</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>20</v>
+      </c>
+      <c r="I36">
+        <v>13</v>
+      </c>
+      <c r="J36">
+        <v>18</v>
+      </c>
+      <c r="K36">
+        <v>14</v>
+      </c>
+      <c r="M36">
+        <v>10</v>
+      </c>
+      <c r="O36">
+        <v>23</v>
+      </c>
+      <c r="P36">
+        <v>20</v>
+      </c>
+      <c r="Q36">
+        <v>20</v>
+      </c>
+      <c r="R36">
+        <v>19</v>
+      </c>
+      <c r="S36">
+        <v>15</v>
+      </c>
+      <c r="T36">
+        <v>12</v>
+      </c>
+      <c r="U36">
+        <v>4</v>
+      </c>
+      <c r="V36">
+        <v>14</v>
+      </c>
+      <c r="W36">
+        <v>12</v>
+      </c>
+      <c r="X36">
+        <v>28</v>
+      </c>
+      <c r="Z36">
+        <v>2</v>
+      </c>
+      <c r="AA36">
+        <v>9</v>
+      </c>
+      <c r="AB36">
+        <v>1</v>
+      </c>
+      <c r="AC36">
+        <v>22</v>
+      </c>
+      <c r="AD36">
+        <v>13</v>
+      </c>
+      <c r="AE36">
+        <v>18</v>
+      </c>
+      <c r="AG36">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <v>70</v>
+      </c>
+      <c r="C37">
+        <v>70</v>
+      </c>
+      <c r="D37">
+        <v>80</v>
+      </c>
+      <c r="E37">
+        <v>54</v>
+      </c>
+      <c r="F37">
+        <v>29</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <v>68</v>
+      </c>
+      <c r="I37">
+        <v>69</v>
+      </c>
+      <c r="J37">
+        <v>73</v>
+      </c>
+      <c r="K37">
+        <v>80</v>
+      </c>
+      <c r="L37">
+        <v>55</v>
+      </c>
+      <c r="M37">
+        <v>29</v>
+      </c>
+      <c r="N37">
+        <v>2</v>
+      </c>
+      <c r="O37">
+        <v>61</v>
+      </c>
+      <c r="P37">
+        <v>53</v>
+      </c>
+      <c r="Q37">
+        <v>74</v>
+      </c>
+      <c r="R37">
+        <v>69</v>
+      </c>
+      <c r="S37">
+        <v>50</v>
+      </c>
+      <c r="T37">
+        <v>32</v>
+      </c>
+      <c r="U37">
+        <v>6</v>
+      </c>
+      <c r="V37">
+        <v>56</v>
+      </c>
+      <c r="W37">
+        <v>69</v>
+      </c>
+      <c r="X37">
+        <v>61</v>
+      </c>
+      <c r="Y37">
+        <v>1</v>
+      </c>
+      <c r="Z37">
+        <v>2</v>
+      </c>
+      <c r="AA37">
+        <v>39</v>
+      </c>
+      <c r="AB37">
+        <v>6</v>
+      </c>
+      <c r="AC37">
+        <v>70</v>
+      </c>
+      <c r="AD37">
+        <v>68</v>
+      </c>
+      <c r="AE37">
+        <v>77</v>
+      </c>
+      <c r="AG37">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>14</v>
+      </c>
+      <c r="E38">
+        <v>13</v>
+      </c>
+      <c r="F38">
+        <v>6</v>
+      </c>
+      <c r="H38">
+        <v>13</v>
+      </c>
+      <c r="I38">
+        <v>11</v>
+      </c>
+      <c r="J38">
+        <v>11</v>
+      </c>
+      <c r="K38">
+        <v>9</v>
+      </c>
+      <c r="L38">
+        <v>14</v>
+      </c>
+      <c r="M38">
+        <v>11</v>
+      </c>
+      <c r="O38">
+        <v>15</v>
+      </c>
+      <c r="P38">
+        <v>19</v>
+      </c>
+      <c r="Q38">
+        <v>17</v>
+      </c>
+      <c r="R38">
+        <v>11</v>
+      </c>
+      <c r="S38">
+        <v>14</v>
+      </c>
+      <c r="T38">
+        <v>7</v>
+      </c>
+      <c r="V38">
+        <v>12</v>
+      </c>
+      <c r="W38">
+        <v>19</v>
+      </c>
+      <c r="X38">
+        <v>17</v>
+      </c>
+      <c r="Z38">
+        <v>1</v>
+      </c>
+      <c r="AA38">
+        <v>10</v>
+      </c>
+      <c r="AB38">
+        <v>2</v>
+      </c>
+      <c r="AC38">
+        <v>9</v>
+      </c>
+      <c r="AD38">
+        <v>13</v>
+      </c>
+      <c r="AE38">
+        <v>9</v>
+      </c>
+      <c r="AG38">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>62</v>
+      </c>
+      <c r="C39">
+        <v>49</v>
+      </c>
+      <c r="D39">
+        <v>51</v>
+      </c>
+      <c r="E39">
+        <v>38</v>
+      </c>
+      <c r="F39">
+        <v>26</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
+      </c>
+      <c r="H39">
+        <v>53</v>
+      </c>
+      <c r="I39">
+        <v>51</v>
+      </c>
+      <c r="J39">
+        <v>36</v>
+      </c>
+      <c r="K39">
+        <v>65</v>
+      </c>
+      <c r="M39">
+        <v>32</v>
+      </c>
+      <c r="N39">
+        <v>2</v>
+      </c>
+      <c r="O39">
+        <v>56</v>
+      </c>
+      <c r="P39">
+        <v>52</v>
+      </c>
+      <c r="Q39">
+        <v>39</v>
+      </c>
+      <c r="R39">
+        <v>35</v>
+      </c>
+      <c r="S39">
+        <v>38</v>
+      </c>
+      <c r="T39">
+        <v>23</v>
+      </c>
+      <c r="U39">
+        <v>1</v>
+      </c>
+      <c r="V39">
+        <v>63</v>
+      </c>
+      <c r="W39">
+        <v>43</v>
+      </c>
+      <c r="X39">
+        <v>60</v>
+      </c>
+      <c r="Y39">
+        <v>2</v>
+      </c>
+      <c r="AA39">
+        <v>34</v>
+      </c>
+      <c r="AB39">
+        <v>2</v>
+      </c>
+      <c r="AC39">
+        <v>58</v>
+      </c>
+      <c r="AD39">
+        <v>61</v>
+      </c>
+      <c r="AE39">
+        <v>41</v>
+      </c>
+      <c r="AG39">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="I40">
+        <v>6</v>
+      </c>
+      <c r="K40">
+        <v>3</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="R40">
+        <v>4</v>
+      </c>
+      <c r="T40">
+        <v>1</v>
+      </c>
+      <c r="W40">
+        <v>4</v>
+      </c>
+      <c r="Y40">
+        <v>1</v>
+      </c>
+      <c r="AA40">
+        <v>1</v>
+      </c>
+      <c r="AD40">
+        <v>6</v>
+      </c>
+      <c r="AG40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41">
+        <v>2</v>
+      </c>
+      <c r="L41">
+        <v>3</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="P41">
+        <v>4</v>
+      </c>
+      <c r="Q41">
+        <v>3</v>
+      </c>
+      <c r="R41">
+        <v>8</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <v>3</v>
+      </c>
+      <c r="W41">
+        <v>2</v>
+      </c>
+      <c r="Y41">
+        <v>2</v>
+      </c>
+      <c r="AC41">
+        <v>1</v>
+      </c>
+      <c r="AE41">
+        <v>2</v>
+      </c>
+      <c r="AG41">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>26</v>
+      </c>
+      <c r="D42">
+        <v>20</v>
+      </c>
+      <c r="E42">
+        <v>11</v>
+      </c>
+      <c r="H42">
+        <v>24</v>
+      </c>
+      <c r="I42">
+        <v>21</v>
+      </c>
+      <c r="J42">
+        <v>31</v>
+      </c>
+      <c r="K42">
+        <v>29</v>
+      </c>
+      <c r="L42">
+        <v>10</v>
+      </c>
+      <c r="O42">
+        <v>12</v>
+      </c>
+      <c r="P42">
+        <v>6</v>
+      </c>
+      <c r="Q42">
+        <v>17</v>
+      </c>
+      <c r="R42">
+        <v>12</v>
+      </c>
+      <c r="S42">
+        <v>4</v>
+      </c>
+      <c r="V42">
+        <v>21</v>
+      </c>
+      <c r="W42">
+        <v>19</v>
+      </c>
+      <c r="AC42">
+        <v>19</v>
+      </c>
+      <c r="AD42">
+        <v>24</v>
+      </c>
+      <c r="AE42">
+        <v>21</v>
+      </c>
+      <c r="AG42">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43">
+        <v>58</v>
+      </c>
+      <c r="C43">
+        <v>64</v>
+      </c>
+      <c r="D43">
+        <v>62</v>
+      </c>
+      <c r="E43">
+        <v>46</v>
+      </c>
+      <c r="H43">
+        <v>75</v>
+      </c>
+      <c r="I43">
+        <v>33</v>
+      </c>
+      <c r="J43">
+        <v>78</v>
+      </c>
+      <c r="K43">
+        <v>81</v>
+      </c>
+      <c r="L43">
+        <v>40</v>
+      </c>
+      <c r="O43">
+        <v>71</v>
+      </c>
+      <c r="P43">
+        <v>68</v>
+      </c>
+      <c r="Q43">
+        <v>65</v>
+      </c>
+      <c r="R43">
+        <v>64</v>
+      </c>
+      <c r="S43">
+        <v>46</v>
+      </c>
+      <c r="V43">
+        <v>67</v>
+      </c>
+      <c r="W43">
+        <v>60</v>
+      </c>
+      <c r="AC43">
+        <v>73</v>
+      </c>
+      <c r="AD43">
+        <v>72</v>
+      </c>
+      <c r="AE43">
+        <v>63</v>
+      </c>
+      <c r="AG43">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+      <c r="S44">
+        <v>1</v>
+      </c>
+      <c r="V44">
+        <v>1</v>
+      </c>
+      <c r="AC44">
+        <v>2</v>
+      </c>
+      <c r="AG44">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45">
+        <v>27</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>6</v>
+      </c>
+      <c r="H45">
+        <v>4</v>
+      </c>
+      <c r="I45">
+        <v>21</v>
+      </c>
+      <c r="J45">
+        <v>4</v>
+      </c>
+      <c r="K45">
+        <v>13</v>
+      </c>
+      <c r="L45">
+        <v>10</v>
+      </c>
+      <c r="O45">
+        <v>5</v>
+      </c>
+      <c r="P45">
+        <v>16</v>
+      </c>
+      <c r="Q45">
+        <v>9</v>
+      </c>
+      <c r="R45">
+        <v>6</v>
+      </c>
+      <c r="S45">
+        <v>1</v>
+      </c>
+      <c r="V45">
+        <v>3</v>
+      </c>
+      <c r="W45">
+        <v>3</v>
+      </c>
+      <c r="AC45">
+        <v>8</v>
+      </c>
+      <c r="AD45">
+        <v>9</v>
+      </c>
+      <c r="AE45">
+        <v>8</v>
+      </c>
+      <c r="AG45">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46">
+        <v>16</v>
+      </c>
+      <c r="D46">
+        <v>17</v>
+      </c>
+      <c r="E46">
+        <v>8</v>
+      </c>
+      <c r="H46">
+        <v>18</v>
+      </c>
+      <c r="J46">
+        <v>18</v>
+      </c>
+      <c r="K46">
+        <v>16</v>
+      </c>
+      <c r="O46">
+        <v>2</v>
+      </c>
+      <c r="P46">
+        <v>9</v>
+      </c>
+      <c r="Q46">
+        <v>21</v>
+      </c>
+      <c r="R46">
+        <v>16</v>
+      </c>
+      <c r="S46">
+        <v>8</v>
+      </c>
+      <c r="W46">
+        <v>19</v>
+      </c>
+      <c r="AE46">
+        <v>21</v>
+      </c>
+      <c r="AG46">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>7</v>
+      </c>
+      <c r="E47">
+        <v>6</v>
+      </c>
+      <c r="F47">
+        <v>7</v>
+      </c>
+      <c r="H47">
+        <v>11</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>10</v>
+      </c>
+      <c r="K47">
+        <v>7</v>
+      </c>
+      <c r="L47">
+        <v>11</v>
+      </c>
+      <c r="M47">
+        <v>7</v>
+      </c>
+      <c r="O47">
+        <v>6</v>
+      </c>
+      <c r="Q47">
+        <v>8</v>
+      </c>
+      <c r="R47">
+        <v>7</v>
+      </c>
+      <c r="S47">
+        <v>9</v>
+      </c>
+      <c r="T47">
+        <v>3</v>
+      </c>
+      <c r="V47">
+        <v>10</v>
+      </c>
+      <c r="X47">
+        <v>7</v>
+      </c>
+      <c r="AC47">
+        <v>10</v>
+      </c>
+      <c r="AE47">
+        <v>9</v>
+      </c>
+      <c r="AG47">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48">
+        <v>30</v>
+      </c>
+      <c r="C48">
+        <v>14</v>
+      </c>
+      <c r="D48">
+        <v>27</v>
+      </c>
+      <c r="E48">
+        <v>15</v>
+      </c>
+      <c r="F48">
+        <v>7</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>17</v>
+      </c>
+      <c r="I48">
+        <v>20</v>
+      </c>
+      <c r="J48">
+        <v>15</v>
+      </c>
+      <c r="K48">
+        <v>10</v>
+      </c>
+      <c r="L48">
+        <v>26</v>
+      </c>
+      <c r="M48">
+        <v>11</v>
+      </c>
+      <c r="O48">
+        <v>14</v>
+      </c>
+      <c r="P48">
+        <v>26</v>
+      </c>
+      <c r="Q48">
+        <v>18</v>
+      </c>
+      <c r="R48">
+        <v>48</v>
+      </c>
+      <c r="S48">
+        <v>37</v>
+      </c>
+      <c r="T48">
+        <v>4</v>
+      </c>
+      <c r="U48">
+        <v>2</v>
+      </c>
+      <c r="V48">
+        <v>21</v>
+      </c>
+      <c r="W48">
+        <v>14</v>
+      </c>
+      <c r="X48">
+        <v>14</v>
+      </c>
+      <c r="AA48">
+        <v>7</v>
+      </c>
+      <c r="AC48">
+        <v>28</v>
+      </c>
+      <c r="AD48">
+        <v>13</v>
+      </c>
+      <c r="AE48">
+        <v>9</v>
+      </c>
+      <c r="AG48">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49">
+        <v>31</v>
+      </c>
+      <c r="C49">
+        <v>35</v>
+      </c>
+      <c r="D49">
+        <v>33</v>
+      </c>
+      <c r="E49">
+        <v>30</v>
+      </c>
+      <c r="F49">
+        <v>12</v>
+      </c>
+      <c r="H49">
+        <v>34</v>
+      </c>
+      <c r="I49">
+        <v>28</v>
+      </c>
+      <c r="J49">
+        <v>22</v>
+      </c>
+      <c r="K49">
+        <v>30</v>
+      </c>
+      <c r="L49">
+        <v>26</v>
+      </c>
+      <c r="M49">
+        <v>14</v>
+      </c>
+      <c r="N49">
+        <v>3</v>
+      </c>
+      <c r="O49">
+        <v>26</v>
+      </c>
+      <c r="P49">
+        <v>18</v>
+      </c>
+      <c r="Q49">
+        <v>18</v>
+      </c>
+      <c r="R49">
+        <v>28</v>
+      </c>
+      <c r="S49">
+        <v>42</v>
+      </c>
+      <c r="T49">
+        <v>6</v>
+      </c>
+      <c r="V49">
+        <v>40</v>
+      </c>
+      <c r="W49">
+        <v>35</v>
+      </c>
+      <c r="X49">
+        <v>32</v>
+      </c>
+      <c r="Y49">
+        <v>1</v>
+      </c>
+      <c r="Z49">
+        <v>24</v>
+      </c>
+      <c r="AA49">
+        <v>14</v>
+      </c>
+      <c r="AB49">
+        <v>1</v>
+      </c>
+      <c r="AC49">
+        <v>30</v>
+      </c>
+      <c r="AD49">
+        <v>19</v>
+      </c>
+      <c r="AE49">
+        <v>25</v>
+      </c>
+      <c r="AG49">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50">
+        <v>16</v>
+      </c>
+      <c r="C50">
+        <v>30</v>
+      </c>
+      <c r="D50">
+        <v>28</v>
+      </c>
+      <c r="E50">
+        <v>18</v>
+      </c>
+      <c r="F50">
+        <v>4</v>
+      </c>
+      <c r="H50">
+        <v>20</v>
+      </c>
+      <c r="I50">
+        <v>21</v>
+      </c>
+      <c r="J50">
+        <v>26</v>
+      </c>
+      <c r="K50">
+        <v>27</v>
+      </c>
+      <c r="L50">
+        <v>13</v>
+      </c>
+      <c r="M50">
+        <v>9</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <v>29</v>
+      </c>
+      <c r="P50">
+        <v>15</v>
+      </c>
+      <c r="Q50">
+        <v>19</v>
+      </c>
+      <c r="R50">
+        <v>23</v>
+      </c>
+      <c r="S50">
+        <v>26</v>
+      </c>
+      <c r="T50">
+        <v>6</v>
+      </c>
+      <c r="V50">
+        <v>40</v>
+      </c>
+      <c r="W50">
+        <v>11</v>
+      </c>
+      <c r="X50">
+        <v>20</v>
+      </c>
+      <c r="Z50">
+        <v>6</v>
+      </c>
+      <c r="AC50">
+        <v>40</v>
+      </c>
+      <c r="AD50">
+        <v>15</v>
+      </c>
+      <c r="AE50">
+        <v>19</v>
+      </c>
+      <c r="AG50">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51">
+        <v>24</v>
+      </c>
+      <c r="C51">
+        <v>18</v>
+      </c>
+      <c r="D51">
+        <v>12</v>
+      </c>
+      <c r="E51">
+        <v>23</v>
+      </c>
+      <c r="F51">
+        <v>5</v>
+      </c>
+      <c r="G51">
+        <v>3</v>
+      </c>
+      <c r="H51">
+        <v>17</v>
+      </c>
+      <c r="I51">
+        <v>43</v>
+      </c>
+      <c r="J51">
+        <v>19</v>
+      </c>
+      <c r="K51">
+        <v>39</v>
+      </c>
+      <c r="L51">
+        <v>14</v>
+      </c>
+      <c r="M51">
+        <v>14</v>
+      </c>
+      <c r="O51">
+        <v>17</v>
+      </c>
+      <c r="P51">
+        <v>26</v>
+      </c>
+      <c r="Q51">
+        <v>26</v>
+      </c>
+      <c r="R51">
+        <v>35</v>
+      </c>
+      <c r="S51">
+        <v>16</v>
+      </c>
+      <c r="T51">
+        <v>5</v>
+      </c>
+      <c r="V51">
+        <v>11</v>
+      </c>
+      <c r="W51">
+        <v>40</v>
+      </c>
+      <c r="X51">
+        <v>31</v>
+      </c>
+      <c r="Z51">
+        <v>1</v>
+      </c>
+      <c r="AA51">
+        <v>5</v>
+      </c>
+      <c r="AC51">
+        <v>13</v>
+      </c>
+      <c r="AD51">
+        <v>14</v>
+      </c>
+      <c r="AE51">
+        <v>31</v>
+      </c>
+      <c r="AG51">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52">
+        <v>31</v>
+      </c>
+      <c r="C52">
+        <v>46</v>
+      </c>
+      <c r="D52">
+        <v>42</v>
+      </c>
+      <c r="E52">
+        <v>33</v>
+      </c>
+      <c r="F52">
+        <v>23</v>
+      </c>
+      <c r="G52">
+        <v>10</v>
+      </c>
+      <c r="H52">
+        <v>30</v>
+      </c>
+      <c r="I52">
+        <v>42</v>
+      </c>
+      <c r="J52">
+        <v>39</v>
+      </c>
+      <c r="K52">
+        <v>45</v>
+      </c>
+      <c r="L52">
+        <v>52</v>
+      </c>
+      <c r="M52">
+        <v>30</v>
+      </c>
+      <c r="N52">
+        <v>7</v>
+      </c>
+      <c r="O52">
+        <v>42</v>
+      </c>
+      <c r="P52">
+        <v>39</v>
+      </c>
+      <c r="Q52">
+        <v>36</v>
+      </c>
+      <c r="R52">
+        <v>33</v>
+      </c>
+      <c r="S52">
+        <v>46</v>
+      </c>
+      <c r="T52">
+        <v>32</v>
+      </c>
+      <c r="U52">
+        <v>10</v>
+      </c>
+      <c r="V52">
+        <v>43</v>
+      </c>
+      <c r="W52">
+        <v>47</v>
+      </c>
+      <c r="X52">
+        <v>47</v>
+      </c>
+      <c r="Y52">
+        <v>1</v>
+      </c>
+      <c r="Z52">
+        <v>15</v>
+      </c>
+      <c r="AA52">
+        <v>22</v>
+      </c>
+      <c r="AB52">
+        <v>10</v>
+      </c>
+      <c r="AC52">
+        <v>46</v>
+      </c>
+      <c r="AD52">
+        <v>55</v>
+      </c>
+      <c r="AE52">
+        <v>40</v>
+      </c>
+      <c r="AG52">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>10</v>
+      </c>
+      <c r="D53">
+        <v>7</v>
+      </c>
+      <c r="E53">
+        <v>5</v>
+      </c>
+      <c r="F53">
+        <v>4</v>
+      </c>
+      <c r="H53">
+        <v>7</v>
+      </c>
+      <c r="I53">
+        <v>6</v>
+      </c>
+      <c r="J53">
+        <v>11</v>
+      </c>
+      <c r="K53">
+        <v>5</v>
+      </c>
+      <c r="L53">
+        <v>6</v>
+      </c>
+      <c r="M53">
+        <v>2</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <v>7</v>
+      </c>
+      <c r="P53">
+        <v>4</v>
+      </c>
+      <c r="Q53">
+        <v>10</v>
+      </c>
+      <c r="R53">
+        <v>7</v>
+      </c>
+      <c r="S53">
+        <v>12</v>
+      </c>
+      <c r="T53">
+        <v>1</v>
+      </c>
+      <c r="V53">
+        <v>5</v>
+      </c>
+      <c r="W53">
+        <v>7</v>
+      </c>
+      <c r="X53">
+        <v>6</v>
+      </c>
+      <c r="Z53">
+        <v>5</v>
+      </c>
+      <c r="AA53">
+        <v>6</v>
+      </c>
+      <c r="AC53">
+        <v>5</v>
+      </c>
+      <c r="AD53">
+        <v>5</v>
+      </c>
+      <c r="AE53">
+        <v>4</v>
+      </c>
+      <c r="AG53">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54">
+        <v>18</v>
+      </c>
+      <c r="C54">
+        <v>25</v>
+      </c>
+      <c r="D54">
+        <v>23</v>
+      </c>
+      <c r="E54">
+        <v>16</v>
+      </c>
+      <c r="F54">
+        <v>9</v>
+      </c>
+      <c r="H54">
+        <v>19</v>
+      </c>
+      <c r="I54">
+        <v>15</v>
+      </c>
+      <c r="J54">
+        <v>26</v>
+      </c>
+      <c r="K54">
+        <v>14</v>
+      </c>
+      <c r="L54">
+        <v>16</v>
+      </c>
+      <c r="M54">
+        <v>20</v>
+      </c>
+      <c r="O54">
+        <v>18</v>
+      </c>
+      <c r="P54">
+        <v>13</v>
+      </c>
+      <c r="Q54">
+        <v>19</v>
+      </c>
+      <c r="R54">
+        <v>21</v>
+      </c>
+      <c r="S54">
+        <v>21</v>
+      </c>
+      <c r="T54">
+        <v>7</v>
+      </c>
+      <c r="V54">
+        <v>19</v>
+      </c>
+      <c r="W54">
+        <v>21</v>
+      </c>
+      <c r="X54">
+        <v>21</v>
+      </c>
+      <c r="Y54">
+        <v>1</v>
+      </c>
+      <c r="Z54">
+        <v>1</v>
+      </c>
+      <c r="AC54">
+        <v>14</v>
+      </c>
+      <c r="AD54">
+        <v>22</v>
+      </c>
+      <c r="AE54">
+        <v>23</v>
+      </c>
+      <c r="AG54">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+      <c r="J55">
+        <v>4</v>
+      </c>
+      <c r="K55">
+        <v>4</v>
+      </c>
+      <c r="L55">
+        <v>6</v>
+      </c>
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="O55">
+        <v>2</v>
+      </c>
+      <c r="P55">
+        <v>2</v>
+      </c>
+      <c r="Q55">
+        <v>2</v>
+      </c>
+      <c r="S55">
+        <v>5</v>
+      </c>
+      <c r="T55">
+        <v>1</v>
+      </c>
+      <c r="V55">
+        <v>3</v>
+      </c>
+      <c r="W55">
+        <v>1</v>
+      </c>
+      <c r="X55">
+        <v>6</v>
+      </c>
+      <c r="AA55">
+        <v>1</v>
+      </c>
+      <c r="AC55">
+        <v>3</v>
+      </c>
+      <c r="AE55">
+        <v>3</v>
+      </c>
+      <c r="AG55">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <v>12</v>
+      </c>
+      <c r="H56">
+        <v>10</v>
+      </c>
+      <c r="I56">
+        <v>6</v>
+      </c>
+      <c r="J56">
+        <v>6</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+      <c r="P56">
+        <v>6</v>
+      </c>
+      <c r="Q56">
+        <v>9</v>
+      </c>
+      <c r="R56">
+        <v>1</v>
+      </c>
+      <c r="S56">
+        <v>1</v>
+      </c>
+      <c r="T56">
+        <v>1</v>
+      </c>
+      <c r="V56">
+        <v>4</v>
+      </c>
+      <c r="W56">
+        <v>2</v>
+      </c>
+      <c r="X56">
+        <v>6</v>
+      </c>
+      <c r="AC56">
+        <v>4</v>
+      </c>
+      <c r="AD56">
+        <v>1</v>
+      </c>
+      <c r="AE56">
+        <v>6</v>
+      </c>
+      <c r="AG56">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>10</v>
+      </c>
+      <c r="I57">
+        <v>5</v>
+      </c>
+      <c r="J57">
+        <v>8</v>
+      </c>
+      <c r="K57">
+        <v>5</v>
+      </c>
+      <c r="L57">
+        <v>6</v>
+      </c>
+      <c r="M57">
+        <v>3</v>
+      </c>
+      <c r="O57">
+        <v>3</v>
+      </c>
+      <c r="P57">
+        <v>1</v>
+      </c>
+      <c r="Q57">
+        <v>4</v>
+      </c>
+      <c r="R57">
+        <v>6</v>
+      </c>
+      <c r="S57">
+        <v>4</v>
+      </c>
+      <c r="T57">
+        <v>2</v>
+      </c>
+      <c r="V57">
+        <v>7</v>
+      </c>
+      <c r="W57">
+        <v>5</v>
+      </c>
+      <c r="X57">
+        <v>5</v>
+      </c>
+      <c r="Y57">
+        <v>1</v>
+      </c>
+      <c r="AC57">
+        <v>7</v>
+      </c>
+      <c r="AD57">
+        <v>6</v>
+      </c>
+      <c r="AE57">
+        <v>4</v>
+      </c>
+      <c r="AG57">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>